<commit_message>
updated till 12 Dec 9pm
</commit_message>
<xml_diff>
--- a/Daily Collection/December-2020-Collection.xlsx
+++ b/Daily Collection/December-2020-Collection.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="103">
   <si>
     <t>S.No.</t>
   </si>
@@ -334,10 +334,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -357,14 +357,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -379,36 +380,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -416,16 +387,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -440,10 +403,17 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -456,7 +426,38 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -469,24 +470,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -527,19 +527,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,7 +665,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -563,151 +707,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -718,15 +718,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -749,7 +740,57 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -769,52 +810,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -823,15 +823,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -841,130 +841,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1320,11 +1320,11 @@
   <dimension ref="A1:AI92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D2" s="6">
         <f>SUM(E2:AI2)</f>
-        <v>362900</v>
+        <v>388500</v>
       </c>
       <c r="E2" s="2">
         <f>SUM(E3:E92)</f>
@@ -1469,11 +1469,11 @@
       </c>
       <c r="I2" s="2">
         <f t="shared" si="0"/>
-        <v>18000</v>
+        <v>20000</v>
       </c>
       <c r="J2" s="2">
         <f t="shared" si="0"/>
-        <v>49500</v>
+        <v>47500</v>
       </c>
       <c r="K2" s="2">
         <f t="shared" si="0"/>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P2" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>25600</v>
       </c>
       <c r="Q2" s="2">
         <f t="shared" si="1"/>
@@ -1600,7 +1600,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:16">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1612,10 +1612,13 @@
       </c>
       <c r="D4" s="2">
         <f t="shared" si="2"/>
-        <v>5000</v>
+        <v>8000</v>
       </c>
       <c r="H4" s="3">
         <v>5000</v>
+      </c>
+      <c r="P4" s="3">
+        <v>3000</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1651,7 +1654,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:16">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1663,7 +1666,10 @@
       </c>
       <c r="D7" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1000</v>
+      </c>
+      <c r="P7" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -1730,7 +1736,6 @@
       <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="3"/>
       <c r="C11" s="7" t="s">
         <v>20</v>
       </c>
@@ -1743,7 +1748,6 @@
       <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="3"/>
       <c r="C12" s="7" t="s">
         <v>21</v>
       </c>
@@ -1798,7 +1802,6 @@
       <c r="A15" s="3">
         <v>13</v>
       </c>
-      <c r="B15" s="3"/>
       <c r="C15" s="7" t="s">
         <v>24</v>
       </c>
@@ -1832,7 +1835,6 @@
       <c r="A17" s="3">
         <v>15</v>
       </c>
-      <c r="B17" s="3"/>
       <c r="C17" s="7" t="s">
         <v>26</v>
       </c>
@@ -1863,7 +1865,6 @@
       <c r="A19" s="3">
         <v>17</v>
       </c>
-      <c r="B19" s="3"/>
       <c r="C19" s="7" t="s">
         <v>28</v>
       </c>
@@ -1876,7 +1877,6 @@
       <c r="A20" s="3">
         <v>18</v>
       </c>
-      <c r="B20" s="3"/>
       <c r="C20" s="7" t="s">
         <v>29</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:16">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1897,12 +1897,15 @@
       </c>
       <c r="D21" s="2">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="H21" s="3">
         <v>2000</v>
       </c>
       <c r="L21" s="3">
+        <v>1000</v>
+      </c>
+      <c r="P21" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -1910,7 +1913,6 @@
       <c r="A22" s="3">
         <v>20</v>
       </c>
-      <c r="B22" s="3"/>
       <c r="C22" s="7" t="s">
         <v>31</v>
       </c>
@@ -1943,20 +1945,16 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:4">
       <c r="A24" s="3">
         <v>22</v>
       </c>
-      <c r="B24" s="3"/>
       <c r="C24" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="2"/>
-        <v>2000</v>
-      </c>
-      <c r="J24" s="3">
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -1987,7 +1985,6 @@
       <c r="A26" s="3">
         <v>24</v>
       </c>
-      <c r="B26" s="3"/>
       <c r="C26" s="7" t="s">
         <v>35</v>
       </c>
@@ -2014,7 +2011,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:16">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -2026,7 +2023,7 @@
       </c>
       <c r="D28" s="2">
         <f t="shared" si="2"/>
-        <v>2900</v>
+        <v>3000</v>
       </c>
       <c r="G28" s="3">
         <v>1000</v>
@@ -2036,6 +2033,9 @@
       </c>
       <c r="M28" s="3">
         <v>900</v>
+      </c>
+      <c r="P28" s="3">
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -2090,7 +2090,6 @@
       <c r="A31" s="3">
         <v>29</v>
       </c>
-      <c r="B31" s="3"/>
       <c r="C31" s="7" t="s">
         <v>41</v>
       </c>
@@ -2103,7 +2102,6 @@
       <c r="A32" s="3">
         <v>30</v>
       </c>
-      <c r="B32" s="3"/>
       <c r="C32" s="7" t="s">
         <v>42</v>
       </c>
@@ -2197,7 +2195,6 @@
       <c r="A37" s="3">
         <v>35</v>
       </c>
-      <c r="B37" s="3"/>
       <c r="C37" s="7" t="s">
         <v>47</v>
       </c>
@@ -2221,7 +2218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:16">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -2233,10 +2230,13 @@
       </c>
       <c r="D39" s="2">
         <f t="shared" si="3"/>
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="M39" s="3">
         <v>6000</v>
+      </c>
+      <c r="P39" s="3">
+        <v>3000</v>
       </c>
     </row>
     <row r="40" spans="1:14">
@@ -2267,7 +2267,6 @@
       <c r="A41" s="3">
         <v>39</v>
       </c>
-      <c r="B41" s="3"/>
       <c r="C41" s="7" t="s">
         <v>51</v>
       </c>
@@ -2280,7 +2279,6 @@
       <c r="A42" s="3">
         <v>40</v>
       </c>
-      <c r="B42" s="3"/>
       <c r="C42" s="7" t="s">
         <v>52</v>
       </c>
@@ -2311,7 +2309,6 @@
       <c r="A44" s="3">
         <v>42</v>
       </c>
-      <c r="B44" s="3"/>
       <c r="C44" s="7" t="s">
         <v>54</v>
       </c>
@@ -2324,7 +2321,6 @@
       <c r="A45" s="3">
         <v>43</v>
       </c>
-      <c r="B45" s="3"/>
       <c r="C45" s="7" t="s">
         <v>55</v>
       </c>
@@ -2373,7 +2369,6 @@
       <c r="A48" s="3">
         <v>46</v>
       </c>
-      <c r="B48" s="3"/>
       <c r="C48" s="7" t="s">
         <v>58</v>
       </c>
@@ -2389,7 +2384,6 @@
       <c r="A49" s="3">
         <v>47</v>
       </c>
-      <c r="B49" s="3"/>
       <c r="C49" s="7" t="s">
         <v>59</v>
       </c>
@@ -2450,7 +2444,6 @@
       <c r="A52" s="3">
         <v>50</v>
       </c>
-      <c r="B52" s="3"/>
       <c r="C52" s="7" t="s">
         <v>62</v>
       </c>
@@ -2462,7 +2455,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:16">
       <c r="A53" s="3">
         <v>51</v>
       </c>
@@ -2474,7 +2467,7 @@
       </c>
       <c r="D53" s="2">
         <f t="shared" si="3"/>
-        <v>13000</v>
+        <v>18000</v>
       </c>
       <c r="G53" s="3">
         <v>2000</v>
@@ -2485,8 +2478,11 @@
       <c r="M53" s="3">
         <v>5000</v>
       </c>
-    </row>
-    <row r="54" spans="1:11">
+      <c r="P53" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
       <c r="A54" s="3">
         <v>52</v>
       </c>
@@ -2498,12 +2494,15 @@
       </c>
       <c r="D54" s="2">
         <f t="shared" si="3"/>
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="G54" s="3">
         <v>3000</v>
       </c>
       <c r="K54" s="3">
+        <v>3000</v>
+      </c>
+      <c r="P54" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -2511,7 +2510,6 @@
       <c r="A55" s="3">
         <v>53</v>
       </c>
-      <c r="B55" s="3"/>
       <c r="C55" s="7" t="s">
         <v>65</v>
       </c>
@@ -2524,7 +2522,6 @@
       <c r="A56" s="3">
         <v>54</v>
       </c>
-      <c r="B56" s="3"/>
       <c r="C56" s="7" t="s">
         <v>66</v>
       </c>
@@ -2537,7 +2534,6 @@
       <c r="A57" s="3">
         <v>55</v>
       </c>
-      <c r="B57" s="3"/>
       <c r="C57" s="7" t="s">
         <v>67</v>
       </c>
@@ -2550,7 +2546,6 @@
       <c r="A58" s="3">
         <v>56</v>
       </c>
-      <c r="B58" s="3"/>
       <c r="C58" s="7" t="s">
         <v>68</v>
       </c>
@@ -2587,7 +2582,6 @@
       <c r="A60" s="3">
         <v>58</v>
       </c>
-      <c r="B60" s="3"/>
       <c r="C60" s="7" t="s">
         <v>70</v>
       </c>
@@ -2596,7 +2590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:16">
       <c r="A61" s="3">
         <v>59</v>
       </c>
@@ -2608,7 +2602,7 @@
       </c>
       <c r="D61" s="2">
         <f t="shared" si="3"/>
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="H61" s="3">
         <v>1000</v>
@@ -2616,18 +2610,26 @@
       <c r="L61" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="P61" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" s="3">
         <v>60</v>
       </c>
-      <c r="B62" s="3"/>
+      <c r="B62" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="C62" s="7" t="s">
         <v>72</v>
       </c>
       <c r="D62" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="I62" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="63" spans="1:14">
@@ -2681,7 +2683,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:16">
       <c r="A65" s="3">
         <v>63</v>
       </c>
@@ -2693,7 +2695,7 @@
       </c>
       <c r="D65" s="2">
         <f t="shared" si="3"/>
-        <v>18000</v>
+        <v>19000</v>
       </c>
       <c r="G65" s="3">
         <v>2000</v>
@@ -2712,6 +2714,9 @@
       </c>
       <c r="O65" s="3">
         <v>2000</v>
+      </c>
+      <c r="P65" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="66" spans="1:13">
@@ -2738,7 +2743,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:16">
       <c r="A67" s="3">
         <v>65</v>
       </c>
@@ -2750,10 +2755,13 @@
       </c>
       <c r="D67" s="2">
         <f t="shared" ref="D67:D92" si="4">SUM(E67:AI67)</f>
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="K67" s="3">
         <v>1500</v>
+      </c>
+      <c r="P67" s="3">
+        <v>500</v>
       </c>
     </row>
     <row r="68" spans="1:14">
@@ -2778,7 +2786,6 @@
       <c r="A69" s="3">
         <v>67</v>
       </c>
-      <c r="B69" s="3"/>
       <c r="C69" s="7" t="s">
         <v>79</v>
       </c>
@@ -2811,7 +2818,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:16">
       <c r="A71" s="3">
         <v>69</v>
       </c>
@@ -2823,7 +2830,7 @@
       </c>
       <c r="D71" s="2">
         <f t="shared" si="4"/>
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="H71" s="3">
         <v>2000</v>
@@ -2833,13 +2840,15 @@
       </c>
       <c r="M71" s="3">
         <v>2000</v>
+      </c>
+      <c r="P71" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="3">
         <v>70</v>
       </c>
-      <c r="B72" s="3"/>
       <c r="C72" s="7" t="s">
         <v>82</v>
       </c>
@@ -2852,7 +2861,6 @@
       <c r="A73" s="3">
         <v>71</v>
       </c>
-      <c r="B73" s="3"/>
       <c r="C73" s="7" t="s">
         <v>83</v>
       </c>
@@ -2886,7 +2894,6 @@
       <c r="A75" s="3">
         <v>73</v>
       </c>
-      <c r="B75" s="3"/>
       <c r="C75" s="7" t="s">
         <v>85</v>
       </c>
@@ -2899,7 +2906,6 @@
       <c r="A76" s="3">
         <v>74</v>
       </c>
-      <c r="B76" s="3"/>
       <c r="C76" s="7" t="s">
         <v>86</v>
       </c>
@@ -3008,7 +3014,6 @@
       <c r="A81" s="3">
         <v>79</v>
       </c>
-      <c r="B81" s="3"/>
       <c r="C81" s="7" t="s">
         <v>91</v>
       </c>
@@ -3038,7 +3043,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="83" spans="1:12">
+    <row r="83" spans="1:16">
       <c r="A83" s="3">
         <v>81</v>
       </c>
@@ -3050,7 +3055,7 @@
       </c>
       <c r="D83" s="2">
         <f t="shared" si="4"/>
-        <v>7000</v>
+        <v>10000</v>
       </c>
       <c r="H83" s="3">
         <v>4000</v>
@@ -3058,8 +3063,11 @@
       <c r="L83" s="3">
         <v>3000</v>
       </c>
-    </row>
-    <row r="84" spans="1:14">
+      <c r="P83" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16">
       <c r="A84" s="3">
         <v>82</v>
       </c>
@@ -3071,13 +3079,16 @@
       </c>
       <c r="D84" s="2">
         <f t="shared" si="4"/>
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="L84" s="3">
         <v>2000</v>
       </c>
       <c r="N84" s="3">
         <v>1000</v>
+      </c>
+      <c r="P84" s="3">
+        <v>3000</v>
       </c>
     </row>
     <row r="85" spans="1:14">

</xml_diff>

<commit_message>
data updated till 15Dec 9AM
</commit_message>
<xml_diff>
--- a/Daily Collection/December-2020-Collection.xlsx
+++ b/Daily Collection/December-2020-Collection.xlsx
@@ -68,6 +68,29 @@
         </r>
       </text>
     </comment>
+    <comment ref="S54" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>Vijay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+2500-Digital
+500-Cash</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="N59" authorId="0">
       <text>
         <r>
@@ -88,6 +111,52 @@
           <t xml:space="preserve">
 3000-Cash
 3000-Digital</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S68" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>Vijay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+2000-Cash
+1000-Digital</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S79" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>Vijay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+1000-Cash
+1000-Digital</t>
         </r>
       </text>
     </comment>
@@ -468,27 +537,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -503,18 +551,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -529,6 +586,35 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -550,27 +636,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -591,21 +674,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -655,13 +724,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -673,13 +880,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -691,151 +904,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -846,15 +915,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -872,6 +932,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -907,21 +982,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -932,6 +992,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -951,7 +1020,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -969,130 +1038,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1454,11 +1523,11 @@
   <dimension ref="A1:AJ92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="M61" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="S64" sqref="S64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1586,7 +1655,7 @@
       </c>
       <c r="E2" s="6">
         <f>SUM(F2:AJ2)</f>
-        <v>394000</v>
+        <v>469000</v>
       </c>
       <c r="F2" s="2">
         <f>SUM(F3:F92)</f>
@@ -1642,7 +1711,7 @@
       </c>
       <c r="S2" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>75000</v>
       </c>
       <c r="T2" s="2">
         <f t="shared" si="1"/>
@@ -1713,20 +1782,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:19">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3"/>
       <c r="D3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" ref="E3:E34" si="2">SUM(F3:AJ3)</f>
-        <v>14000</v>
+        <v>19000</v>
       </c>
       <c r="I3" s="3">
         <v>3000</v>
@@ -1735,6 +1803,9 @@
         <v>6000</v>
       </c>
       <c r="N3" s="8">
+        <v>5000</v>
+      </c>
+      <c r="S3" s="8">
         <v>5000</v>
       </c>
     </row>
@@ -1745,7 +1816,6 @@
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3"/>
       <c r="D4" s="7" t="s">
         <v>9</v>
       </c>
@@ -1760,20 +1830,22 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:19">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3"/>
       <c r="D5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1000</v>
+      </c>
+      <c r="S5" s="8">
+        <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1783,7 +1855,6 @@
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3"/>
       <c r="D6" s="7" t="s">
         <v>12</v>
       </c>
@@ -1802,7 +1873,6 @@
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3"/>
       <c r="D7" s="7" t="s">
         <v>14</v>
       </c>
@@ -1821,7 +1891,6 @@
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3"/>
       <c r="D8" s="7" t="s">
         <v>16</v>
       </c>
@@ -1846,7 +1915,6 @@
       <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="3"/>
       <c r="D9" s="7" t="s">
         <v>18</v>
       </c>
@@ -1855,25 +1923,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:19">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="3"/>
       <c r="D10" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="I10" s="8">
         <v>1000</v>
       </c>
       <c r="L10" s="8">
+        <v>2000</v>
+      </c>
+      <c r="S10" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -1901,20 +1971,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:19">
       <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="3"/>
       <c r="D13" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="2"/>
-        <v>7000</v>
+        <v>10000</v>
       </c>
       <c r="I13" s="3">
         <v>2000</v>
@@ -1925,23 +1994,28 @@
       <c r="O13" s="3">
         <v>3000</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="S13" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="3"/>
       <c r="D14" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="2"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="I14" s="8">
+        <v>2000</v>
+      </c>
+      <c r="S14" s="8">
         <v>2000</v>
       </c>
     </row>
@@ -1957,25 +2031,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:19">
       <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="3"/>
       <c r="D16" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="I16" s="3">
         <v>1000</v>
       </c>
       <c r="M16" s="3">
+        <v>2000</v>
+      </c>
+      <c r="S16" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -1998,7 +2074,6 @@
       <c r="B18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="3"/>
       <c r="D18" s="7" t="s">
         <v>28</v>
       </c>
@@ -2034,20 +2109,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:19">
       <c r="A21" s="3">
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="3"/>
       <c r="D21" s="7" t="s">
         <v>31</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="2"/>
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="I21" s="3">
         <v>2000</v>
@@ -2056,6 +2130,9 @@
         <v>1000</v>
       </c>
       <c r="Q21" s="3">
+        <v>1000</v>
+      </c>
+      <c r="S21" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -2078,7 +2155,6 @@
       <c r="B23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="3"/>
       <c r="D23" s="7" t="s">
         <v>33</v>
       </c>
@@ -2108,20 +2184,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:19">
       <c r="A25" s="3">
         <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="3"/>
       <c r="D25" s="7" t="s">
         <v>35</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" si="2"/>
-        <v>9000</v>
+        <v>12000</v>
       </c>
       <c r="J25" s="8">
         <v>3000</v>
@@ -2130,6 +2205,9 @@
         <v>3000</v>
       </c>
       <c r="O25" s="3">
+        <v>3000</v>
+      </c>
+      <c r="S25" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -2152,7 +2230,6 @@
       <c r="B27" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="3"/>
       <c r="D27" s="7" t="s">
         <v>37</v>
       </c>
@@ -2171,7 +2248,6 @@
       <c r="B28" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="3"/>
       <c r="D28" s="7" t="s">
         <v>38</v>
       </c>
@@ -2199,7 +2275,6 @@
       <c r="B29" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="3"/>
       <c r="D29" s="7" t="s">
         <v>40</v>
       </c>
@@ -2217,20 +2292,19 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:19">
       <c r="A30" s="3">
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="3"/>
       <c r="D30" s="7" t="s">
         <v>41</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" si="2"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="H30" s="3">
         <v>1000</v>
@@ -2239,6 +2313,9 @@
         <v>1000</v>
       </c>
       <c r="N30" s="3">
+        <v>2000</v>
+      </c>
+      <c r="S30" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -2266,25 +2343,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:19">
       <c r="A33" s="3">
         <v>31</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="3"/>
       <c r="D33" s="7" t="s">
         <v>44</v>
       </c>
       <c r="E33" s="2">
         <f t="shared" si="2"/>
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="I33" s="3">
         <v>3000</v>
       </c>
       <c r="O33" s="3">
+        <v>3000</v>
+      </c>
+      <c r="S33" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -2295,7 +2374,6 @@
       <c r="B34" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="3"/>
       <c r="D34" s="7" t="s">
         <v>45</v>
       </c>
@@ -2313,20 +2391,22 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:19">
       <c r="A35" s="3">
         <v>33</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="3"/>
       <c r="D35" s="7" t="s">
         <v>46</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" ref="E35:E66" si="3">SUM(F35:AJ35)</f>
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="S35" s="8">
+        <v>2000</v>
       </c>
     </row>
     <row r="36" spans="1:15">
@@ -2336,7 +2416,6 @@
       <c r="B36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="3"/>
       <c r="D36" s="7" t="s">
         <v>47</v>
       </c>
@@ -2370,7 +2449,6 @@
       <c r="B38" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="3"/>
       <c r="D38" s="7" t="s">
         <v>49</v>
       </c>
@@ -2386,7 +2464,6 @@
       <c r="B39" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="3"/>
       <c r="D39" s="7" t="s">
         <v>50</v>
       </c>
@@ -2408,7 +2485,6 @@
       <c r="B40" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="3"/>
       <c r="D40" s="7" t="s">
         <v>51</v>
       </c>
@@ -2450,23 +2526,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:19">
       <c r="A43" s="3">
         <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="3"/>
       <c r="D43" s="7" t="s">
         <v>54</v>
       </c>
       <c r="E43" s="2">
         <f t="shared" si="3"/>
-        <v>3000</v>
+        <v>4500</v>
       </c>
       <c r="M43" s="3">
         <v>3000</v>
+      </c>
+      <c r="S43" s="3">
+        <v>1500</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2500,7 +2578,6 @@
       <c r="B46" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="3"/>
       <c r="D46" s="7" t="s">
         <v>57</v>
       </c>
@@ -2519,7 +2596,6 @@
       <c r="B47" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C47" s="3"/>
       <c r="D47" s="7" t="s">
         <v>58</v>
       </c>
@@ -2538,7 +2614,6 @@
       <c r="B48" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C48" s="3"/>
       <c r="D48" s="7" t="s">
         <v>60</v>
       </c>
@@ -2569,7 +2644,6 @@
       <c r="B50" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C50" s="3"/>
       <c r="D50" s="7" t="s">
         <v>62</v>
       </c>
@@ -2588,7 +2662,6 @@
       <c r="B51" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C51" s="3"/>
       <c r="D51" s="7" t="s">
         <v>63</v>
       </c>
@@ -2634,7 +2707,6 @@
       <c r="B53" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C53" s="3"/>
       <c r="D53" s="7" t="s">
         <v>65</v>
       </c>
@@ -2655,20 +2727,19 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="54" spans="1:17">
+    <row r="54" spans="1:19">
       <c r="A54" s="3">
         <v>52</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C54" s="3"/>
       <c r="D54" s="7" t="s">
         <v>66</v>
       </c>
       <c r="E54" s="2">
         <f t="shared" si="3"/>
-        <v>9000</v>
+        <v>12000</v>
       </c>
       <c r="H54" s="8">
         <v>3000</v>
@@ -2677,6 +2748,9 @@
         <v>3000</v>
       </c>
       <c r="Q54" s="8">
+        <v>3000</v>
+      </c>
+      <c r="S54" s="8">
         <v>3000</v>
       </c>
     </row>
@@ -2704,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:17">
+    <row r="57" spans="1:19">
       <c r="A57" s="3">
         <v>55</v>
       </c>
@@ -2713,13 +2787,16 @@
       </c>
       <c r="E57" s="2">
         <f t="shared" si="3"/>
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="J57" s="3">
         <v>1000</v>
       </c>
       <c r="Q57" s="8">
         <v>2000</v>
+      </c>
+      <c r="S57" s="8">
+        <v>1000</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2734,20 +2811,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:17">
+    <row r="59" spans="1:19">
       <c r="A59" s="3">
         <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C59" s="3"/>
       <c r="D59" s="7" t="s">
         <v>71</v>
       </c>
       <c r="E59" s="2">
         <f t="shared" si="3"/>
-        <v>14500</v>
+        <v>19000</v>
       </c>
       <c r="H59" s="3">
         <v>2000</v>
@@ -2760,6 +2836,9 @@
       </c>
       <c r="Q59" s="8">
         <v>1500</v>
+      </c>
+      <c r="S59" s="8">
+        <v>4500</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2774,20 +2853,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:17">
+    <row r="61" spans="1:19">
       <c r="A61" s="3">
         <v>59</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C61" s="3"/>
       <c r="D61" s="7" t="s">
         <v>73</v>
       </c>
       <c r="E61" s="2">
         <f t="shared" si="3"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="I61" s="3">
         <v>1000</v>
@@ -2797,6 +2875,9 @@
       </c>
       <c r="Q61" s="3">
         <v>1000</v>
+      </c>
+      <c r="S61" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2806,7 +2887,6 @@
       <c r="B62" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C62" s="3"/>
       <c r="D62" s="7" t="s">
         <v>74</v>
       </c>
@@ -2818,26 +2898,28 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:19">
       <c r="A63" s="3">
         <v>61</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C63" s="3"/>
       <c r="D63" s="7" t="s">
         <v>75</v>
       </c>
       <c r="E63" s="2">
         <f t="shared" si="3"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="L63" s="3">
         <v>1000</v>
       </c>
       <c r="O63" s="3">
         <v>3000</v>
+      </c>
+      <c r="S63" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="64" spans="1:15">
@@ -2847,7 +2929,6 @@
       <c r="B64" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C64" s="3"/>
       <c r="D64" s="7" t="s">
         <v>76</v>
       </c>
@@ -2871,20 +2952,19 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="65" spans="1:17">
+    <row r="65" spans="1:19">
       <c r="A65" s="3">
         <v>63</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C65" s="3"/>
       <c r="D65" s="7" t="s">
         <v>77</v>
       </c>
       <c r="E65" s="2">
         <f t="shared" si="3"/>
-        <v>19000</v>
+        <v>24000</v>
       </c>
       <c r="H65" s="3">
         <v>2000</v>
@@ -2907,21 +2987,23 @@
       <c r="Q65" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="66" spans="1:14">
+      <c r="S65" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19">
       <c r="A66" s="3">
         <v>64</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C66" s="3"/>
       <c r="D66" s="7" t="s">
         <v>78</v>
       </c>
       <c r="E66" s="2">
         <f t="shared" si="3"/>
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="H66" s="3">
         <v>2000</v>
@@ -2930,6 +3012,9 @@
         <v>1000</v>
       </c>
       <c r="N66" s="3">
+        <v>2000</v>
+      </c>
+      <c r="S66" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -2940,7 +3025,6 @@
       <c r="B67" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C67" s="3"/>
       <c r="D67" s="7" t="s">
         <v>79</v>
       </c>
@@ -2955,23 +3039,25 @@
         <v>500</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:19">
       <c r="A68" s="3">
         <v>66</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C68" s="3"/>
       <c r="D68" s="7" t="s">
         <v>80</v>
       </c>
       <c r="E68" s="2">
         <f t="shared" si="4"/>
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="O68" s="3">
         <v>2000</v>
+      </c>
+      <c r="S68" s="8">
+        <v>3000</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2986,20 +3072,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:14">
+    <row r="70" spans="1:19">
       <c r="A70" s="3">
         <v>68</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C70" s="3"/>
       <c r="D70" s="7" t="s">
         <v>82</v>
       </c>
       <c r="E70" s="2">
         <f t="shared" si="4"/>
-        <v>12000</v>
+        <v>15000</v>
       </c>
       <c r="H70" s="3">
         <v>2000</v>
@@ -3010,21 +3095,23 @@
       <c r="N70" s="3">
         <v>6000</v>
       </c>
-    </row>
-    <row r="71" spans="1:17">
+      <c r="S70" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19">
       <c r="A71" s="3">
         <v>69</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C71" s="3"/>
       <c r="D71" s="7" t="s">
         <v>83</v>
       </c>
       <c r="E71" s="2">
         <f t="shared" si="4"/>
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="I71" s="3">
         <v>2000</v>
@@ -3037,6 +3124,9 @@
       </c>
       <c r="Q71" s="3">
         <v>1000</v>
+      </c>
+      <c r="S71" s="8">
+        <v>3000</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -3070,7 +3160,6 @@
       <c r="B74" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C74" s="3"/>
       <c r="D74" s="7" t="s">
         <v>86</v>
       </c>
@@ -3116,7 +3205,6 @@
       <c r="B77" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C77" s="3"/>
       <c r="D77" s="7" t="s">
         <v>89</v>
       </c>
@@ -3141,7 +3229,6 @@
       <c r="B78" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C78" s="3"/>
       <c r="D78" s="7" t="s">
         <v>90</v>
       </c>
@@ -3162,20 +3249,19 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="79" spans="1:15">
+    <row r="79" spans="1:19">
       <c r="A79" s="3">
         <v>77</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C79" s="3"/>
       <c r="D79" s="7" t="s">
         <v>91</v>
       </c>
       <c r="E79" s="2">
         <f t="shared" si="4"/>
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="I79" s="3">
         <v>1000</v>
@@ -3183,21 +3269,23 @@
       <c r="O79" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="80" spans="1:15">
+      <c r="S79" s="8">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19">
       <c r="A80" s="3">
         <v>78</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C80" s="3"/>
       <c r="D80" s="7" t="s">
         <v>92</v>
       </c>
       <c r="E80" s="2">
         <f t="shared" si="4"/>
-        <v>22000</v>
+        <v>27000</v>
       </c>
       <c r="J80" s="3">
         <v>2000</v>
@@ -3208,8 +3296,11 @@
       <c r="O80" s="3">
         <v>5000</v>
       </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="S80" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19">
       <c r="A81" s="3">
         <v>79</v>
       </c>
@@ -3224,7 +3315,10 @@
       </c>
       <c r="E81" s="2">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="S81" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="82" spans="1:13">
@@ -3320,7 +3414,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="86" spans="1:15">
+    <row r="86" spans="1:19">
       <c r="A86" s="3">
         <v>84</v>
       </c>
@@ -3332,7 +3426,7 @@
       </c>
       <c r="E86" s="2">
         <f t="shared" si="4"/>
-        <v>9000</v>
+        <v>12000</v>
       </c>
       <c r="K86" s="8">
         <v>4000</v>
@@ -3341,6 +3435,9 @@
         <v>2000</v>
       </c>
       <c r="O86" s="3">
+        <v>3000</v>
+      </c>
+      <c r="S86" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -3380,7 +3477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:15">
+    <row r="89" spans="1:19">
       <c r="A89" s="3">
         <v>87</v>
       </c>
@@ -3392,7 +3489,7 @@
       </c>
       <c r="E89" s="2">
         <f t="shared" si="4"/>
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="H89" s="3">
         <v>2000</v>
@@ -3406,8 +3503,11 @@
       <c r="O89" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="90" spans="1:14">
+      <c r="S89" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19">
       <c r="A90" s="3">
         <v>88</v>
       </c>
@@ -3419,7 +3519,7 @@
       </c>
       <c r="E90" s="2">
         <f t="shared" si="4"/>
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="I90" s="3">
         <v>1000</v>
@@ -3433,8 +3533,11 @@
       <c r="N90" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="91" spans="1:13">
+      <c r="S90" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19">
       <c r="A91" s="3">
         <v>89</v>
       </c>
@@ -3446,13 +3549,16 @@
       </c>
       <c r="E91" s="2">
         <f t="shared" si="4"/>
-        <v>8000</v>
+        <v>9000</v>
       </c>
       <c r="H91" s="8">
         <v>5000</v>
       </c>
       <c r="M91" s="8">
         <v>3000</v>
+      </c>
+      <c r="S91" s="8">
+        <v>1000</v>
       </c>
     </row>
     <row r="92" spans="1:5">

</xml_diff>

<commit_message>
data updated till 15 Dec 11PM
</commit_message>
<xml_diff>
--- a/Daily Collection/December-2020-Collection.xlsx
+++ b/Daily Collection/December-2020-Collection.xlsx
@@ -515,9 +515,9 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="[$-409]d\-mmm;@"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -551,22 +551,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -575,27 +559,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -613,53 +581,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -675,6 +599,82 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -736,7 +736,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -748,13 +820,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -772,49 +868,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -826,7 +886,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -838,73 +904,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -923,15 +923,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -966,6 +957,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -977,6 +979,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1004,23 +1015,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1038,130 +1038,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1523,11 +1523,11 @@
   <dimension ref="A1:AJ92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="M61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="M42" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S64" sqref="S64"/>
+      <selection pane="bottomRight" activeCell="T51" sqref="T51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="E2" s="6">
         <f>SUM(F2:AJ2)</f>
-        <v>469000</v>
+        <v>515500</v>
       </c>
       <c r="F2" s="2">
         <f>SUM(F3:F92)</f>
@@ -1715,7 +1715,7 @@
       </c>
       <c r="T2" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>46500</v>
       </c>
       <c r="U2" s="2">
         <f t="shared" si="1"/>
@@ -1809,7 +1809,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:20">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1821,12 +1821,15 @@
       </c>
       <c r="E4" s="2">
         <f t="shared" si="2"/>
-        <v>8000</v>
+        <v>11000</v>
       </c>
       <c r="I4" s="3">
         <v>5000</v>
       </c>
       <c r="Q4" s="3">
+        <v>3000</v>
+      </c>
+      <c r="T4" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -1866,7 +1869,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:20">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1878,10 +1881,13 @@
       </c>
       <c r="E7" s="2">
         <f t="shared" si="2"/>
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="Q7" s="3">
         <v>1000</v>
+      </c>
+      <c r="T7" s="3">
+        <v>4000</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -2031,7 +2037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:20">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -2043,7 +2049,7 @@
       </c>
       <c r="E16" s="2">
         <f t="shared" si="2"/>
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="I16" s="3">
         <v>1000</v>
@@ -2053,6 +2059,9 @@
       </c>
       <c r="S16" s="3">
         <v>2000</v>
+      </c>
+      <c r="T16" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2067,7 +2076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:20">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -2079,10 +2088,13 @@
       </c>
       <c r="E18" s="2">
         <f t="shared" si="2"/>
-        <v>5000</v>
+        <v>12000</v>
       </c>
       <c r="P18" s="8">
         <v>5000</v>
+      </c>
+      <c r="T18" s="8">
+        <v>7000</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2184,7 +2196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:20">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -2196,7 +2208,7 @@
       </c>
       <c r="E25" s="2">
         <f t="shared" si="2"/>
-        <v>12000</v>
+        <v>15000</v>
       </c>
       <c r="J25" s="8">
         <v>3000</v>
@@ -2208,6 +2220,9 @@
         <v>3000</v>
       </c>
       <c r="S25" s="3">
+        <v>3000</v>
+      </c>
+      <c r="T25" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -2391,7 +2406,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="35" spans="1:19">
+    <row r="35" spans="1:20">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -2403,10 +2418,13 @@
       </c>
       <c r="E35" s="2">
         <f t="shared" ref="E35:E66" si="3">SUM(F35:AJ35)</f>
-        <v>2000</v>
+        <v>7000</v>
       </c>
       <c r="S35" s="8">
         <v>2000</v>
+      </c>
+      <c r="T35" s="8">
+        <v>5000</v>
       </c>
     </row>
     <row r="36" spans="1:15">
@@ -2457,7 +2475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:20">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -2469,12 +2487,15 @@
       </c>
       <c r="E39" s="2">
         <f t="shared" si="3"/>
-        <v>9000</v>
+        <v>12000</v>
       </c>
       <c r="N39" s="3">
         <v>6000</v>
       </c>
       <c r="Q39" s="3">
+        <v>3000</v>
+      </c>
+      <c r="T39" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -2526,7 +2547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:19">
+    <row r="43" spans="1:20">
       <c r="A43" s="3">
         <v>41</v>
       </c>
@@ -2538,13 +2559,16 @@
       </c>
       <c r="E43" s="2">
         <f t="shared" si="3"/>
-        <v>4500</v>
+        <v>6500</v>
       </c>
       <c r="M43" s="3">
         <v>3000</v>
       </c>
       <c r="S43" s="3">
         <v>1500</v>
+      </c>
+      <c r="T43" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2637,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:20">
       <c r="A50" s="3">
         <v>48</v>
       </c>
@@ -2649,10 +2673,13 @@
       </c>
       <c r="E50" s="2">
         <f t="shared" si="3"/>
-        <v>8000</v>
+        <v>13000</v>
       </c>
       <c r="N50" s="3">
         <v>8000</v>
+      </c>
+      <c r="T50" s="3">
+        <v>5000</v>
       </c>
     </row>
     <row r="51" spans="1:15">
@@ -2880,7 +2907,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:20">
       <c r="A62" s="3">
         <v>60</v>
       </c>
@@ -2892,9 +2919,12 @@
       </c>
       <c r="E62" s="2">
         <f t="shared" si="3"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="J62" s="3">
+        <v>2000</v>
+      </c>
+      <c r="T62" s="8">
         <v>2000</v>
       </c>
     </row>
@@ -3018,7 +3048,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="67" spans="1:17">
+    <row r="67" spans="1:20">
       <c r="A67" s="3">
         <v>65</v>
       </c>
@@ -3030,13 +3060,16 @@
       </c>
       <c r="E67" s="2">
         <f t="shared" ref="E67:E92" si="4">SUM(F67:AJ67)</f>
-        <v>2000</v>
+        <v>3500</v>
       </c>
       <c r="L67" s="3">
         <v>1500</v>
       </c>
       <c r="Q67" s="3">
         <v>500</v>
+      </c>
+      <c r="T67" s="3">
+        <v>1500</v>
       </c>
     </row>
     <row r="68" spans="1:19">
@@ -3198,7 +3231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:20">
       <c r="A77" s="3">
         <v>75</v>
       </c>
@@ -3210,7 +3243,7 @@
       </c>
       <c r="E77" s="2">
         <f t="shared" si="4"/>
-        <v>9000</v>
+        <v>12000</v>
       </c>
       <c r="I77" s="8">
         <v>2000</v>
@@ -3219,6 +3252,9 @@
         <v>4000</v>
       </c>
       <c r="O77" s="3">
+        <v>3000</v>
+      </c>
+      <c r="T77" s="8">
         <v>3000</v>
       </c>
     </row>
@@ -3366,7 +3402,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="84" spans="1:17">
+    <row r="84" spans="1:20">
       <c r="A84" s="3">
         <v>82</v>
       </c>
@@ -3378,7 +3414,7 @@
       </c>
       <c r="E84" s="2">
         <f t="shared" si="4"/>
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="M84" s="3">
         <v>2000</v>
@@ -3387,6 +3423,9 @@
         <v>1000</v>
       </c>
       <c r="Q84" s="3">
+        <v>3000</v>
+      </c>
+      <c r="T84" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -3507,7 +3546,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="90" spans="1:19">
+    <row r="90" spans="1:20">
       <c r="A90" s="3">
         <v>88</v>
       </c>
@@ -3519,7 +3558,7 @@
       </c>
       <c r="E90" s="2">
         <f t="shared" si="4"/>
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="I90" s="3">
         <v>1000</v>
@@ -3536,8 +3575,11 @@
       <c r="S90" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="91" spans="1:19">
+      <c r="T90" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20">
       <c r="A91" s="3">
         <v>89</v>
       </c>
@@ -3549,7 +3591,7 @@
       </c>
       <c r="E91" s="2">
         <f t="shared" si="4"/>
-        <v>9000</v>
+        <v>12000</v>
       </c>
       <c r="H91" s="8">
         <v>5000</v>
@@ -3559,6 +3601,9 @@
       </c>
       <c r="S91" s="8">
         <v>1000</v>
+      </c>
+      <c r="T91" s="3">
+        <v>3000</v>
       </c>
     </row>
     <row r="92" spans="1:5">

</xml_diff>

<commit_message>
data updated till 16 Dec 2 PM
</commit_message>
<xml_diff>
--- a/Daily Collection/December-2020-Collection.xlsx
+++ b/Daily Collection/December-2020-Collection.xlsx
@@ -515,8 +515,8 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="[$-409]d\-mmm;@"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
@@ -537,7 +537,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -551,68 +559,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -628,14 +576,89 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -650,31 +673,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -724,7 +724,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -736,175 +904,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -915,80 +915,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1010,8 +936,82 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1020,7 +1020,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1038,130 +1038,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1523,11 +1523,11 @@
   <dimension ref="A1:AJ92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="M42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="M59" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T51" sqref="T51"/>
+      <selection pane="bottomRight" activeCell="U71" sqref="U71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="E2" s="6">
         <f>SUM(F2:AJ2)</f>
-        <v>515500</v>
+        <v>518500</v>
       </c>
       <c r="F2" s="2">
         <f>SUM(F3:F92)</f>
@@ -1715,7 +1715,7 @@
       </c>
       <c r="T2" s="2">
         <f t="shared" si="1"/>
-        <v>46500</v>
+        <v>49500</v>
       </c>
       <c r="U2" s="2">
         <f t="shared" si="1"/>
@@ -3072,7 +3072,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="68" spans="1:19">
+    <row r="68" spans="1:20">
       <c r="A68" s="3">
         <v>66</v>
       </c>
@@ -3084,12 +3084,15 @@
       </c>
       <c r="E68" s="2">
         <f t="shared" si="4"/>
-        <v>5000</v>
+        <v>8000</v>
       </c>
       <c r="O68" s="3">
         <v>2000</v>
       </c>
       <c r="S68" s="8">
+        <v>3000</v>
+      </c>
+      <c r="T68" s="8">
         <v>3000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data updated till 18Dec 9AM
</commit_message>
<xml_diff>
--- a/Daily Collection/December-2020-Collection.xlsx
+++ b/Daily Collection/December-2020-Collection.xlsx
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="110">
   <si>
     <t>S.No.</t>
   </si>
@@ -391,12 +391,21 @@
     <t>MS OM COMPUTER(661542289)</t>
   </si>
   <si>
+    <t>NIRANJANPUR</t>
+  </si>
+  <si>
     <t>RAJESH TELECOM(661613671)</t>
   </si>
   <si>
     <t>SURAJ KIRANA STORE(661735618)</t>
   </si>
   <si>
+    <t>ITWA</t>
+  </si>
+  <si>
+    <t>D.K.</t>
+  </si>
+  <si>
     <t>chintu electronics(662114680)</t>
   </si>
   <si>
@@ -455,6 +464,9 @@
   </si>
   <si>
     <t>RAJU PHONE GHAR(661613675)</t>
+  </si>
+  <si>
+    <t>Vikash Kr.</t>
   </si>
   <si>
     <t>PATEL TELECOM(661644686)</t>
@@ -515,9 +527,9 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="[$-409]d\-mmm;@"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -537,7 +549,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -545,7 +571,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -560,7 +586,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -568,31 +594,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -605,15 +615,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -642,8 +646,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -652,29 +687,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -724,7 +736,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -736,19 +862,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -760,79 +874,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -844,67 +916,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -915,6 +927,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -937,7 +973,31 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -957,45 +1017,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1006,21 +1027,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1038,130 +1050,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1523,17 +1535,18 @@
   <dimension ref="A1:AJ92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="M59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="N39" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="U71" sqref="U71"/>
+      <selection pane="bottomRight" activeCell="V57" sqref="V57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.71428571428571" style="3" customWidth="1"/>
-    <col min="2" max="3" width="11.5714285714286" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.5714285714286" style="3" customWidth="1"/>
     <col min="4" max="4" width="51.1428571428571" style="3" customWidth="1"/>
     <col min="5" max="5" width="11" style="3" customWidth="1"/>
     <col min="6" max="16384" width="9.14285714285714" style="3"/>
@@ -1655,7 +1668,7 @@
       </c>
       <c r="E2" s="6">
         <f>SUM(F2:AJ2)</f>
-        <v>518500</v>
+        <v>618500</v>
       </c>
       <c r="F2" s="2">
         <f>SUM(F3:F92)</f>
@@ -1719,11 +1732,11 @@
       </c>
       <c r="U2" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>47000</v>
       </c>
       <c r="V2" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>53000</v>
       </c>
       <c r="W2" s="2">
         <f t="shared" si="1"/>
@@ -1851,7 +1864,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:22">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1863,10 +1876,13 @@
       </c>
       <c r="E6" s="2">
         <f t="shared" si="2"/>
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="P6" s="3">
         <v>5000</v>
+      </c>
+      <c r="V6" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -1914,7 +1930,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:21">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1926,10 +1942,13 @@
       </c>
       <c r="E9" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19">
+        <v>3000</v>
+      </c>
+      <c r="U9" s="8">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1941,7 +1960,7 @@
       </c>
       <c r="E10" s="2">
         <f t="shared" si="2"/>
-        <v>5000</v>
+        <v>8500</v>
       </c>
       <c r="I10" s="8">
         <v>1000</v>
@@ -1951,6 +1970,12 @@
       </c>
       <c r="S10" s="3">
         <v>2000</v>
+      </c>
+      <c r="U10" s="3">
+        <v>2500</v>
+      </c>
+      <c r="V10" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1977,7 +2002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:22">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1989,7 +2014,7 @@
       </c>
       <c r="E13" s="2">
         <f t="shared" si="2"/>
-        <v>10000</v>
+        <v>13000</v>
       </c>
       <c r="I13" s="3">
         <v>2000</v>
@@ -2001,6 +2026,9 @@
         <v>3000</v>
       </c>
       <c r="S13" s="3">
+        <v>3000</v>
+      </c>
+      <c r="V13" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -2160,7 +2188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:22">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -2172,7 +2200,7 @@
       </c>
       <c r="E23" s="2">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="H23" s="3">
         <v>1000</v>
@@ -2181,6 +2209,12 @@
         <v>1000</v>
       </c>
       <c r="O23" s="3">
+        <v>1000</v>
+      </c>
+      <c r="U23" s="3">
+        <v>1000</v>
+      </c>
+      <c r="V23" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -2283,7 +2317,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:22">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -2295,7 +2329,7 @@
       </c>
       <c r="E29" s="2">
         <f t="shared" si="2"/>
-        <v>9000</v>
+        <v>11000</v>
       </c>
       <c r="H29" s="8">
         <v>2000</v>
@@ -2306,8 +2340,11 @@
       <c r="N29" s="8">
         <v>5000</v>
       </c>
-    </row>
-    <row r="30" spans="1:19">
+      <c r="V29" s="8">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -2319,7 +2356,7 @@
       </c>
       <c r="E30" s="2">
         <f t="shared" si="2"/>
-        <v>6000</v>
+        <v>8000</v>
       </c>
       <c r="H30" s="3">
         <v>1000</v>
@@ -2331,6 +2368,9 @@
         <v>2000</v>
       </c>
       <c r="S30" s="3">
+        <v>2000</v>
+      </c>
+      <c r="U30" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -2382,7 +2422,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:21">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -2394,7 +2434,7 @@
       </c>
       <c r="E34" s="2">
         <f t="shared" si="2"/>
-        <v>12000</v>
+        <v>15000</v>
       </c>
       <c r="H34" s="3">
         <v>2000</v>
@@ -2404,6 +2444,9 @@
       </c>
       <c r="P34" s="8">
         <v>6000</v>
+      </c>
+      <c r="U34" s="8">
+        <v>3000</v>
       </c>
     </row>
     <row r="35" spans="1:20">
@@ -2427,7 +2470,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:22">
       <c r="A36" s="3">
         <v>34</v>
       </c>
@@ -2439,12 +2482,15 @@
       </c>
       <c r="E36" s="2">
         <f t="shared" si="3"/>
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="J36" s="3">
         <v>3000</v>
       </c>
       <c r="O36" s="3">
+        <v>2000</v>
+      </c>
+      <c r="V36" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -2460,7 +2506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:22">
       <c r="A38" s="3">
         <v>36</v>
       </c>
@@ -2472,10 +2518,13 @@
       </c>
       <c r="E38" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20">
+        <v>2000</v>
+      </c>
+      <c r="V38" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -2487,7 +2536,7 @@
       </c>
       <c r="E39" s="2">
         <f t="shared" si="3"/>
-        <v>12000</v>
+        <v>14500</v>
       </c>
       <c r="N39" s="3">
         <v>6000</v>
@@ -2498,8 +2547,11 @@
       <c r="T39" s="3">
         <v>3000</v>
       </c>
-    </row>
-    <row r="40" spans="1:15">
+      <c r="V39" s="3">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22">
       <c r="A40" s="3">
         <v>38</v>
       </c>
@@ -2511,7 +2563,7 @@
       </c>
       <c r="E40" s="2">
         <f t="shared" si="3"/>
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="L40" s="3">
         <v>1000</v>
@@ -2520,6 +2572,9 @@
         <v>1000</v>
       </c>
       <c r="O40" s="3">
+        <v>1000</v>
+      </c>
+      <c r="V40" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -2547,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:22">
       <c r="A43" s="3">
         <v>41</v>
       </c>
@@ -2559,7 +2614,7 @@
       </c>
       <c r="E43" s="2">
         <f t="shared" si="3"/>
-        <v>6500</v>
+        <v>7500</v>
       </c>
       <c r="M43" s="3">
         <v>3000</v>
@@ -2569,6 +2624,9 @@
       </c>
       <c r="T43" s="3">
         <v>2000</v>
+      </c>
+      <c r="V43" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2595,7 +2653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:22">
       <c r="A46" s="3">
         <v>44</v>
       </c>
@@ -2607,10 +2665,13 @@
       </c>
       <c r="E46" s="2">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="J46" s="3">
         <v>1000</v>
+      </c>
+      <c r="V46" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2661,7 +2722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:20">
+    <row r="50" spans="1:22">
       <c r="A50" s="3">
         <v>48</v>
       </c>
@@ -2673,7 +2734,7 @@
       </c>
       <c r="E50" s="2">
         <f t="shared" si="3"/>
-        <v>13000</v>
+        <v>18000</v>
       </c>
       <c r="N50" s="3">
         <v>8000</v>
@@ -2681,8 +2742,11 @@
       <c r="T50" s="3">
         <v>5000</v>
       </c>
-    </row>
-    <row r="51" spans="1:15">
+      <c r="V50" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21">
       <c r="A51" s="3">
         <v>49</v>
       </c>
@@ -2694,7 +2758,7 @@
       </c>
       <c r="E51" s="2">
         <f t="shared" si="3"/>
-        <v>14500</v>
+        <v>16500</v>
       </c>
       <c r="H51" s="8">
         <v>3000</v>
@@ -2710,6 +2774,9 @@
       </c>
       <c r="O51" s="8">
         <v>4000</v>
+      </c>
+      <c r="U51" s="8">
+        <v>2000</v>
       </c>
     </row>
     <row r="52" spans="1:16">
@@ -2781,16 +2848,22 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:22">
       <c r="A55" s="3">
         <v>53</v>
       </c>
+      <c r="B55" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="D55" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E55" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="V55" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2798,23 +2871,29 @@
         <v>54</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E56" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:19">
+    <row r="57" spans="1:22">
       <c r="A57" s="3">
         <v>55</v>
       </c>
+      <c r="B57" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="D57" s="7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E57" s="2">
         <f t="shared" si="3"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="J57" s="3">
         <v>1000</v>
@@ -2824,6 +2903,9 @@
       </c>
       <c r="S57" s="8">
         <v>1000</v>
+      </c>
+      <c r="V57" s="8">
+        <v>2000</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2831,14 +2913,14 @@
         <v>56</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E58" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:19">
+    <row r="59" spans="1:22">
       <c r="A59" s="3">
         <v>57</v>
       </c>
@@ -2846,11 +2928,11 @@
         <v>17</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E59" s="2">
         <f t="shared" si="3"/>
-        <v>19000</v>
+        <v>24000</v>
       </c>
       <c r="H59" s="3">
         <v>2000</v>
@@ -2867,20 +2949,32 @@
       <c r="S59" s="8">
         <v>4500</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="U59" s="3">
+        <v>1500</v>
+      </c>
+      <c r="V59" s="8">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22">
       <c r="A60" s="3">
         <v>58</v>
       </c>
+      <c r="B60" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="D60" s="7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E60" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19">
+        <v>3000</v>
+      </c>
+      <c r="V60" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22">
       <c r="A61" s="3">
         <v>59</v>
       </c>
@@ -2888,11 +2982,11 @@
         <v>6</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E61" s="2">
         <f t="shared" si="3"/>
-        <v>6000</v>
+        <v>7000</v>
       </c>
       <c r="I61" s="3">
         <v>1000</v>
@@ -2905,6 +2999,9 @@
       </c>
       <c r="S61" s="3">
         <v>2000</v>
+      </c>
+      <c r="V61" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="62" spans="1:20">
@@ -2915,7 +3012,7 @@
         <v>15</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E62" s="2">
         <f t="shared" si="3"/>
@@ -2928,7 +3025,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="63" spans="1:19">
+    <row r="63" spans="1:21">
       <c r="A63" s="3">
         <v>61</v>
       </c>
@@ -2936,11 +3033,11 @@
         <v>15</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E63" s="2">
         <f t="shared" si="3"/>
-        <v>6000</v>
+        <v>8000</v>
       </c>
       <c r="L63" s="3">
         <v>1000</v>
@@ -2951,8 +3048,11 @@
       <c r="S63" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="64" spans="1:15">
+      <c r="U63" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21">
       <c r="A64" s="3">
         <v>62</v>
       </c>
@@ -2960,11 +3060,11 @@
         <v>6</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E64" s="2">
         <f t="shared" si="3"/>
-        <v>12000</v>
+        <v>17000</v>
       </c>
       <c r="H64" s="8">
         <v>2000</v>
@@ -2981,8 +3081,11 @@
       <c r="O64" s="8">
         <v>5000</v>
       </c>
-    </row>
-    <row r="65" spans="1:19">
+      <c r="U64" s="8">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22">
       <c r="A65" s="3">
         <v>63</v>
       </c>
@@ -2990,11 +3093,11 @@
         <v>39</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E65" s="2">
         <f t="shared" si="3"/>
-        <v>24000</v>
+        <v>28000</v>
       </c>
       <c r="H65" s="3">
         <v>2000</v>
@@ -3019,6 +3122,12 @@
       </c>
       <c r="S65" s="3">
         <v>5000</v>
+      </c>
+      <c r="U65" s="3">
+        <v>2000</v>
+      </c>
+      <c r="V65" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="66" spans="1:19">
@@ -3029,7 +3138,7 @@
         <v>15</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E66" s="2">
         <f t="shared" si="3"/>
@@ -3056,7 +3165,7 @@
         <v>13</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E67" s="2">
         <f t="shared" ref="E67:E92" si="4">SUM(F67:AJ67)</f>
@@ -3080,7 +3189,7 @@
         <v>8</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E68" s="2">
         <f t="shared" si="4"/>
@@ -3101,14 +3210,14 @@
         <v>67</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E69" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:19">
+    <row r="70" spans="1:21">
       <c r="A70" s="3">
         <v>68</v>
       </c>
@@ -3116,11 +3225,11 @@
         <v>15</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E70" s="2">
         <f t="shared" si="4"/>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="H70" s="3">
         <v>2000</v>
@@ -3134,8 +3243,11 @@
       <c r="S70" s="3">
         <v>3000</v>
       </c>
-    </row>
-    <row r="71" spans="1:19">
+      <c r="U70" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21">
       <c r="A71" s="3">
         <v>69</v>
       </c>
@@ -3143,11 +3255,11 @@
         <v>19</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E71" s="2">
         <f t="shared" si="4"/>
-        <v>9000</v>
+        <v>11000</v>
       </c>
       <c r="I71" s="3">
         <v>2000</v>
@@ -3163,6 +3275,9 @@
       </c>
       <c r="S71" s="8">
         <v>3000</v>
+      </c>
+      <c r="U71" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -3170,7 +3285,7 @@
         <v>70</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E72" s="2">
         <f t="shared" si="4"/>
@@ -3182,7 +3297,7 @@
         <v>71</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E73" s="2">
         <f t="shared" si="4"/>
@@ -3197,7 +3312,7 @@
         <v>17</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E74" s="2">
         <f t="shared" si="4"/>
@@ -3215,7 +3330,7 @@
         <v>73</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E75" s="2">
         <f t="shared" si="4"/>
@@ -3227,26 +3342,29 @@
         <v>74</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E76" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:20">
+    <row r="77" spans="1:22">
       <c r="A77" s="3">
         <v>75</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="C77" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="D77" s="7" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E77" s="2">
         <f t="shared" si="4"/>
-        <v>12000</v>
+        <v>14500</v>
       </c>
       <c r="I77" s="8">
         <v>2000</v>
@@ -3260,8 +3378,11 @@
       <c r="T77" s="8">
         <v>3000</v>
       </c>
-    </row>
-    <row r="78" spans="1:16">
+      <c r="V77" s="8">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21">
       <c r="A78" s="3">
         <v>76</v>
       </c>
@@ -3269,11 +3390,11 @@
         <v>6</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E78" s="2">
         <f t="shared" si="4"/>
-        <v>24000</v>
+        <v>34000</v>
       </c>
       <c r="I78" s="3">
         <v>2000</v>
@@ -3286,6 +3407,9 @@
       </c>
       <c r="P78" s="8">
         <v>5000</v>
+      </c>
+      <c r="U78" s="8">
+        <v>10000</v>
       </c>
     </row>
     <row r="79" spans="1:19">
@@ -3296,7 +3420,7 @@
         <v>8</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E79" s="2">
         <f t="shared" si="4"/>
@@ -3312,7 +3436,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="80" spans="1:19">
+    <row r="80" spans="1:22">
       <c r="A80" s="3">
         <v>78</v>
       </c>
@@ -3320,11 +3444,11 @@
         <v>11</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E80" s="2">
         <f t="shared" si="4"/>
-        <v>27000</v>
+        <v>32000</v>
       </c>
       <c r="J80" s="3">
         <v>2000</v>
@@ -3338,8 +3462,11 @@
       <c r="S80" s="3">
         <v>5000</v>
       </c>
-    </row>
-    <row r="81" spans="1:19">
+      <c r="V80" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:22">
       <c r="A81" s="3">
         <v>79</v>
       </c>
@@ -3347,20 +3474,23 @@
         <v>39</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E81" s="2">
         <f t="shared" si="4"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="S81" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="82" spans="1:13">
+      <c r="V81" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21">
       <c r="A82" s="3">
         <v>80</v>
       </c>
@@ -3368,11 +3498,11 @@
         <v>8</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E82" s="2">
         <f t="shared" si="4"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="I82" s="3">
         <v>1000</v>
@@ -3380,8 +3510,11 @@
       <c r="M82" s="8">
         <v>3000</v>
       </c>
-    </row>
-    <row r="83" spans="1:17">
+      <c r="U82" s="8">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21">
       <c r="A83" s="3">
         <v>81</v>
       </c>
@@ -3389,11 +3522,11 @@
         <v>8</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E83" s="2">
         <f t="shared" si="4"/>
-        <v>10000</v>
+        <v>13000</v>
       </c>
       <c r="I83" s="8">
         <v>4000</v>
@@ -3402,6 +3535,9 @@
         <v>3000</v>
       </c>
       <c r="Q83" s="3">
+        <v>3000</v>
+      </c>
+      <c r="U83" s="8">
         <v>3000</v>
       </c>
     </row>
@@ -3413,7 +3549,7 @@
         <v>39</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E84" s="2">
         <f t="shared" si="4"/>
@@ -3432,7 +3568,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="85" spans="1:15">
+    <row r="85" spans="1:21">
       <c r="A85" s="3">
         <v>83</v>
       </c>
@@ -3440,11 +3576,11 @@
         <v>17</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E85" s="2">
         <f t="shared" si="4"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="H85" s="3">
         <v>2000</v>
@@ -3454,6 +3590,9 @@
       </c>
       <c r="O85" s="3">
         <v>1000</v>
+      </c>
+      <c r="U85" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="86" spans="1:19">
@@ -3464,7 +3603,7 @@
         <v>11</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E86" s="2">
         <f t="shared" si="4"/>
@@ -3491,7 +3630,7 @@
         <v>15</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E87" s="2">
         <f t="shared" si="4"/>
@@ -3512,14 +3651,14 @@
         <v>15</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E88" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:19">
+    <row r="89" spans="1:22">
       <c r="A89" s="3">
         <v>87</v>
       </c>
@@ -3527,11 +3666,11 @@
         <v>17</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="E89" s="2">
         <f t="shared" si="4"/>
-        <v>20000</v>
+        <v>25000</v>
       </c>
       <c r="H89" s="3">
         <v>2000</v>
@@ -3548,8 +3687,11 @@
       <c r="S89" s="3">
         <v>5000</v>
       </c>
-    </row>
-    <row r="90" spans="1:20">
+      <c r="V89" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:22">
       <c r="A90" s="3">
         <v>88</v>
       </c>
@@ -3557,11 +3699,11 @@
         <v>6</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E90" s="2">
         <f t="shared" si="4"/>
-        <v>6000</v>
+        <v>7500</v>
       </c>
       <c r="I90" s="3">
         <v>1000</v>
@@ -3580,6 +3722,12 @@
       </c>
       <c r="T90" s="3">
         <v>1000</v>
+      </c>
+      <c r="U90" s="3">
+        <v>1000</v>
+      </c>
+      <c r="V90" s="3">
+        <v>500</v>
       </c>
     </row>
     <row r="91" spans="1:20">
@@ -3590,7 +3738,7 @@
         <v>15</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="E91" s="2">
         <f t="shared" si="4"/>
@@ -3614,7 +3762,7 @@
         <v>90</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E92" s="2">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
updated data at 21Dec 8AM
</commit_message>
<xml_diff>
--- a/Daily Collection/December-2020-Collection.xlsx
+++ b/Daily Collection/December-2020-Collection.xlsx
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="112">
   <si>
     <t>S.No.</t>
   </si>
@@ -436,6 +436,9 @@
     <t>SANDEEP TELECOM(661066825)</t>
   </si>
   <si>
+    <t>RAJESH TELECOM &amp; KIRANA DUKAN(661063895)</t>
+  </si>
+  <si>
     <t>BELSAR</t>
   </si>
   <si>
@@ -491,9 +494,6 @@
   </si>
   <si>
     <t>MUSKAN COMMUNICATION(662077126)</t>
-  </si>
-  <si>
-    <t>RAJESH TELECOM &amp; KIRANA DUKAN(661063895)</t>
   </si>
   <si>
     <t>KRISHNA KIRANA STORE(661613674)</t>
@@ -531,11 +531,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -563,48 +563,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -624,9 +586,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -640,7 +609,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -648,7 +617,37 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -662,10 +661,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -677,14 +685,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -692,7 +692,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -742,67 +742,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -820,7 +760,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -832,7 +850,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -844,37 +868,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -886,37 +916,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -936,36 +936,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -982,6 +956,21 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1004,23 +993,34 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1028,8 +1028,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1038,15 +1038,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1056,31 +1056,31 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1089,101 +1089,101 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1196,7 +1196,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1205,7 +1208,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1541,11 +1544,11 @@
   <dimension ref="A1:AJ92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="Q45" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:A92"/>
+      <selection pane="bottomRight" activeCell="Y61" sqref="Y61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1554,7 +1557,7 @@
     <col min="2" max="2" width="11.5714285714286" style="3" customWidth="1"/>
     <col min="3" max="3" width="15" style="3" customWidth="1"/>
     <col min="4" max="4" width="51.1428571428571" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11" style="4" customWidth="1"/>
     <col min="6" max="16384" width="9.14285714285714" style="3"/>
   </cols>
   <sheetData>
@@ -1574,107 +1577,107 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="5">
         <v>44166</v>
       </c>
-      <c r="G1" s="4">
+      <c r="G1" s="5">
         <v>44167</v>
       </c>
-      <c r="H1" s="4">
+      <c r="H1" s="5">
         <v>44168</v>
       </c>
-      <c r="I1" s="4">
+      <c r="I1" s="5">
         <v>44169</v>
       </c>
-      <c r="J1" s="4">
+      <c r="J1" s="5">
         <v>44170</v>
       </c>
-      <c r="K1" s="4">
+      <c r="K1" s="5">
         <v>44171</v>
       </c>
-      <c r="L1" s="4">
+      <c r="L1" s="5">
         <v>44172</v>
       </c>
-      <c r="M1" s="4">
+      <c r="M1" s="5">
         <v>44173</v>
       </c>
-      <c r="N1" s="4">
+      <c r="N1" s="5">
         <v>44174</v>
       </c>
-      <c r="O1" s="4">
+      <c r="O1" s="5">
         <v>44175</v>
       </c>
-      <c r="P1" s="4">
+      <c r="P1" s="5">
         <v>44176</v>
       </c>
-      <c r="Q1" s="4">
+      <c r="Q1" s="5">
         <v>44177</v>
       </c>
-      <c r="R1" s="4">
+      <c r="R1" s="5">
         <v>44178</v>
       </c>
-      <c r="S1" s="4">
+      <c r="S1" s="5">
         <v>44179</v>
       </c>
-      <c r="T1" s="4">
+      <c r="T1" s="5">
         <v>44180</v>
       </c>
-      <c r="U1" s="4">
+      <c r="U1" s="5">
         <v>44181</v>
       </c>
-      <c r="V1" s="4">
+      <c r="V1" s="5">
         <v>44182</v>
       </c>
-      <c r="W1" s="4">
+      <c r="W1" s="5">
         <v>44183</v>
       </c>
-      <c r="X1" s="4">
+      <c r="X1" s="5">
         <v>44184</v>
       </c>
-      <c r="Y1" s="4">
+      <c r="Y1" s="5">
         <v>44185</v>
       </c>
-      <c r="Z1" s="4">
+      <c r="Z1" s="5">
         <v>44186</v>
       </c>
-      <c r="AA1" s="4">
+      <c r="AA1" s="5">
         <v>44187</v>
       </c>
-      <c r="AB1" s="4">
+      <c r="AB1" s="5">
         <v>44188</v>
       </c>
-      <c r="AC1" s="4">
+      <c r="AC1" s="5">
         <v>44189</v>
       </c>
-      <c r="AD1" s="4">
+      <c r="AD1" s="5">
         <v>44190</v>
       </c>
-      <c r="AE1" s="4">
+      <c r="AE1" s="5">
         <v>44191</v>
       </c>
-      <c r="AF1" s="4">
+      <c r="AF1" s="5">
         <v>44192</v>
       </c>
-      <c r="AG1" s="4">
+      <c r="AG1" s="5">
         <v>44193</v>
       </c>
-      <c r="AH1" s="4">
+      <c r="AH1" s="5">
         <v>44194</v>
       </c>
-      <c r="AI1" s="4">
+      <c r="AI1" s="5">
         <v>44195</v>
       </c>
-      <c r="AJ1" s="4">
+      <c r="AJ1" s="5">
         <v>44196</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" spans="4:36">
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="7">
         <f>SUM(F2:AJ2)</f>
-        <v>674800</v>
+        <v>723900</v>
       </c>
       <c r="F2" s="2">
         <f>SUM(F3:F92)</f>
@@ -1750,11 +1753,11 @@
       </c>
       <c r="X2" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>42100</v>
       </c>
       <c r="Y2" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7000</v>
       </c>
       <c r="Z2" s="2">
         <f t="shared" si="1"/>
@@ -1808,13 +1811,14 @@
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2">
-        <v>3000</v>
-      </c>
-      <c r="U3" s="8">
+      <c r="E3" s="8">
+        <f t="shared" ref="E3:E34" si="2">SUM(F3:AJ3)</f>
+        <v>3000</v>
+      </c>
+      <c r="U3" s="9">
         <v>3000</v>
       </c>
     </row>
@@ -1825,29 +1829,30 @@
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="2">
-        <v>2000</v>
-      </c>
-      <c r="K4" s="8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" s="3" customFormat="1" spans="1:23">
+      <c r="E4" s="8">
+        <f t="shared" si="2"/>
+        <v>2000</v>
+      </c>
+      <c r="K4" s="9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" s="3" customFormat="1" spans="1:24">
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="2">
-        <v>9000</v>
+      <c r="E5" s="8">
+        <f t="shared" si="2"/>
+        <v>10000</v>
       </c>
       <c r="H5" s="3">
         <v>1000</v>
@@ -1867,74 +1872,83 @@
       <c r="W5" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="6" s="3" customFormat="1" spans="1:21">
+      <c r="X5" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" s="3" customFormat="1" spans="1:24">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="2">
-        <v>16500</v>
-      </c>
-      <c r="H6" s="8">
-        <v>3000</v>
-      </c>
-      <c r="J6" s="8">
-        <v>2000</v>
-      </c>
-      <c r="K6" s="8">
+      <c r="E6" s="8">
+        <f t="shared" si="2"/>
+        <v>19500</v>
+      </c>
+      <c r="H6" s="9">
+        <v>3000</v>
+      </c>
+      <c r="J6" s="9">
+        <v>2000</v>
+      </c>
+      <c r="K6" s="9">
         <v>1500</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="9">
         <v>4000</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="9">
         <v>4000</v>
       </c>
-      <c r="P6" s="3"/>
-      <c r="U6" s="8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="7" s="3" customFormat="1" spans="1:22">
+      <c r="U6" s="9">
+        <v>2000</v>
+      </c>
+      <c r="X6" s="9">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="7" s="3" customFormat="1" spans="1:24">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="2">
-        <v>24000</v>
+      <c r="E7" s="8">
+        <f t="shared" si="2"/>
+        <v>29000</v>
       </c>
       <c r="H7" s="3">
         <v>2000</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="9">
         <v>6000</v>
       </c>
-      <c r="O7" s="8">
+      <c r="O7" s="9">
         <v>5000</v>
       </c>
-      <c r="Q7" s="8">
+      <c r="Q7" s="9">
         <v>1500</v>
       </c>
-      <c r="S7" s="8">
+      <c r="S7" s="9">
         <v>4500</v>
       </c>
-      <c r="T7" s="3"/>
       <c r="U7" s="3">
         <v>1500</v>
       </c>
-      <c r="V7" s="8">
+      <c r="V7" s="9">
         <v>3500</v>
+      </c>
+      <c r="X7" s="3">
+        <v>5000</v>
       </c>
     </row>
     <row r="8" s="3" customFormat="1" spans="1:23">
@@ -1944,10 +1958,11 @@
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="8">
+        <f t="shared" si="2"/>
         <v>5000</v>
       </c>
       <c r="N8" s="3">
@@ -1967,10 +1982,11 @@
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="8">
+        <f t="shared" si="2"/>
         <v>6000</v>
       </c>
       <c r="H9" s="3">
@@ -1993,16 +2009,16 @@
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="8">
+        <f t="shared" si="2"/>
         <v>25000</v>
       </c>
       <c r="H10" s="3">
         <v>2000</v>
       </c>
-      <c r="I10" s="3"/>
       <c r="J10" s="3">
         <v>4000</v>
       </c>
@@ -2026,22 +2042,23 @@
       <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="8">
+        <f t="shared" si="2"/>
         <v>11000</v>
       </c>
-      <c r="H11" s="8">
-        <v>2000</v>
-      </c>
-      <c r="K11" s="8">
-        <v>2000</v>
-      </c>
-      <c r="N11" s="8">
+      <c r="H11" s="9">
+        <v>2000</v>
+      </c>
+      <c r="K11" s="9">
+        <v>2000</v>
+      </c>
+      <c r="N11" s="9">
         <v>5000</v>
       </c>
-      <c r="V11" s="8">
+      <c r="V11" s="9">
         <v>2000</v>
       </c>
     </row>
@@ -2052,10 +2069,11 @@
       <c r="C12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="8">
+        <f t="shared" si="2"/>
         <v>4000</v>
       </c>
       <c r="L12" s="3">
@@ -2078,24 +2096,22 @@
       <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="8">
+        <f t="shared" si="2"/>
         <v>23000</v>
       </c>
       <c r="H13" s="3">
         <v>2000</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="L13" s="8">
+      <c r="L13" s="9">
         <v>6000</v>
       </c>
-      <c r="M13" s="3"/>
       <c r="N13" s="3">
         <v>5000</v>
       </c>
-      <c r="O13" s="3"/>
       <c r="Q13" s="3">
         <v>5000</v>
       </c>
@@ -2103,23 +2119,23 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="14" s="3" customFormat="1" spans="1:23">
+    <row r="14" s="3" customFormat="1" spans="1:24">
       <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="2">
-        <v>29000</v>
+      <c r="E14" s="8">
+        <f t="shared" si="2"/>
+        <v>30000</v>
       </c>
       <c r="H14" s="3">
         <v>2000</v>
       </c>
-      <c r="I14" s="3"/>
       <c r="K14" s="3">
         <v>4000</v>
       </c>
@@ -2148,6 +2164,9 @@
         <v>2000</v>
       </c>
       <c r="W14" s="3">
+        <v>1000</v>
+      </c>
+      <c r="X14" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -2161,10 +2180,11 @@
       <c r="C15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="8">
+        <f t="shared" si="2"/>
         <v>4000</v>
       </c>
       <c r="S15" s="3">
@@ -2181,10 +2201,11 @@
       <c r="C16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="8">
+        <f t="shared" si="2"/>
         <v>12000</v>
       </c>
       <c r="M16" s="3">
@@ -2210,10 +2231,11 @@
       <c r="C17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="8">
+        <f t="shared" si="2"/>
         <v>19000</v>
       </c>
       <c r="I17" s="3">
@@ -2222,14 +2244,14 @@
       <c r="L17" s="3">
         <v>6000</v>
       </c>
-      <c r="N17" s="8">
+      <c r="N17" s="9">
         <v>5000</v>
       </c>
-      <c r="S17" s="8">
+      <c r="S17" s="9">
         <v>5000</v>
       </c>
     </row>
-    <row r="18" s="3" customFormat="1" spans="1:23">
+    <row r="18" s="3" customFormat="1" spans="1:24">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -2239,17 +2261,20 @@
       <c r="C18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="2">
-        <v>2000</v>
-      </c>
-      <c r="S18" s="8">
-        <v>1000</v>
-      </c>
-      <c r="T18" s="3"/>
-      <c r="W18" s="8">
+      <c r="E18" s="8">
+        <f t="shared" si="2"/>
+        <v>3000</v>
+      </c>
+      <c r="S18" s="9">
+        <v>1000</v>
+      </c>
+      <c r="W18" s="9">
+        <v>1000</v>
+      </c>
+      <c r="X18" s="9">
         <v>1000</v>
       </c>
     </row>
@@ -2260,10 +2285,11 @@
       <c r="C19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="8">
+        <f t="shared" si="2"/>
         <v>7500</v>
       </c>
       <c r="I19" s="3">
@@ -2282,24 +2308,28 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="20" s="3" customFormat="1" spans="1:20">
+    <row r="20" s="3" customFormat="1" spans="1:24">
       <c r="A20" s="3">
         <v>18</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="2">
-        <v>12000</v>
-      </c>
-      <c r="P20" s="8">
+      <c r="E20" s="8">
+        <f t="shared" si="2"/>
+        <v>17000</v>
+      </c>
+      <c r="P20" s="9">
         <v>5000</v>
       </c>
-      <c r="T20" s="8">
+      <c r="T20" s="9">
         <v>7000</v>
+      </c>
+      <c r="X20" s="9">
+        <v>5000</v>
       </c>
     </row>
     <row r="21" s="3" customFormat="1" spans="1:23">
@@ -2309,10 +2339,11 @@
       <c r="C21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="8">
+        <f t="shared" si="2"/>
         <v>6000</v>
       </c>
       <c r="I21" s="3">
@@ -2338,10 +2369,11 @@
       <c r="C22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="8">
+        <f t="shared" si="2"/>
         <v>12000</v>
       </c>
       <c r="I22" s="3">
@@ -2364,21 +2396,20 @@
       <c r="C23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="8">
+        <f t="shared" si="2"/>
         <v>12000</v>
       </c>
-      <c r="S23" s="8">
-        <v>2000</v>
-      </c>
-      <c r="T23" s="8">
+      <c r="S23" s="9">
+        <v>2000</v>
+      </c>
+      <c r="T23" s="9">
         <v>5000</v>
       </c>
-      <c r="U23" s="3"/>
-      <c r="V23" s="3"/>
-      <c r="W23" s="8">
+      <c r="W23" s="9">
         <v>5000</v>
       </c>
     </row>
@@ -2389,10 +2420,11 @@
       <c r="C24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="8">
+        <f t="shared" si="2"/>
         <v>15000</v>
       </c>
       <c r="N24" s="3">
@@ -2411,18 +2443,19 @@
         <v>500</v>
       </c>
     </row>
-    <row r="25" s="3" customFormat="1" spans="1:22">
+    <row r="25" s="3" customFormat="1" spans="1:24">
       <c r="A25" s="3">
         <v>23</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="2">
-        <v>7500</v>
+      <c r="E25" s="8">
+        <f t="shared" si="2"/>
+        <v>8500</v>
       </c>
       <c r="M25" s="3">
         <v>3000</v>
@@ -2434,6 +2467,9 @@
         <v>2000</v>
       </c>
       <c r="V25" s="3">
+        <v>1000</v>
+      </c>
+      <c r="X25" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -2444,10 +2480,11 @@
       <c r="C26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="8">
+        <f t="shared" si="2"/>
         <v>3000</v>
       </c>
       <c r="V26" s="3">
@@ -2461,10 +2498,11 @@
       <c r="C27" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="8">
+        <f t="shared" si="2"/>
         <v>8000</v>
       </c>
       <c r="I27" s="3">
@@ -2493,30 +2531,29 @@
       <c r="C28" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="8">
+        <f t="shared" si="2"/>
         <v>17000</v>
       </c>
-      <c r="H28" s="8">
-        <v>2000</v>
-      </c>
-      <c r="I28" s="8">
-        <v>1000</v>
-      </c>
-      <c r="K28" s="8">
-        <v>3000</v>
-      </c>
-      <c r="L28" s="3"/>
-      <c r="M28" s="8">
-        <v>1000</v>
-      </c>
-      <c r="N28" s="3"/>
-      <c r="O28" s="8">
+      <c r="H28" s="9">
+        <v>2000</v>
+      </c>
+      <c r="I28" s="9">
+        <v>1000</v>
+      </c>
+      <c r="K28" s="9">
+        <v>3000</v>
+      </c>
+      <c r="M28" s="9">
+        <v>1000</v>
+      </c>
+      <c r="O28" s="9">
         <v>5000</v>
       </c>
-      <c r="U28" s="8">
+      <c r="U28" s="9">
         <v>5000</v>
       </c>
     </row>
@@ -2527,49 +2564,49 @@
       <c r="C29" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="8">
+        <f t="shared" si="2"/>
         <v>39000</v>
       </c>
       <c r="I29" s="3">
         <v>2000</v>
       </c>
-      <c r="K29" s="8">
+      <c r="K29" s="9">
         <v>12000</v>
       </c>
       <c r="N29" s="3">
         <v>5000</v>
       </c>
-      <c r="P29" s="8">
+      <c r="P29" s="9">
         <v>5000</v>
       </c>
-      <c r="U29" s="8">
+      <c r="U29" s="9">
         <v>10000</v>
       </c>
-      <c r="V29" s="3"/>
       <c r="W29" s="3">
         <v>5000</v>
       </c>
     </row>
-    <row r="30" s="3" customFormat="1" spans="1:23">
+    <row r="30" s="3" customFormat="1" spans="1:24">
       <c r="A30" s="3">
         <v>28</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="2">
-        <v>9000</v>
+      <c r="E30" s="8">
+        <f t="shared" si="2"/>
+        <v>9500</v>
       </c>
       <c r="I30" s="3">
         <v>1000</v>
       </c>
-      <c r="J30" s="3"/>
       <c r="K30" s="3">
         <v>1000</v>
       </c>
@@ -2593,6 +2630,9 @@
       </c>
       <c r="W30" s="3">
         <v>1500</v>
+      </c>
+      <c r="X30" s="3">
+        <v>500</v>
       </c>
     </row>
     <row r="31" s="3" customFormat="1" spans="1:23">
@@ -2602,10 +2642,11 @@
       <c r="C31" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="8">
+        <f t="shared" si="2"/>
         <v>8000</v>
       </c>
       <c r="H31" s="3">
@@ -2628,10 +2669,11 @@
       <c r="C32" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="8">
+        <f t="shared" si="2"/>
         <v>5000</v>
       </c>
       <c r="H32" s="3">
@@ -2657,23 +2699,22 @@
       <c r="C33" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="8">
+        <f t="shared" si="2"/>
         <v>3000</v>
       </c>
       <c r="H33" s="3">
         <v>1000</v>
       </c>
-      <c r="I33" s="3"/>
       <c r="L33" s="3">
         <v>1000</v>
       </c>
       <c r="N33" s="3">
         <v>900</v>
       </c>
-      <c r="O33" s="3"/>
       <c r="Q33" s="3">
         <v>100</v>
       </c>
@@ -2685,10 +2726,11 @@
       <c r="C34" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="8">
+        <f t="shared" si="2"/>
         <v>18000</v>
       </c>
       <c r="H34" s="3">
@@ -2697,13 +2739,13 @@
       <c r="L34" s="3">
         <v>4000</v>
       </c>
-      <c r="P34" s="8">
+      <c r="P34" s="9">
         <v>6000</v>
       </c>
-      <c r="U34" s="8">
-        <v>3000</v>
-      </c>
-      <c r="W34" s="8">
+      <c r="U34" s="9">
+        <v>3000</v>
+      </c>
+      <c r="W34" s="9">
         <v>3000</v>
       </c>
     </row>
@@ -2714,10 +2756,11 @@
       <c r="C35" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="8">
+        <f t="shared" ref="E35:E66" si="3">SUM(F35:AJ35)</f>
         <v>2000</v>
       </c>
       <c r="V35" s="3">
@@ -2731,22 +2774,23 @@
       <c r="C36" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="8">
+        <f t="shared" si="3"/>
         <v>15000</v>
       </c>
-      <c r="H36" s="8">
-        <v>3000</v>
-      </c>
-      <c r="L36" s="8">
-        <v>3000</v>
-      </c>
-      <c r="Q36" s="8">
-        <v>3000</v>
-      </c>
-      <c r="S36" s="8">
+      <c r="H36" s="9">
+        <v>3000</v>
+      </c>
+      <c r="L36" s="9">
+        <v>3000</v>
+      </c>
+      <c r="Q36" s="9">
+        <v>3000</v>
+      </c>
+      <c r="S36" s="9">
         <v>3000</v>
       </c>
       <c r="W36" s="3">
@@ -2760,16 +2804,17 @@
       <c r="C37" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="8">
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="J37" s="3">
         <v>2000</v>
       </c>
-      <c r="T37" s="8">
+      <c r="T37" s="9">
         <v>2000</v>
       </c>
     </row>
@@ -2780,10 +2825,11 @@
       <c r="C38" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="8">
+        <f t="shared" si="3"/>
         <v>8000</v>
       </c>
       <c r="L38" s="3">
@@ -2806,10 +2852,11 @@
       <c r="C39" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="8">
+        <f t="shared" si="3"/>
         <v>7000</v>
       </c>
       <c r="H39" s="3">
@@ -2832,10 +2879,11 @@
       <c r="C40" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40" s="8">
+        <f t="shared" si="3"/>
         <v>21000</v>
       </c>
       <c r="H40" s="3">
@@ -2847,14 +2895,12 @@
       <c r="N40" s="3">
         <v>6000</v>
       </c>
-      <c r="O40" s="3"/>
       <c r="S40" s="3">
         <v>3000</v>
       </c>
       <c r="U40" s="3">
         <v>3000</v>
       </c>
-      <c r="V40" s="3"/>
       <c r="W40" s="3">
         <v>3000</v>
       </c>
@@ -2866,10 +2912,11 @@
       <c r="C41" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="8">
+        <f t="shared" si="3"/>
         <v>3000</v>
       </c>
       <c r="K41" s="3">
@@ -2886,10 +2933,11 @@
       <c r="C42" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="8">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2900,19 +2948,20 @@
       <c r="C43" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43" s="8">
+        <f t="shared" si="3"/>
         <v>15000</v>
       </c>
-      <c r="H43" s="8">
+      <c r="H43" s="9">
         <v>5000</v>
       </c>
-      <c r="M43" s="8">
-        <v>3000</v>
-      </c>
-      <c r="S43" s="8">
+      <c r="M43" s="9">
+        <v>3000</v>
+      </c>
+      <c r="S43" s="9">
         <v>1000</v>
       </c>
       <c r="T43" s="3">
@@ -2922,18 +2971,19 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="44" s="3" customFormat="1" spans="1:20">
+    <row r="44" s="3" customFormat="1" spans="1:24">
       <c r="A44" s="3">
         <v>42</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E44" s="2">
-        <v>11000</v>
+      <c r="E44" s="8">
+        <f t="shared" si="3"/>
+        <v>14000</v>
       </c>
       <c r="I44" s="3">
         <v>5000</v>
@@ -2944,19 +2994,23 @@
       <c r="T44" s="3">
         <v>3000</v>
       </c>
-    </row>
-    <row r="45" s="3" customFormat="1" spans="1:22">
+      <c r="X44" s="9">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="45" s="3" customFormat="1" spans="1:24">
       <c r="A45" s="3">
         <v>43</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E45" s="2">
-        <v>13000</v>
+      <c r="E45" s="8">
+        <f t="shared" si="3"/>
+        <v>16000</v>
       </c>
       <c r="I45" s="3">
         <v>2000</v>
@@ -2971,6 +3025,9 @@
         <v>3000</v>
       </c>
       <c r="V45" s="3">
+        <v>3000</v>
+      </c>
+      <c r="X45" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -2981,44 +3038,48 @@
       <c r="C46" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46" s="8">
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
-      <c r="I46" s="8">
-        <v>2000</v>
-      </c>
-      <c r="J46" s="3"/>
-      <c r="S46" s="8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="47" s="3" customFormat="1" spans="1:20">
+      <c r="I46" s="9">
+        <v>2000</v>
+      </c>
+      <c r="S46" s="9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="47" s="3" customFormat="1" spans="1:24">
       <c r="A47" s="3">
         <v>45</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E47" s="2">
-        <v>8000</v>
+      <c r="E47" s="8">
+        <f t="shared" si="3"/>
+        <v>11000</v>
       </c>
       <c r="O47" s="3">
         <v>2000</v>
       </c>
-      <c r="S47" s="8">
-        <v>3000</v>
-      </c>
-      <c r="T47" s="8">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="48" s="3" customFormat="1" spans="1:22">
+      <c r="S47" s="9">
+        <v>3000</v>
+      </c>
+      <c r="T47" s="9">
+        <v>3000</v>
+      </c>
+      <c r="X47" s="9">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="48" s="3" customFormat="1" spans="1:24">
       <c r="A48" s="3">
         <v>46</v>
       </c>
@@ -3028,13 +3089,14 @@
       <c r="C48" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E48" s="2">
-        <v>14500</v>
-      </c>
-      <c r="I48" s="8">
+      <c r="E48" s="8">
+        <f t="shared" si="3"/>
+        <v>15000</v>
+      </c>
+      <c r="I48" s="9">
         <v>2000</v>
       </c>
       <c r="M48" s="3">
@@ -3043,25 +3105,29 @@
       <c r="O48" s="3">
         <v>3000</v>
       </c>
-      <c r="T48" s="8">
-        <v>3000</v>
-      </c>
-      <c r="V48" s="8">
+      <c r="T48" s="9">
+        <v>3000</v>
+      </c>
+      <c r="V48" s="9">
         <v>2500</v>
       </c>
-    </row>
-    <row r="49" s="3" customFormat="1" spans="1:19">
+      <c r="X48" s="9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="49" s="3" customFormat="1" spans="1:24">
       <c r="A49" s="3">
         <v>47</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E49" s="2">
-        <v>5000</v>
+      <c r="E49" s="8">
+        <f t="shared" si="3"/>
+        <v>7000</v>
       </c>
       <c r="I49" s="3">
         <v>1000</v>
@@ -3069,7 +3135,10 @@
       <c r="O49" s="3">
         <v>2000</v>
       </c>
-      <c r="S49" s="8">
+      <c r="S49" s="9">
+        <v>2000</v>
+      </c>
+      <c r="X49" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -3080,24 +3149,24 @@
       <c r="C50" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E50" s="8">
+        <f t="shared" si="3"/>
         <v>6000</v>
       </c>
       <c r="I50" s="3">
         <v>1000</v>
       </c>
-      <c r="M50" s="8">
-        <v>3000</v>
-      </c>
-      <c r="N50" s="3"/>
-      <c r="U50" s="8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="51" s="3" customFormat="1" spans="1:23">
+      <c r="M50" s="9">
+        <v>3000</v>
+      </c>
+      <c r="U50" s="9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="51" s="3" customFormat="1" spans="1:24">
       <c r="A51" s="3">
         <v>49</v>
       </c>
@@ -3107,50 +3176,54 @@
       <c r="C51" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E51" s="2">
-        <v>15000</v>
-      </c>
-      <c r="I51" s="8">
+      <c r="E51" s="8">
+        <f t="shared" si="3"/>
+        <v>16000</v>
+      </c>
+      <c r="I51" s="9">
         <v>4000</v>
       </c>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="M51" s="8">
-        <v>3000</v>
-      </c>
-      <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
+      <c r="M51" s="9">
+        <v>3000</v>
+      </c>
       <c r="Q51" s="3">
         <v>3000</v>
       </c>
-      <c r="U51" s="8">
-        <v>3000</v>
-      </c>
-      <c r="W51" s="8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="52" s="3" customFormat="1" spans="1:20">
+      <c r="U51" s="9">
+        <v>3000</v>
+      </c>
+      <c r="W51" s="9">
+        <v>2000</v>
+      </c>
+      <c r="X51" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="52" s="3" customFormat="1" spans="1:24">
       <c r="A52" s="3">
         <v>50</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E52" s="2">
-        <v>5000</v>
+      <c r="E52" s="8">
+        <f t="shared" si="3"/>
+        <v>7000</v>
       </c>
       <c r="Q52" s="3">
         <v>1000</v>
       </c>
       <c r="T52" s="3">
         <v>4000</v>
+      </c>
+      <c r="X52" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="53" s="3" customFormat="1" spans="1:22">
@@ -3160,10 +3233,11 @@
       <c r="C53" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E53" s="8">
+        <f t="shared" si="3"/>
         <v>18000</v>
       </c>
       <c r="N53" s="3">
@@ -3183,10 +3257,11 @@
       <c r="C54" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E54" s="2">
+      <c r="E54" s="8">
+        <f t="shared" si="3"/>
         <v>3500</v>
       </c>
       <c r="L54" s="3">
@@ -3206,14 +3281,14 @@
       <c r="C55" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E55" s="2">
-        <f t="shared" ref="E55:E57" si="2">SUM(F55:AJ55)</f>
+      <c r="E55" s="8">
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
-      <c r="O55" s="8">
+      <c r="O55" s="9">
         <v>4000</v>
       </c>
     </row>
@@ -3227,23 +3302,23 @@
       <c r="C56" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E56" s="2">
-        <f t="shared" si="2"/>
+      <c r="E56" s="8">
+        <f t="shared" si="3"/>
         <v>6000</v>
       </c>
       <c r="J56" s="3">
         <v>1000</v>
       </c>
-      <c r="Q56" s="8">
-        <v>2000</v>
-      </c>
-      <c r="S56" s="8">
-        <v>1000</v>
-      </c>
-      <c r="V56" s="8">
+      <c r="Q56" s="9">
+        <v>2000</v>
+      </c>
+      <c r="S56" s="9">
+        <v>1000</v>
+      </c>
+      <c r="V56" s="9">
         <v>2000</v>
       </c>
     </row>
@@ -3251,15 +3326,14 @@
       <c r="A57" s="3">
         <v>55</v>
       </c>
-      <c r="B57" s="3"/>
       <c r="C57" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E57" s="2">
-        <f t="shared" si="2"/>
+      <c r="E57" s="8">
+        <f t="shared" si="3"/>
         <v>2000</v>
       </c>
       <c r="V57" s="3">
@@ -3273,10 +3347,11 @@
       <c r="C58" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E58" s="8">
+        <f t="shared" si="3"/>
         <v>7000</v>
       </c>
       <c r="P58" s="3">
@@ -3293,10 +3368,11 @@
       <c r="C59" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E59" s="2">
+      <c r="E59" s="8">
+        <f t="shared" si="3"/>
         <v>7000</v>
       </c>
       <c r="J59" s="3">
@@ -3309,18 +3385,19 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="60" s="3" customFormat="1" spans="1:22">
+    <row r="60" s="3" customFormat="1" spans="1:25">
       <c r="A60" s="3">
         <v>58</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E60" s="2">
-        <v>3000</v>
+      <c r="E60" s="8">
+        <f t="shared" si="3"/>
+        <v>5000</v>
       </c>
       <c r="J60" s="3">
         <v>1000</v>
@@ -3328,36 +3405,44 @@
       <c r="V60" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="61" s="3" customFormat="1" spans="1:10">
+      <c r="Y60" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="61" s="3" customFormat="1" spans="1:24">
       <c r="A61" s="3">
         <v>59</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E61" s="2">
-        <v>2000</v>
+      <c r="E61" s="8">
+        <f t="shared" si="3"/>
+        <v>3000</v>
       </c>
       <c r="J61" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="62" s="3" customFormat="1" spans="1:22">
+      <c r="X61" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="62" s="3" customFormat="1" spans="1:25">
       <c r="A62" s="3">
         <v>60</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D62" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E62" s="2">
-        <v>32000</v>
+      <c r="E62" s="8">
+        <f t="shared" si="3"/>
+        <v>37000</v>
       </c>
       <c r="J62" s="3">
         <v>2000</v>
@@ -3371,8 +3456,10 @@
       <c r="S62" s="3">
         <v>5000</v>
       </c>
-      <c r="T62" s="3"/>
       <c r="V62" s="3">
+        <v>5000</v>
+      </c>
+      <c r="Y62" s="3">
         <v>5000</v>
       </c>
     </row>
@@ -3383,13 +3470,14 @@
       <c r="C63" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E63" s="2">
+      <c r="E63" s="8">
+        <f t="shared" si="3"/>
         <v>15000</v>
       </c>
-      <c r="K63" s="8">
+      <c r="K63" s="9">
         <v>4000</v>
       </c>
       <c r="L63" s="3">
@@ -3405,162 +3493,180 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="64" s="3" customFormat="1" spans="1:23">
+    <row r="64" s="3" customFormat="1" spans="1:24">
       <c r="A64" s="3">
         <v>62</v>
       </c>
       <c r="C64" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D64" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E64" s="2">
-        <v>10300</v>
-      </c>
-      <c r="I64" s="8">
-        <v>1000</v>
-      </c>
-      <c r="L64" s="8">
-        <v>2000</v>
-      </c>
-      <c r="M64" s="3"/>
-      <c r="S64" s="3">
-        <v>2000</v>
-      </c>
-      <c r="U64" s="3">
-        <v>2500</v>
-      </c>
-      <c r="V64" s="3">
-        <v>1000</v>
-      </c>
-      <c r="W64" s="3">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="65" s="3" customFormat="1" spans="1:20">
+      <c r="E64" s="8">
+        <f t="shared" si="3"/>
+        <v>1500</v>
+      </c>
+      <c r="X64" s="3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="65" s="3" customFormat="1" spans="1:24">
       <c r="A65" s="3">
         <v>63</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D65" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D65" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E65" s="2">
-        <v>15000</v>
-      </c>
-      <c r="J65" s="8">
-        <v>3000</v>
-      </c>
-      <c r="K65" s="3"/>
-      <c r="L65" s="8">
-        <v>3000</v>
-      </c>
-      <c r="O65" s="3">
-        <v>3000</v>
-      </c>
-      <c r="P65" s="3"/>
-      <c r="Q65" s="3"/>
+      <c r="E65" s="8">
+        <f t="shared" si="3"/>
+        <v>10900</v>
+      </c>
+      <c r="I65" s="9">
+        <v>1000</v>
+      </c>
+      <c r="L65" s="9">
+        <v>2000</v>
+      </c>
       <c r="S65" s="3">
-        <v>3000</v>
-      </c>
-      <c r="T65" s="3">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="66" s="3" customFormat="1" spans="1:21">
+        <v>2000</v>
+      </c>
+      <c r="U65" s="3">
+        <v>2500</v>
+      </c>
+      <c r="V65" s="3">
+        <v>1000</v>
+      </c>
+      <c r="W65" s="3">
+        <v>1800</v>
+      </c>
+      <c r="X65" s="3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="66" s="3" customFormat="1" spans="1:24">
       <c r="A66" s="3">
         <v>64</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D66" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D66" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E66" s="2">
-        <v>11000</v>
-      </c>
-      <c r="I66" s="3">
-        <v>2000</v>
-      </c>
-      <c r="K66" s="3">
-        <v>1000</v>
-      </c>
-      <c r="L66" s="3"/>
-      <c r="N66" s="3">
-        <v>2000</v>
-      </c>
-      <c r="Q66" s="3">
-        <v>1000</v>
-      </c>
-      <c r="S66" s="8">
-        <v>3000</v>
-      </c>
-      <c r="U66" s="3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="67" s="3" customFormat="1" spans="1:5">
+      <c r="E66" s="8">
+        <f t="shared" si="3"/>
+        <v>18000</v>
+      </c>
+      <c r="J66" s="9">
+        <v>3000</v>
+      </c>
+      <c r="L66" s="9">
+        <v>3000</v>
+      </c>
+      <c r="O66" s="3">
+        <v>3000</v>
+      </c>
+      <c r="S66" s="3">
+        <v>3000</v>
+      </c>
+      <c r="T66" s="3">
+        <v>3000</v>
+      </c>
+      <c r="X66" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="67" s="3" customFormat="1" spans="1:24">
       <c r="A67" s="3">
         <v>65</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="C67" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D67" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E67" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" s="3" customFormat="1" spans="1:23">
+      <c r="E67" s="8">
+        <f t="shared" ref="E67:E92" si="4">SUM(F67:AJ67)</f>
+        <v>15000</v>
+      </c>
+      <c r="I67" s="3">
+        <v>2000</v>
+      </c>
+      <c r="K67" s="3">
+        <v>1000</v>
+      </c>
+      <c r="N67" s="3">
+        <v>2000</v>
+      </c>
+      <c r="Q67" s="3">
+        <v>1000</v>
+      </c>
+      <c r="S67" s="9">
+        <v>3000</v>
+      </c>
+      <c r="U67" s="3">
+        <v>2000</v>
+      </c>
+      <c r="X67" s="9">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="68" s="3" customFormat="1" spans="1:5">
       <c r="A68" s="3">
         <v>66</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D68" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E68" s="2">
-        <v>4000</v>
-      </c>
-      <c r="W68" s="3">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="69" s="3" customFormat="1" spans="1:16">
+      <c r="E68" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" s="3" customFormat="1" spans="1:23">
       <c r="A69" s="3">
         <v>67</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D69" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E69" s="2">
-        <v>2000</v>
-      </c>
-      <c r="P69" s="8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="70" s="3" customFormat="1" spans="1:5">
+      <c r="E69" s="8">
+        <f t="shared" si="4"/>
+        <v>4000</v>
+      </c>
+      <c r="W69" s="3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="70" s="3" customFormat="1" spans="1:16">
       <c r="A70" s="3">
         <v>68</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D70" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E70" s="2">
-        <v>0</v>
+      <c r="E70" s="8">
+        <f t="shared" si="4"/>
+        <v>2000</v>
+      </c>
+      <c r="P70" s="9">
+        <v>2000</v>
       </c>
     </row>
     <row r="71" s="3" customFormat="1" spans="1:5">
       <c r="A71" s="3">
         <v>69</v>
       </c>
-      <c r="D71" s="7" t="s">
+      <c r="D71" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E71" s="2">
+      <c r="E71" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3568,10 +3674,11 @@
       <c r="A72" s="3">
         <v>70</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D72" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E72" s="2">
+      <c r="E72" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3579,10 +3686,11 @@
       <c r="A73" s="3">
         <v>71</v>
       </c>
-      <c r="D73" s="7" t="s">
+      <c r="D73" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E73" s="2">
+      <c r="E73" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3590,10 +3698,11 @@
       <c r="A74" s="3">
         <v>72</v>
       </c>
-      <c r="D74" s="7" t="s">
+      <c r="D74" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E74" s="2">
+      <c r="E74" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3601,10 +3710,11 @@
       <c r="A75" s="3">
         <v>73</v>
       </c>
-      <c r="D75" s="7" t="s">
+      <c r="D75" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E75" s="2">
+      <c r="E75" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3612,10 +3722,11 @@
       <c r="A76" s="3">
         <v>74</v>
       </c>
-      <c r="D76" s="7" t="s">
+      <c r="D76" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E76" s="2">
+      <c r="E76" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3623,10 +3734,11 @@
       <c r="A77" s="3">
         <v>75</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D77" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E77" s="2">
+      <c r="E77" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3634,12 +3746,11 @@
       <c r="A78" s="3">
         <v>76</v>
       </c>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="7" t="s">
+      <c r="D78" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E78" s="2">
+      <c r="E78" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3647,10 +3758,11 @@
       <c r="A79" s="3">
         <v>77</v>
       </c>
-      <c r="D79" s="7" t="s">
+      <c r="D79" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E79" s="2">
+      <c r="E79" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3658,10 +3770,11 @@
       <c r="A80" s="3">
         <v>78</v>
       </c>
-      <c r="D80" s="7" t="s">
+      <c r="D80" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E80" s="2">
+      <c r="E80" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3669,10 +3782,11 @@
       <c r="A81" s="3">
         <v>79</v>
       </c>
-      <c r="D81" s="7" t="s">
+      <c r="D81" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E81" s="2">
+      <c r="E81" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3680,12 +3794,11 @@
       <c r="A82" s="3">
         <v>80</v>
       </c>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="7" t="s">
+      <c r="D82" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E82" s="2">
+      <c r="E82" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3693,10 +3806,11 @@
       <c r="A83" s="3">
         <v>81</v>
       </c>
-      <c r="D83" s="7" t="s">
+      <c r="D83" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E83" s="2">
+      <c r="E83" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3704,12 +3818,11 @@
       <c r="A84" s="3">
         <v>82</v>
       </c>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="7" t="s">
+      <c r="D84" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E84" s="2">
+      <c r="E84" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3717,10 +3830,11 @@
       <c r="A85" s="3">
         <v>83</v>
       </c>
-      <c r="D85" s="7" t="s">
+      <c r="D85" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E85" s="2">
+      <c r="E85" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3728,10 +3842,11 @@
       <c r="A86" s="3">
         <v>84</v>
       </c>
-      <c r="D86" s="7" t="s">
+      <c r="D86" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E86" s="2">
+      <c r="E86" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3739,10 +3854,11 @@
       <c r="A87" s="3">
         <v>85</v>
       </c>
-      <c r="D87" s="7" t="s">
+      <c r="D87" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E87" s="2">
+      <c r="E87" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3750,10 +3866,11 @@
       <c r="A88" s="3">
         <v>86</v>
       </c>
-      <c r="D88" s="7" t="s">
+      <c r="D88" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E88" s="2">
+      <c r="E88" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3761,10 +3878,11 @@
       <c r="A89" s="3">
         <v>87</v>
       </c>
-      <c r="D89" s="7" t="s">
+      <c r="D89" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E89" s="2">
+      <c r="E89" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3772,10 +3890,11 @@
       <c r="A90" s="3">
         <v>88</v>
       </c>
-      <c r="D90" s="7" t="s">
+      <c r="D90" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E90" s="2">
+      <c r="E90" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3783,10 +3902,11 @@
       <c r="A91" s="3">
         <v>89</v>
       </c>
-      <c r="D91" s="7" t="s">
+      <c r="D91" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E91" s="2">
+      <c r="E91" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3794,10 +3914,11 @@
       <c r="A92" s="3">
         <v>90</v>
       </c>
-      <c r="D92" s="7" t="s">
+      <c r="D92" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E92" s="2">
+      <c r="E92" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data updated till 22Dec 11AM
</commit_message>
<xml_diff>
--- a/Daily Collection/December-2020-Collection.xlsx
+++ b/Daily Collection/December-2020-Collection.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7830"/>
+    <workbookView windowWidth="20490" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="December 2020" sheetId="1" r:id="rId1"/>
@@ -160,6 +160,29 @@
         </r>
       </text>
     </comment>
+    <comment ref="Z54" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>Vijay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+1500-Cash
+500-Digital</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="K63" authorId="0">
       <text>
         <r>
@@ -531,11 +554,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -554,8 +577,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -563,7 +647,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -578,92 +662,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -678,7 +678,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -691,8 +706,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -742,7 +765,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -754,7 +885,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -766,157 +939,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -945,6 +968,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -956,21 +1003,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -992,35 +1024,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1033,18 +1041,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1056,130 +1079,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1199,7 +1222,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1223,12 +1246,12 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Currency" xfId="5" builtinId="4"/>
     <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
     <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
@@ -1544,11 +1567,11 @@
   <dimension ref="A1:AJ92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="Q45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="T46" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Y61" sqref="Y61"/>
+      <selection pane="bottomRight" activeCell="Z63" sqref="Z63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1677,7 +1700,7 @@
       </c>
       <c r="E2" s="7">
         <f>SUM(F2:AJ2)</f>
-        <v>723900</v>
+        <v>756900</v>
       </c>
       <c r="F2" s="2">
         <f>SUM(F3:F92)</f>
@@ -1761,7 +1784,7 @@
       </c>
       <c r="Z2" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>33000</v>
       </c>
       <c r="AA2" s="2">
         <f t="shared" si="1"/>
@@ -2002,7 +2025,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" s="3" customFormat="1" spans="1:22">
+    <row r="10" s="3" customFormat="1" spans="1:26">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2014,7 +2037,7 @@
       </c>
       <c r="E10" s="8">
         <f t="shared" si="2"/>
-        <v>25000</v>
+        <v>30000</v>
       </c>
       <c r="H10" s="3">
         <v>2000</v>
@@ -2032,6 +2055,9 @@
         <v>5000</v>
       </c>
       <c r="V10" s="3">
+        <v>5000</v>
+      </c>
+      <c r="Z10" s="3">
         <v>5000</v>
       </c>
     </row>
@@ -2119,7 +2145,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="14" s="3" customFormat="1" spans="1:24">
+    <row r="14" s="3" customFormat="1" spans="1:26">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2131,7 +2157,7 @@
       </c>
       <c r="E14" s="8">
         <f t="shared" si="2"/>
-        <v>30000</v>
+        <v>32500</v>
       </c>
       <c r="H14" s="3">
         <v>2000</v>
@@ -2168,6 +2194,9 @@
       </c>
       <c r="X14" s="3">
         <v>1000</v>
+      </c>
+      <c r="Z14" s="3">
+        <v>2500</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" spans="1:22">
@@ -2278,7 +2307,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="19" s="3" customFormat="1" spans="1:23">
+    <row r="19" s="3" customFormat="1" spans="1:26">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -2290,7 +2319,7 @@
       </c>
       <c r="E19" s="8">
         <f t="shared" si="2"/>
-        <v>7500</v>
+        <v>9000</v>
       </c>
       <c r="I19" s="3">
         <v>1000</v>
@@ -2305,6 +2334,9 @@
         <v>1000</v>
       </c>
       <c r="W19" s="3">
+        <v>1500</v>
+      </c>
+      <c r="Z19" s="3">
         <v>1500</v>
       </c>
     </row>
@@ -2413,7 +2445,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="24" s="3" customFormat="1" spans="1:23">
+    <row r="24" s="3" customFormat="1" spans="1:26">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -2425,7 +2457,7 @@
       </c>
       <c r="E24" s="8">
         <f t="shared" si="2"/>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="N24" s="3">
         <v>6000</v>
@@ -2441,6 +2473,9 @@
       </c>
       <c r="W24" s="3">
         <v>500</v>
+      </c>
+      <c r="Z24" s="3">
+        <v>3000</v>
       </c>
     </row>
     <row r="25" s="3" customFormat="1" spans="1:24">
@@ -2590,7 +2625,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="30" s="3" customFormat="1" spans="1:24">
+    <row r="30" s="3" customFormat="1" spans="1:26">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -2602,7 +2637,7 @@
       </c>
       <c r="E30" s="8">
         <f t="shared" si="2"/>
-        <v>9500</v>
+        <v>10000</v>
       </c>
       <c r="I30" s="3">
         <v>1000</v>
@@ -2634,8 +2669,11 @@
       <c r="X30" s="3">
         <v>500</v>
       </c>
-    </row>
-    <row r="31" s="3" customFormat="1" spans="1:23">
+      <c r="Z30" s="3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" s="3" customFormat="1" spans="1:26">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -2647,7 +2685,7 @@
       </c>
       <c r="E31" s="8">
         <f t="shared" si="2"/>
-        <v>8000</v>
+        <v>9000</v>
       </c>
       <c r="H31" s="3">
         <v>2000</v>
@@ -2660,6 +2698,9 @@
       </c>
       <c r="W31" s="3">
         <v>2000</v>
+      </c>
+      <c r="Z31" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="32" s="3" customFormat="1" spans="1:22">
@@ -2797,7 +2838,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="37" s="3" customFormat="1" spans="1:20">
+    <row r="37" s="3" customFormat="1" spans="1:26">
       <c r="A37" s="3">
         <v>35</v>
       </c>
@@ -2809,12 +2850,15 @@
       </c>
       <c r="E37" s="8">
         <f t="shared" si="3"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="J37" s="3">
         <v>2000</v>
       </c>
       <c r="T37" s="9">
+        <v>2000</v>
+      </c>
+      <c r="Z37" s="9">
         <v>2000</v>
       </c>
     </row>
@@ -2872,7 +2916,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="40" s="3" customFormat="1" spans="1:23">
+    <row r="40" s="3" customFormat="1" spans="1:26">
       <c r="A40" s="3">
         <v>38</v>
       </c>
@@ -2884,7 +2928,7 @@
       </c>
       <c r="E40" s="8">
         <f t="shared" si="3"/>
-        <v>21000</v>
+        <v>24000</v>
       </c>
       <c r="H40" s="3">
         <v>2000</v>
@@ -2902,6 +2946,9 @@
         <v>3000</v>
       </c>
       <c r="W40" s="3">
+        <v>3000</v>
+      </c>
+      <c r="Z40" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -3226,7 +3273,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="53" s="3" customFormat="1" spans="1:22">
+    <row r="53" s="3" customFormat="1" spans="1:26">
       <c r="A53" s="3">
         <v>51</v>
       </c>
@@ -3238,7 +3285,7 @@
       </c>
       <c r="E53" s="8">
         <f t="shared" si="3"/>
-        <v>18000</v>
+        <v>22000</v>
       </c>
       <c r="N53" s="3">
         <v>8000</v>
@@ -3249,8 +3296,11 @@
       <c r="V53" s="3">
         <v>5000</v>
       </c>
-    </row>
-    <row r="54" s="3" customFormat="1" spans="1:20">
+      <c r="Z53" s="3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="54" s="3" customFormat="1" spans="1:26">
       <c r="A54" s="3">
         <v>52</v>
       </c>
@@ -3262,7 +3312,7 @@
       </c>
       <c r="E54" s="8">
         <f t="shared" si="3"/>
-        <v>3500</v>
+        <v>5500</v>
       </c>
       <c r="L54" s="3">
         <v>1500</v>
@@ -3272,6 +3322,9 @@
       </c>
       <c r="T54" s="3">
         <v>1500</v>
+      </c>
+      <c r="Z54" s="9">
+        <v>2000</v>
       </c>
     </row>
     <row r="55" s="3" customFormat="1" spans="1:15">
@@ -3430,7 +3483,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="62" s="3" customFormat="1" spans="1:25">
+    <row r="62" s="3" customFormat="1" spans="1:26">
       <c r="A62" s="3">
         <v>60</v>
       </c>
@@ -3442,7 +3495,7 @@
       </c>
       <c r="E62" s="8">
         <f t="shared" si="3"/>
-        <v>37000</v>
+        <v>42000</v>
       </c>
       <c r="J62" s="3">
         <v>2000</v>
@@ -3460,6 +3513,9 @@
         <v>5000</v>
       </c>
       <c r="Y62" s="3">
+        <v>5000</v>
+      </c>
+      <c r="Z62" s="3">
         <v>5000</v>
       </c>
     </row>
@@ -3493,7 +3549,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="64" s="3" customFormat="1" spans="1:24">
+    <row r="64" s="3" customFormat="1" spans="1:26">
       <c r="A64" s="3">
         <v>62</v>
       </c>
@@ -3505,10 +3561,13 @@
       </c>
       <c r="E64" s="8">
         <f t="shared" si="3"/>
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="X64" s="3">
         <v>1500</v>
+      </c>
+      <c r="Z64" s="3">
+        <v>500</v>
       </c>
     </row>
     <row r="65" s="3" customFormat="1" spans="1:24">
@@ -3547,7 +3606,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="66" s="3" customFormat="1" spans="1:24">
+    <row r="66" s="3" customFormat="1" spans="1:26">
       <c r="A66" s="3">
         <v>64</v>
       </c>
@@ -3559,7 +3618,7 @@
       </c>
       <c r="E66" s="8">
         <f t="shared" si="3"/>
-        <v>18000</v>
+        <v>21000</v>
       </c>
       <c r="J66" s="9">
         <v>3000</v>
@@ -3577,6 +3636,9 @@
         <v>3000</v>
       </c>
       <c r="X66" s="3">
+        <v>3000</v>
+      </c>
+      <c r="Z66" s="3">
         <v>3000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data updated till 23Dec 8AM
</commit_message>
<xml_diff>
--- a/Daily Collection/December-2020-Collection.xlsx
+++ b/Daily Collection/December-2020-Collection.xlsx
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="119">
   <si>
     <t>S.No.</t>
   </si>
@@ -381,6 +381,9 @@
     <t>PAWAN PAY PHONE(660297502)</t>
   </si>
   <si>
+    <t>Ranjit Kr.</t>
+  </si>
+  <si>
     <t>KUMAR INTERNET(660322625)</t>
   </si>
   <si>
@@ -393,6 +396,9 @@
     <t>PATEL TELECOM(661644686)</t>
   </si>
   <si>
+    <t>Chandan</t>
+  </si>
+  <si>
     <t>KRISH RAJ MOBILE &amp; ELECTRONIC(661032970)</t>
   </si>
   <si>
@@ -480,6 +486,12 @@
     <t>SHRI SAI ELECTRONICS(661673670)</t>
   </si>
   <si>
+    <t>Indrijeet</t>
+  </si>
+  <si>
+    <t>Dhewai</t>
+  </si>
+  <si>
     <t>maa phone ghar(662077151)</t>
   </si>
   <si>
@@ -510,6 +522,9 @@
     <t>sugam phone bathe(661711006)</t>
   </si>
   <si>
+    <t>Arwal</t>
+  </si>
+  <si>
     <t>RAJ PHONE HIRDYACHAK(661712682)</t>
   </si>
   <si>
@@ -519,6 +534,9 @@
     <t>MUSKAN COMMUNICATION(662077126)</t>
   </si>
   <si>
+    <t>Sabbir Ahmad</t>
+  </si>
+  <si>
     <t>KRISHNA KIRANA STORE(661613674)</t>
   </si>
   <si>
@@ -547,6 +565,9 @@
   </si>
   <si>
     <t>6201704055(662077143)</t>
+  </si>
+  <si>
+    <t>Manish mobile center(662157439)</t>
   </si>
 </sst>
 </file>
@@ -554,11 +575,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -577,9 +598,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -592,31 +635,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -632,22 +653,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -662,15 +667,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -678,7 +676,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -691,9 +689,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -707,15 +704,39 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -765,13 +786,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -789,7 +822,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -801,37 +834,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -849,25 +864,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -879,7 +876,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -891,7 +900,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -903,49 +960,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -959,11 +980,74 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -985,45 +1069,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1032,39 +1077,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1079,88 +1100,94 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1169,40 +1196,34 @@
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1222,7 +1243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1564,14 +1585,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AJ92"/>
+  <dimension ref="A1:AJ93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="T46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="U81" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Z63" sqref="Z63"/>
+      <selection pane="bottomRight" activeCell="A93" sqref="A93:D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1700,7 +1721,7 @@
       </c>
       <c r="E2" s="7">
         <f>SUM(F2:AJ2)</f>
-        <v>756900</v>
+        <v>796300</v>
       </c>
       <c r="F2" s="2">
         <f>SUM(F3:F92)</f>
@@ -1788,7 +1809,7 @@
       </c>
       <c r="AA2" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>39400</v>
       </c>
       <c r="AB2" s="2">
         <f t="shared" si="1"/>
@@ -1935,7 +1956,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" spans="1:24">
+    <row r="7" s="3" customFormat="1" spans="1:27">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1947,7 +1968,7 @@
       </c>
       <c r="E7" s="8">
         <f t="shared" si="2"/>
-        <v>29000</v>
+        <v>35000</v>
       </c>
       <c r="H7" s="3">
         <v>2000</v>
@@ -1972,6 +1993,9 @@
       </c>
       <c r="X7" s="3">
         <v>5000</v>
+      </c>
+      <c r="AA7" s="9">
+        <v>6000</v>
       </c>
     </row>
     <row r="8" s="3" customFormat="1" spans="1:23">
@@ -2145,7 +2169,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="14" s="3" customFormat="1" spans="1:26">
+    <row r="14" s="3" customFormat="1" spans="1:27">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2157,7 +2181,7 @@
       </c>
       <c r="E14" s="8">
         <f t="shared" si="2"/>
-        <v>32500</v>
+        <v>34000</v>
       </c>
       <c r="H14" s="3">
         <v>2000</v>
@@ -2197,6 +2221,9 @@
       </c>
       <c r="Z14" s="3">
         <v>2500</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>1500</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" spans="1:22">
@@ -2478,7 +2505,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="25" s="3" customFormat="1" spans="1:24">
+    <row r="25" s="3" customFormat="1" spans="1:27">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -2490,7 +2517,7 @@
       </c>
       <c r="E25" s="8">
         <f t="shared" si="2"/>
-        <v>8500</v>
+        <v>9500</v>
       </c>
       <c r="M25" s="3">
         <v>3000</v>
@@ -2505,6 +2532,9 @@
         <v>1000</v>
       </c>
       <c r="X25" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AA25" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -2592,7 +2622,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="29" s="3" customFormat="1" spans="1:23">
+    <row r="29" s="3" customFormat="1" spans="1:27">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -2604,7 +2634,7 @@
       </c>
       <c r="E29" s="8">
         <f t="shared" si="2"/>
-        <v>39000</v>
+        <v>44000</v>
       </c>
       <c r="I29" s="3">
         <v>2000</v>
@@ -2622,6 +2652,9 @@
         <v>10000</v>
       </c>
       <c r="W29" s="3">
+        <v>5000</v>
+      </c>
+      <c r="AA29" s="9">
         <v>5000</v>
       </c>
     </row>
@@ -2808,7 +2841,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="36" s="3" customFormat="1" spans="1:23">
+    <row r="36" s="3" customFormat="1" spans="1:27">
       <c r="A36" s="3">
         <v>34</v>
       </c>
@@ -2820,7 +2853,7 @@
       </c>
       <c r="E36" s="8">
         <f t="shared" si="3"/>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="H36" s="9">
         <v>3000</v>
@@ -2835,6 +2868,9 @@
         <v>3000</v>
       </c>
       <c r="W36" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AA36" s="9">
         <v>3000</v>
       </c>
     </row>
@@ -2889,7 +2925,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="39" s="3" customFormat="1" spans="1:19">
+    <row r="39" s="3" customFormat="1" spans="1:27">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -2901,7 +2937,7 @@
       </c>
       <c r="E39" s="8">
         <f t="shared" si="3"/>
-        <v>7000</v>
+        <v>8000</v>
       </c>
       <c r="H39" s="3">
         <v>2000</v>
@@ -2915,8 +2951,11 @@
       <c r="S39" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="40" s="3" customFormat="1" spans="1:26">
+      <c r="AA39" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="40" s="3" customFormat="1" spans="1:27">
       <c r="A40" s="3">
         <v>38</v>
       </c>
@@ -2928,7 +2967,7 @@
       </c>
       <c r="E40" s="8">
         <f t="shared" si="3"/>
-        <v>24000</v>
+        <v>26000</v>
       </c>
       <c r="H40" s="3">
         <v>2000</v>
@@ -2950,6 +2989,9 @@
       </c>
       <c r="Z40" s="3">
         <v>3000</v>
+      </c>
+      <c r="AA40" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="41" s="3" customFormat="1" spans="1:16">
@@ -3018,7 +3060,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="44" s="3" customFormat="1" spans="1:24">
+    <row r="44" s="3" customFormat="1" spans="1:27">
       <c r="A44" s="3">
         <v>42</v>
       </c>
@@ -3030,7 +3072,7 @@
       </c>
       <c r="E44" s="8">
         <f t="shared" si="3"/>
-        <v>14000</v>
+        <v>17000</v>
       </c>
       <c r="I44" s="3">
         <v>5000</v>
@@ -3042,6 +3084,9 @@
         <v>3000</v>
       </c>
       <c r="X44" s="9">
+        <v>3000</v>
+      </c>
+      <c r="AA44" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -3078,24 +3123,30 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="46" s="3" customFormat="1" spans="1:19">
+    <row r="46" s="3" customFormat="1" spans="1:27">
       <c r="A46" s="3">
         <v>44</v>
       </c>
+      <c r="B46" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C46" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E46" s="8">
         <f t="shared" si="3"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="I46" s="9">
         <v>2000</v>
       </c>
       <c r="S46" s="9">
+        <v>2000</v>
+      </c>
+      <c r="AA46" s="9">
         <v>2000</v>
       </c>
     </row>
@@ -3107,7 +3158,7 @@
         <v>53</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E47" s="8">
         <f t="shared" si="3"/>
@@ -3131,13 +3182,13 @@
         <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E48" s="8">
         <f t="shared" si="3"/>
@@ -3162,19 +3213,22 @@
         <v>500</v>
       </c>
     </row>
-    <row r="49" s="3" customFormat="1" spans="1:24">
+    <row r="49" s="3" customFormat="1" spans="1:27">
       <c r="A49" s="3">
         <v>47</v>
       </c>
+      <c r="B49" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="C49" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E49" s="8">
         <f t="shared" si="3"/>
-        <v>7000</v>
+        <v>9000</v>
       </c>
       <c r="I49" s="3">
         <v>1000</v>
@@ -3186,6 +3240,9 @@
         <v>2000</v>
       </c>
       <c r="X49" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AA49" s="9">
         <v>2000</v>
       </c>
     </row>
@@ -3197,7 +3254,7 @@
         <v>53</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E50" s="8">
         <f t="shared" si="3"/>
@@ -3218,13 +3275,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E51" s="8">
         <f t="shared" si="3"/>
@@ -3254,10 +3311,10 @@
         <v>50</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E52" s="8">
         <f t="shared" si="3"/>
@@ -3278,10 +3335,10 @@
         <v>51</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E53" s="8">
         <f t="shared" si="3"/>
@@ -3305,10 +3362,10 @@
         <v>52</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E54" s="8">
         <f t="shared" si="3"/>
@@ -3332,10 +3389,10 @@
         <v>53</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E55" s="8">
         <f t="shared" si="3"/>
@@ -3350,13 +3407,13 @@
         <v>54</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E56" s="8">
         <f t="shared" si="3"/>
@@ -3380,10 +3437,10 @@
         <v>55</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E57" s="8">
         <f t="shared" si="3"/>
@@ -3393,24 +3450,27 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="58" s="3" customFormat="1" spans="1:22">
+    <row r="58" s="3" customFormat="1" spans="1:27">
       <c r="A58" s="3">
         <v>56</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E58" s="8">
         <f t="shared" si="3"/>
-        <v>7000</v>
+        <v>9000</v>
       </c>
       <c r="P58" s="3">
         <v>5000</v>
       </c>
       <c r="V58" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AA58" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -3419,10 +3479,10 @@
         <v>57</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E59" s="8">
         <f t="shared" si="3"/>
@@ -3443,10 +3503,10 @@
         <v>58</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E60" s="8">
         <f t="shared" si="3"/>
@@ -3467,10 +3527,10 @@
         <v>59</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E61" s="8">
         <f t="shared" si="3"/>
@@ -3488,10 +3548,10 @@
         <v>60</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E62" s="8">
         <f t="shared" si="3"/>
@@ -3519,19 +3579,19 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="63" s="3" customFormat="1" spans="1:23">
+    <row r="63" s="3" customFormat="1" spans="1:27">
       <c r="A63" s="3">
         <v>61</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E63" s="8">
         <f t="shared" si="3"/>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="K63" s="9">
         <v>4000</v>
@@ -3546,6 +3606,9 @@
         <v>3000</v>
       </c>
       <c r="W63" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AA63" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -3554,10 +3617,10 @@
         <v>62</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E64" s="8">
         <f t="shared" si="3"/>
@@ -3570,19 +3633,19 @@
         <v>500</v>
       </c>
     </row>
-    <row r="65" s="3" customFormat="1" spans="1:24">
+    <row r="65" s="3" customFormat="1" spans="1:27">
       <c r="A65" s="3">
         <v>63</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E65" s="8">
         <f t="shared" si="3"/>
-        <v>10900</v>
+        <v>12800</v>
       </c>
       <c r="I65" s="9">
         <v>1000</v>
@@ -3604,6 +3667,9 @@
       </c>
       <c r="X65" s="3">
         <v>600</v>
+      </c>
+      <c r="AA65" s="3">
+        <v>1900</v>
       </c>
     </row>
     <row r="66" s="3" customFormat="1" spans="1:26">
@@ -3611,10 +3677,10 @@
         <v>64</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E66" s="8">
         <f t="shared" si="3"/>
@@ -3647,10 +3713,10 @@
         <v>65</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E67" s="8">
         <f t="shared" ref="E67:E92" si="4">SUM(F67:AJ67)</f>
@@ -3683,7 +3749,7 @@
         <v>66</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E68" s="8">
         <f t="shared" si="4"/>
@@ -3695,7 +3761,7 @@
         <v>67</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E69" s="8">
         <f t="shared" si="4"/>
@@ -3705,18 +3771,27 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="70" s="3" customFormat="1" spans="1:16">
+    <row r="70" s="3" customFormat="1" spans="1:27">
       <c r="A70" s="3">
         <v>68</v>
       </c>
+      <c r="B70" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="D70" s="4" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E70" s="8">
         <f t="shared" si="4"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="P70" s="9">
+        <v>2000</v>
+      </c>
+      <c r="AA70" s="9">
         <v>2000</v>
       </c>
     </row>
@@ -3725,7 +3800,7 @@
         <v>69</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E71" s="8">
         <f t="shared" si="4"/>
@@ -3737,7 +3812,7 @@
         <v>70</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E72" s="8">
         <f t="shared" si="4"/>
@@ -3749,7 +3824,7 @@
         <v>71</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E73" s="8">
         <f t="shared" si="4"/>
@@ -3761,7 +3836,7 @@
         <v>72</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E74" s="8">
         <f t="shared" si="4"/>
@@ -3773,7 +3848,7 @@
         <v>73</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E75" s="8">
         <f t="shared" si="4"/>
@@ -3785,7 +3860,7 @@
         <v>74</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E76" s="8">
         <f t="shared" si="4"/>
@@ -3797,7 +3872,7 @@
         <v>75</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E77" s="8">
         <f t="shared" si="4"/>
@@ -3809,7 +3884,7 @@
         <v>76</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E78" s="8">
         <f t="shared" si="4"/>
@@ -3821,23 +3896,29 @@
         <v>77</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E79" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="80" s="3" customFormat="1" spans="1:5">
+    <row r="80" s="3" customFormat="1" spans="1:27">
       <c r="A80" s="3">
         <v>78</v>
       </c>
+      <c r="C80" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="D80" s="4" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E80" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="AA80" s="9">
+        <v>2000</v>
       </c>
     </row>
     <row r="81" s="3" customFormat="1" spans="1:5">
@@ -3845,7 +3926,7 @@
         <v>79</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E81" s="8">
         <f t="shared" si="4"/>
@@ -3857,23 +3938,32 @@
         <v>80</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E82" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="83" s="3" customFormat="1" spans="1:5">
+    <row r="83" s="3" customFormat="1" spans="1:27">
       <c r="A83" s="3">
         <v>81</v>
       </c>
+      <c r="B83" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="D83" s="4" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E83" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="AA83" s="9">
+        <v>2000</v>
       </c>
     </row>
     <row r="84" s="3" customFormat="1" spans="1:5">
@@ -3881,7 +3971,7 @@
         <v>82</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="E84" s="8">
         <f t="shared" si="4"/>
@@ -3893,7 +3983,7 @@
         <v>83</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E85" s="8">
         <f t="shared" si="4"/>
@@ -3905,7 +3995,7 @@
         <v>84</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="E86" s="8">
         <f t="shared" si="4"/>
@@ -3917,7 +4007,7 @@
         <v>85</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E87" s="8">
         <f t="shared" si="4"/>
@@ -3929,7 +4019,7 @@
         <v>86</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="E88" s="8">
         <f t="shared" si="4"/>
@@ -3941,7 +4031,7 @@
         <v>87</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="E89" s="8">
         <f t="shared" si="4"/>
@@ -3953,7 +4043,7 @@
         <v>88</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="E90" s="8">
         <f t="shared" si="4"/>
@@ -3965,7 +4055,7 @@
         <v>89</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E91" s="8">
         <f t="shared" si="4"/>
@@ -3977,10 +4067,22 @@
         <v>90</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E92" s="8">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="3">
+        <v>91</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E93" s="8">
+        <f>SUM(F93:AJ93)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data updated till 26Dec 7AM
</commit_message>
<xml_diff>
--- a/Daily Collection/December-2020-Collection.xlsx
+++ b/Daily Collection/December-2020-Collection.xlsx
@@ -160,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z54" authorId="0">
+    <comment ref="Z55" authorId="0">
       <text>
         <r>
           <rPr>
@@ -183,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K63" authorId="0">
+    <comment ref="K64" authorId="0">
       <text>
         <r>
           <rPr>
@@ -206,12 +206,35 @@
         </r>
       </text>
     </comment>
+    <comment ref="AD66" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>Vijay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+2000-Digital
+200-Cash</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="120">
   <si>
     <t>S.No.</t>
   </si>
@@ -411,6 +434,9 @@
     <t>DIVYANKA MOBILE CENTER(660315660)</t>
   </si>
   <si>
+    <t>Neha Phonex(660614432)</t>
+  </si>
+  <si>
     <t>PARASI</t>
   </si>
   <si>
@@ -423,6 +449,9 @@
     <t>KALER ENTERPRISES(661674410)</t>
   </si>
   <si>
+    <t>Amresh Kr.</t>
+  </si>
+  <si>
     <t>BADRABAD</t>
   </si>
   <si>
@@ -538,9 +567,6 @@
   </si>
   <si>
     <t>KRISHNA KIRANA STORE(661613674)</t>
-  </si>
-  <si>
-    <t>Neha Phonex(660614432)</t>
   </si>
   <si>
     <t>SURAJ KIRANA STORE(661735618)</t>
@@ -575,11 +601,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -598,6 +624,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -608,36 +672,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -660,14 +694,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -676,38 +702,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -726,6 +723,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -736,7 +747,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -786,7 +812,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -798,7 +848,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -810,13 +890,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -828,103 +944,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -942,13 +968,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -977,6 +1003,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1010,26 +1060,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1039,15 +1074,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1082,15 +1108,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1100,130 +1126,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1243,7 +1269,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1588,11 +1614,11 @@
   <dimension ref="A1:AJ93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="U81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="X77" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A93" sqref="A93:D93"/>
+      <selection pane="bottomRight" activeCell="A51" sqref="A51:A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1721,7 +1747,7 @@
       </c>
       <c r="E2" s="7">
         <f>SUM(F2:AJ2)</f>
-        <v>796300</v>
+        <v>932000</v>
       </c>
       <c r="F2" s="2">
         <f>SUM(F3:F92)</f>
@@ -1813,15 +1839,15 @@
       </c>
       <c r="AB2" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>41500</v>
       </c>
       <c r="AC2" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>54500</v>
       </c>
       <c r="AD2" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>39700</v>
       </c>
       <c r="AE2" s="2">
         <f t="shared" si="1"/>
@@ -1848,7 +1874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" s="3" customFormat="1" spans="1:21">
+    <row r="3" s="3" customFormat="1" spans="1:28">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1860,13 +1886,16 @@
       </c>
       <c r="E3" s="8">
         <f t="shared" ref="E3:E34" si="2">SUM(F3:AJ3)</f>
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="U3" s="9">
         <v>3000</v>
       </c>
-    </row>
-    <row r="4" s="3" customFormat="1" spans="1:11">
+      <c r="AB3" s="9">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="4" s="3" customFormat="1" spans="1:28">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1878,13 +1907,16 @@
       </c>
       <c r="E4" s="8">
         <f t="shared" si="2"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="K4" s="9">
         <v>2000</v>
       </c>
-    </row>
-    <row r="5" s="3" customFormat="1" spans="1:24">
+      <c r="AB4" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" s="3" customFormat="1" spans="1:29">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1896,7 +1928,7 @@
       </c>
       <c r="E5" s="8">
         <f t="shared" si="2"/>
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="H5" s="3">
         <v>1000</v>
@@ -1919,8 +1951,11 @@
       <c r="X5" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="6" s="3" customFormat="1" spans="1:24">
+      <c r="AC5" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" s="3" customFormat="1" spans="1:28">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1932,7 +1967,7 @@
       </c>
       <c r="E6" s="8">
         <f t="shared" si="2"/>
-        <v>19500</v>
+        <v>21500</v>
       </c>
       <c r="H6" s="9">
         <v>3000</v>
@@ -1955,8 +1990,11 @@
       <c r="X6" s="9">
         <v>3000</v>
       </c>
-    </row>
-    <row r="7" s="3" customFormat="1" spans="1:27">
+      <c r="AB6" s="9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" s="3" customFormat="1" spans="1:29">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1968,7 +2006,7 @@
       </c>
       <c r="E7" s="8">
         <f t="shared" si="2"/>
-        <v>35000</v>
+        <v>39000</v>
       </c>
       <c r="H7" s="3">
         <v>2000</v>
@@ -1996,6 +2034,9 @@
       </c>
       <c r="AA7" s="9">
         <v>6000</v>
+      </c>
+      <c r="AC7" s="9">
+        <v>4000</v>
       </c>
     </row>
     <row r="8" s="3" customFormat="1" spans="1:23">
@@ -2049,7 +2090,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" s="3" customFormat="1" spans="1:26">
+    <row r="10" s="3" customFormat="1" spans="1:29">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2061,7 +2102,7 @@
       </c>
       <c r="E10" s="8">
         <f t="shared" si="2"/>
-        <v>30000</v>
+        <v>35000</v>
       </c>
       <c r="H10" s="3">
         <v>2000</v>
@@ -2082,6 +2123,9 @@
         <v>5000</v>
       </c>
       <c r="Z10" s="3">
+        <v>5000</v>
+      </c>
+      <c r="AC10" s="3">
         <v>5000</v>
       </c>
     </row>
@@ -2112,7 +2156,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="12" s="3" customFormat="1" spans="1:22">
+    <row r="12" s="3" customFormat="1" spans="1:28">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -2124,7 +2168,7 @@
       </c>
       <c r="E12" s="8">
         <f t="shared" si="2"/>
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="L12" s="3">
         <v>1000</v>
@@ -2138,8 +2182,11 @@
       <c r="V12" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="13" s="3" customFormat="1" spans="1:23">
+      <c r="AB12" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" s="3" customFormat="1" spans="1:30">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -2151,7 +2198,7 @@
       </c>
       <c r="E13" s="8">
         <f t="shared" si="2"/>
-        <v>23000</v>
+        <v>28000</v>
       </c>
       <c r="H13" s="3">
         <v>2000</v>
@@ -2168,8 +2215,11 @@
       <c r="W13" s="3">
         <v>5000</v>
       </c>
-    </row>
-    <row r="14" s="3" customFormat="1" spans="1:27">
+      <c r="AD13" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="14" s="3" customFormat="1" spans="1:30">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2181,7 +2231,7 @@
       </c>
       <c r="E14" s="8">
         <f t="shared" si="2"/>
-        <v>34000</v>
+        <v>38500</v>
       </c>
       <c r="H14" s="3">
         <v>2000</v>
@@ -2225,8 +2275,17 @@
       <c r="AA14" s="3">
         <v>1500</v>
       </c>
-    </row>
-    <row r="15" s="3" customFormat="1" spans="1:22">
+      <c r="AB14" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>1500</v>
+      </c>
+      <c r="AD14" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="15" s="3" customFormat="1" spans="1:28">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -2241,7 +2300,7 @@
       </c>
       <c r="E15" s="8">
         <f t="shared" si="2"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="S15" s="3">
         <v>2000</v>
@@ -2249,8 +2308,11 @@
       <c r="V15" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="16" s="3" customFormat="1" spans="1:23">
+      <c r="AB15" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" s="3" customFormat="1" spans="1:29">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -2262,7 +2324,7 @@
       </c>
       <c r="E16" s="8">
         <f t="shared" si="2"/>
-        <v>12000</v>
+        <v>15000</v>
       </c>
       <c r="M16" s="3">
         <v>2000</v>
@@ -2279,8 +2341,11 @@
       <c r="W16" s="3">
         <v>3000</v>
       </c>
-    </row>
-    <row r="17" s="3" customFormat="1" spans="1:19">
+      <c r="AC16" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="17" s="3" customFormat="1" spans="1:29">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -2292,7 +2357,7 @@
       </c>
       <c r="E17" s="8">
         <f t="shared" si="2"/>
-        <v>19000</v>
+        <v>24000</v>
       </c>
       <c r="I17" s="3">
         <v>3000</v>
@@ -2306,8 +2371,11 @@
       <c r="S17" s="9">
         <v>5000</v>
       </c>
-    </row>
-    <row r="18" s="3" customFormat="1" spans="1:24">
+      <c r="AC17" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="18" s="3" customFormat="1" spans="1:29">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -2322,7 +2390,7 @@
       </c>
       <c r="E18" s="8">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>7000</v>
       </c>
       <c r="S18" s="9">
         <v>1000</v>
@@ -2332,6 +2400,12 @@
       </c>
       <c r="X18" s="9">
         <v>1000</v>
+      </c>
+      <c r="AB18" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AC18" s="9">
+        <v>2000</v>
       </c>
     </row>
     <row r="19" s="3" customFormat="1" spans="1:26">
@@ -2391,7 +2465,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="21" s="3" customFormat="1" spans="1:23">
+    <row r="21" s="3" customFormat="1" spans="1:28">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -2403,7 +2477,7 @@
       </c>
       <c r="E21" s="8">
         <f t="shared" si="2"/>
-        <v>6000</v>
+        <v>7000</v>
       </c>
       <c r="I21" s="3">
         <v>2000</v>
@@ -2420,8 +2494,11 @@
       <c r="W21" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="22" s="3" customFormat="1" spans="1:23">
+      <c r="AB21" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" s="3" customFormat="1" spans="1:29">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -2433,7 +2510,7 @@
       </c>
       <c r="E22" s="8">
         <f t="shared" si="2"/>
-        <v>12000</v>
+        <v>15000</v>
       </c>
       <c r="I22" s="3">
         <v>3000</v>
@@ -2447,8 +2524,11 @@
       <c r="W22" s="3">
         <v>3000</v>
       </c>
-    </row>
-    <row r="23" s="3" customFormat="1" spans="1:23">
+      <c r="AC22" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="23" s="3" customFormat="1" spans="1:28">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -2460,7 +2540,7 @@
       </c>
       <c r="E23" s="8">
         <f t="shared" si="2"/>
-        <v>12000</v>
+        <v>17000</v>
       </c>
       <c r="S23" s="9">
         <v>2000</v>
@@ -2471,8 +2551,11 @@
       <c r="W23" s="9">
         <v>5000</v>
       </c>
-    </row>
-    <row r="24" s="3" customFormat="1" spans="1:26">
+      <c r="AB23" s="9">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="24" s="3" customFormat="1" spans="1:30">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -2484,7 +2567,7 @@
       </c>
       <c r="E24" s="8">
         <f t="shared" si="2"/>
-        <v>18000</v>
+        <v>21000</v>
       </c>
       <c r="N24" s="3">
         <v>6000</v>
@@ -2504,8 +2587,14 @@
       <c r="Z24" s="3">
         <v>3000</v>
       </c>
-    </row>
-    <row r="25" s="3" customFormat="1" spans="1:27">
+      <c r="AB24" s="3">
+        <v>500</v>
+      </c>
+      <c r="AD24" s="3">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="25" s="3" customFormat="1" spans="1:29">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -2517,7 +2606,7 @@
       </c>
       <c r="E25" s="8">
         <f t="shared" si="2"/>
-        <v>9500</v>
+        <v>10500</v>
       </c>
       <c r="M25" s="3">
         <v>3000</v>
@@ -2537,8 +2626,11 @@
       <c r="AA25" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="26" s="3" customFormat="1" spans="1:22">
+      <c r="AC25" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26" s="3" customFormat="1" spans="1:29">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -2550,10 +2642,13 @@
       </c>
       <c r="E26" s="8">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="V26" s="3">
         <v>3000</v>
+      </c>
+      <c r="AC26" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="27" s="3" customFormat="1" spans="1:23">
@@ -2622,7 +2717,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="29" s="3" customFormat="1" spans="1:27">
+    <row r="29" s="3" customFormat="1" spans="1:28">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -2634,7 +2729,7 @@
       </c>
       <c r="E29" s="8">
         <f t="shared" si="2"/>
-        <v>44000</v>
+        <v>49000</v>
       </c>
       <c r="I29" s="3">
         <v>2000</v>
@@ -2657,8 +2752,11 @@
       <c r="AA29" s="9">
         <v>5000</v>
       </c>
-    </row>
-    <row r="30" s="3" customFormat="1" spans="1:26">
+      <c r="AB29" s="9">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="30" s="3" customFormat="1" spans="1:30">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -2670,7 +2768,7 @@
       </c>
       <c r="E30" s="8">
         <f t="shared" si="2"/>
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="I30" s="3">
         <v>1000</v>
@@ -2704,6 +2802,12 @@
       </c>
       <c r="Z30" s="3">
         <v>500</v>
+      </c>
+      <c r="AC30" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AD30" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="31" s="3" customFormat="1" spans="1:26">
@@ -2793,7 +2897,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" s="3" customFormat="1" spans="1:23">
+    <row r="34" s="3" customFormat="1" spans="1:30">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -2805,7 +2909,7 @@
       </c>
       <c r="E34" s="8">
         <f t="shared" si="2"/>
-        <v>18000</v>
+        <v>24000</v>
       </c>
       <c r="H34" s="3">
         <v>2000</v>
@@ -2822,8 +2926,14 @@
       <c r="W34" s="9">
         <v>3000</v>
       </c>
-    </row>
-    <row r="35" s="3" customFormat="1" spans="1:22">
+      <c r="AB34" s="9">
+        <v>3000</v>
+      </c>
+      <c r="AD34" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="35" s="3" customFormat="1" spans="1:30">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -2835,9 +2945,12 @@
       </c>
       <c r="E35" s="8">
         <f t="shared" ref="E35:E66" si="3">SUM(F35:AJ35)</f>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="V35" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AD35" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -2925,7 +3038,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="39" s="3" customFormat="1" spans="1:27">
+    <row r="39" s="3" customFormat="1" spans="1:29">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -2937,7 +3050,7 @@
       </c>
       <c r="E39" s="8">
         <f t="shared" si="3"/>
-        <v>8000</v>
+        <v>9000</v>
       </c>
       <c r="H39" s="3">
         <v>2000</v>
@@ -2954,8 +3067,11 @@
       <c r="AA39" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="40" s="3" customFormat="1" spans="1:27">
+      <c r="AC39" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="40" s="3" customFormat="1" spans="1:30">
       <c r="A40" s="3">
         <v>38</v>
       </c>
@@ -2967,7 +3083,7 @@
       </c>
       <c r="E40" s="8">
         <f t="shared" si="3"/>
-        <v>26000</v>
+        <v>30000</v>
       </c>
       <c r="H40" s="3">
         <v>2000</v>
@@ -2993,8 +3109,11 @@
       <c r="AA40" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="41" s="3" customFormat="1" spans="1:16">
+      <c r="AD40" s="3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="41" s="3" customFormat="1" spans="1:29">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -3006,13 +3125,16 @@
       </c>
       <c r="E41" s="8">
         <f t="shared" si="3"/>
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="K41" s="3">
         <v>2000</v>
       </c>
       <c r="P41" s="3">
         <v>1000</v>
+      </c>
+      <c r="AC41" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="42" s="3" customFormat="1" spans="1:5">
@@ -3030,7 +3152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" s="3" customFormat="1" spans="1:23">
+    <row r="43" s="3" customFormat="1" spans="1:29">
       <c r="A43" s="3">
         <v>41</v>
       </c>
@@ -3042,7 +3164,7 @@
       </c>
       <c r="E43" s="8">
         <f t="shared" si="3"/>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="H43" s="9">
         <v>5000</v>
@@ -3057,6 +3179,9 @@
         <v>3000</v>
       </c>
       <c r="W43" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AC43" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -3090,7 +3215,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="45" s="3" customFormat="1" spans="1:24">
+    <row r="45" s="3" customFormat="1" spans="1:28">
       <c r="A45" s="3">
         <v>43</v>
       </c>
@@ -3102,7 +3227,7 @@
       </c>
       <c r="E45" s="8">
         <f t="shared" si="3"/>
-        <v>16000</v>
+        <v>19000</v>
       </c>
       <c r="I45" s="3">
         <v>2000</v>
@@ -3120,6 +3245,9 @@
         <v>3000</v>
       </c>
       <c r="X45" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AB45" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -3150,7 +3278,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="47" s="3" customFormat="1" spans="1:24">
+    <row r="47" s="3" customFormat="1" spans="1:29">
       <c r="A47" s="3">
         <v>45</v>
       </c>
@@ -3162,7 +3290,7 @@
       </c>
       <c r="E47" s="8">
         <f t="shared" si="3"/>
-        <v>11000</v>
+        <v>14000</v>
       </c>
       <c r="O47" s="3">
         <v>2000</v>
@@ -3176,8 +3304,11 @@
       <c r="X47" s="9">
         <v>3000</v>
       </c>
-    </row>
-    <row r="48" s="3" customFormat="1" spans="1:24">
+      <c r="AC47" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="48" s="3" customFormat="1" spans="1:29">
       <c r="A48" s="3">
         <v>46</v>
       </c>
@@ -3192,7 +3323,7 @@
       </c>
       <c r="E48" s="8">
         <f t="shared" si="3"/>
-        <v>15000</v>
+        <v>21000</v>
       </c>
       <c r="I48" s="9">
         <v>2000</v>
@@ -3211,6 +3342,9 @@
       </c>
       <c r="X48" s="9">
         <v>500</v>
+      </c>
+      <c r="AC48" s="9">
+        <v>6000</v>
       </c>
     </row>
     <row r="49" s="3" customFormat="1" spans="1:27">
@@ -3270,7 +3404,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="51" s="3" customFormat="1" spans="1:24">
+    <row r="51" s="3" customFormat="1" spans="1:30">
       <c r="A51" s="3">
         <v>49</v>
       </c>
@@ -3285,7 +3419,7 @@
       </c>
       <c r="E51" s="8">
         <f t="shared" si="3"/>
-        <v>16000</v>
+        <v>19000</v>
       </c>
       <c r="I51" s="9">
         <v>4000</v>
@@ -3305,137 +3439,143 @@
       <c r="X51" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="52" s="3" customFormat="1" spans="1:24">
+      <c r="AD51" s="9">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="52" s="3" customFormat="1" spans="1:28">
       <c r="A52" s="3">
         <v>50</v>
       </c>
       <c r="C52" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D52" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D52" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="E52" s="8">
-        <f t="shared" si="3"/>
-        <v>7000</v>
-      </c>
-      <c r="Q52" s="3">
-        <v>1000</v>
-      </c>
-      <c r="T52" s="3">
-        <v>4000</v>
-      </c>
-      <c r="X52" s="3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="53" s="3" customFormat="1" spans="1:26">
+        <f>SUM(F52:AJ52)</f>
+        <v>2000</v>
+      </c>
+      <c r="AB52" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="53" s="3" customFormat="1" spans="1:24">
       <c r="A53" s="3">
         <v>51</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E53" s="8">
-        <f t="shared" si="3"/>
-        <v>22000</v>
-      </c>
-      <c r="N53" s="3">
-        <v>8000</v>
+        <f>SUM(F53:AJ53)</f>
+        <v>7000</v>
+      </c>
+      <c r="Q53" s="3">
+        <v>1000</v>
       </c>
       <c r="T53" s="3">
-        <v>5000</v>
-      </c>
-      <c r="V53" s="3">
-        <v>5000</v>
-      </c>
-      <c r="Z53" s="3">
         <v>4000</v>
       </c>
-    </row>
-    <row r="54" s="3" customFormat="1" spans="1:26">
+      <c r="X53" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="54" s="3" customFormat="1" spans="1:29">
       <c r="A54" s="3">
         <v>52</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>69</v>
       </c>
       <c r="E54" s="8">
-        <f t="shared" si="3"/>
-        <v>5500</v>
-      </c>
-      <c r="L54" s="3">
-        <v>1500</v>
-      </c>
-      <c r="Q54" s="3">
-        <v>500</v>
+        <f>SUM(F54:AJ54)</f>
+        <v>28000</v>
+      </c>
+      <c r="N54" s="3">
+        <v>8000</v>
       </c>
       <c r="T54" s="3">
-        <v>1500</v>
-      </c>
-      <c r="Z54" s="9">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="55" s="3" customFormat="1" spans="1:15">
+        <v>5000</v>
+      </c>
+      <c r="V54" s="3">
+        <v>5000</v>
+      </c>
+      <c r="Z54" s="3">
+        <v>4000</v>
+      </c>
+      <c r="AB54" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AC54" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="55" s="3" customFormat="1" spans="1:26">
       <c r="A55" s="3">
         <v>53</v>
       </c>
       <c r="C55" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="E55" s="8">
-        <f t="shared" si="3"/>
-        <v>4000</v>
-      </c>
-      <c r="O55" s="9">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="56" s="3" customFormat="1" spans="1:22">
+        <f>SUM(F55:AJ55)</f>
+        <v>5500</v>
+      </c>
+      <c r="L55" s="3">
+        <v>1500</v>
+      </c>
+      <c r="Q55" s="3">
+        <v>500</v>
+      </c>
+      <c r="T55" s="3">
+        <v>1500</v>
+      </c>
+      <c r="Z55" s="9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="56" s="3" customFormat="1" spans="1:28">
       <c r="A56" s="3">
         <v>54</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="D56" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D56" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="E56" s="8">
-        <f t="shared" si="3"/>
-        <v>6000</v>
-      </c>
-      <c r="J56" s="3">
-        <v>1000</v>
-      </c>
-      <c r="Q56" s="9">
-        <v>2000</v>
-      </c>
-      <c r="S56" s="9">
-        <v>1000</v>
-      </c>
-      <c r="V56" s="9">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="57" s="3" customFormat="1" spans="1:22">
+        <f>SUM(F56:AJ56)</f>
+        <v>9000</v>
+      </c>
+      <c r="O56" s="9">
+        <v>4000</v>
+      </c>
+      <c r="AB56" s="9">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="57" s="3" customFormat="1" spans="1:29">
       <c r="A57" s="3">
         <v>55</v>
       </c>
+      <c r="B57" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="C57" s="3" t="s">
         <v>75</v>
       </c>
@@ -3443,14 +3583,26 @@
         <v>76</v>
       </c>
       <c r="E57" s="8">
-        <f t="shared" si="3"/>
-        <v>2000</v>
-      </c>
-      <c r="V57" s="3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="58" s="3" customFormat="1" spans="1:27">
+        <f>SUM(F57:AJ57)</f>
+        <v>10000</v>
+      </c>
+      <c r="J57" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q57" s="9">
+        <v>2000</v>
+      </c>
+      <c r="S57" s="9">
+        <v>1000</v>
+      </c>
+      <c r="V57" s="9">
+        <v>2000</v>
+      </c>
+      <c r="AC57" s="9">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="58" s="3" customFormat="1" spans="1:29">
       <c r="A58" s="3">
         <v>56</v>
       </c>
@@ -3461,350 +3613,377 @@
         <v>78</v>
       </c>
       <c r="E58" s="8">
-        <f t="shared" si="3"/>
-        <v>9000</v>
-      </c>
-      <c r="P58" s="3">
-        <v>5000</v>
+        <f>SUM(F58:AJ58)</f>
+        <v>4000</v>
       </c>
       <c r="V58" s="3">
         <v>2000</v>
       </c>
-      <c r="AA58" s="3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="59" s="3" customFormat="1" spans="1:22">
+      <c r="AC58" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="59" s="3" customFormat="1" spans="1:27">
       <c r="A59" s="3">
         <v>57</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E59" s="8">
-        <f t="shared" si="3"/>
-        <v>7000</v>
-      </c>
-      <c r="J59" s="3">
-        <v>3000</v>
-      </c>
-      <c r="O59" s="3">
-        <v>2000</v>
+        <f>SUM(F59:AJ59)</f>
+        <v>9000</v>
+      </c>
+      <c r="P59" s="3">
+        <v>5000</v>
       </c>
       <c r="V59" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="60" s="3" customFormat="1" spans="1:25">
+      <c r="AA59" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="60" s="3" customFormat="1" spans="1:30">
       <c r="A60" s="3">
         <v>58</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E60" s="8">
-        <f t="shared" si="3"/>
-        <v>5000</v>
+        <f>SUM(F60:AJ60)</f>
+        <v>9000</v>
       </c>
       <c r="J60" s="3">
-        <v>1000</v>
+        <v>3000</v>
+      </c>
+      <c r="O60" s="3">
+        <v>2000</v>
       </c>
       <c r="V60" s="3">
         <v>2000</v>
       </c>
-      <c r="Y60" s="3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="61" s="3" customFormat="1" spans="1:24">
+      <c r="AD60" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="61" s="3" customFormat="1" spans="1:25">
       <c r="A61" s="3">
         <v>59</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E61" s="8">
-        <f t="shared" si="3"/>
-        <v>3000</v>
+        <f>SUM(F61:AJ61)</f>
+        <v>5000</v>
       </c>
       <c r="J61" s="3">
-        <v>2000</v>
-      </c>
-      <c r="X61" s="3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="62" s="3" customFormat="1" spans="1:26">
+        <v>1000</v>
+      </c>
+      <c r="V61" s="3">
+        <v>2000</v>
+      </c>
+      <c r="Y61" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="62" s="3" customFormat="1" spans="1:30">
       <c r="A62" s="3">
         <v>60</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E62" s="8">
-        <f t="shared" si="3"/>
-        <v>42000</v>
+        <f>SUM(F62:AJ62)</f>
+        <v>4000</v>
       </c>
       <c r="J62" s="3">
         <v>2000</v>
       </c>
-      <c r="K62" s="3">
-        <v>15000</v>
-      </c>
-      <c r="O62" s="3">
-        <v>5000</v>
-      </c>
-      <c r="S62" s="3">
-        <v>5000</v>
-      </c>
-      <c r="V62" s="3">
-        <v>5000</v>
-      </c>
-      <c r="Y62" s="3">
-        <v>5000</v>
-      </c>
-      <c r="Z62" s="3">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="63" s="3" customFormat="1" spans="1:27">
+      <c r="X62" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AD62" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="63" s="3" customFormat="1" spans="1:26">
       <c r="A63" s="3">
         <v>61</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E63" s="8">
-        <f t="shared" si="3"/>
-        <v>18000</v>
-      </c>
-      <c r="K63" s="9">
-        <v>4000</v>
-      </c>
-      <c r="L63" s="3">
-        <v>2000</v>
+        <f>SUM(F63:AJ63)</f>
+        <v>42000</v>
+      </c>
+      <c r="J63" s="3">
+        <v>2000</v>
+      </c>
+      <c r="K63" s="3">
+        <v>15000</v>
       </c>
       <c r="O63" s="3">
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="S63" s="3">
-        <v>3000</v>
-      </c>
-      <c r="W63" s="3">
-        <v>3000</v>
-      </c>
-      <c r="AA63" s="3">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="64" s="3" customFormat="1" spans="1:26">
+        <v>5000</v>
+      </c>
+      <c r="V63" s="3">
+        <v>5000</v>
+      </c>
+      <c r="Y63" s="3">
+        <v>5000</v>
+      </c>
+      <c r="Z63" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="64" s="3" customFormat="1" spans="1:27">
       <c r="A64" s="3">
         <v>62</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E64" s="8">
-        <f t="shared" si="3"/>
-        <v>2000</v>
-      </c>
-      <c r="X64" s="3">
-        <v>1500</v>
-      </c>
-      <c r="Z64" s="3">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="65" s="3" customFormat="1" spans="1:27">
+        <f>SUM(F64:AJ64)</f>
+        <v>18000</v>
+      </c>
+      <c r="K64" s="9">
+        <v>4000</v>
+      </c>
+      <c r="L64" s="3">
+        <v>2000</v>
+      </c>
+      <c r="O64" s="3">
+        <v>3000</v>
+      </c>
+      <c r="S64" s="3">
+        <v>3000</v>
+      </c>
+      <c r="W64" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AA64" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="65" s="3" customFormat="1" spans="1:30">
       <c r="A65" s="3">
         <v>63</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>86</v>
       </c>
       <c r="E65" s="8">
-        <f t="shared" si="3"/>
-        <v>12800</v>
-      </c>
-      <c r="I65" s="9">
-        <v>1000</v>
-      </c>
-      <c r="L65" s="9">
-        <v>2000</v>
-      </c>
-      <c r="S65" s="3">
-        <v>2000</v>
-      </c>
-      <c r="U65" s="3">
-        <v>2500</v>
-      </c>
-      <c r="V65" s="3">
-        <v>1000</v>
-      </c>
-      <c r="W65" s="3">
-        <v>1800</v>
+        <f>SUM(F65:AJ65)</f>
+        <v>3000</v>
       </c>
       <c r="X65" s="3">
-        <v>600</v>
-      </c>
-      <c r="AA65" s="3">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="66" s="3" customFormat="1" spans="1:26">
+        <v>1500</v>
+      </c>
+      <c r="Z65" s="3">
+        <v>500</v>
+      </c>
+      <c r="AD65" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="66" s="3" customFormat="1" spans="1:30">
       <c r="A66" s="3">
         <v>64</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E66" s="8">
-        <f t="shared" si="3"/>
-        <v>21000</v>
-      </c>
-      <c r="J66" s="9">
-        <v>3000</v>
+        <f>SUM(F66:AJ66)</f>
+        <v>15000</v>
+      </c>
+      <c r="I66" s="9">
+        <v>1000</v>
       </c>
       <c r="L66" s="9">
-        <v>3000</v>
-      </c>
-      <c r="O66" s="3">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="S66" s="3">
-        <v>3000</v>
-      </c>
-      <c r="T66" s="3">
-        <v>3000</v>
+        <v>2000</v>
+      </c>
+      <c r="U66" s="3">
+        <v>2500</v>
+      </c>
+      <c r="V66" s="3">
+        <v>1000</v>
+      </c>
+      <c r="W66" s="3">
+        <v>1800</v>
       </c>
       <c r="X66" s="3">
-        <v>3000</v>
-      </c>
-      <c r="Z66" s="3">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="67" s="3" customFormat="1" spans="1:24">
+        <v>600</v>
+      </c>
+      <c r="AA66" s="3">
+        <v>1900</v>
+      </c>
+      <c r="AD66" s="9">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="67" s="3" customFormat="1" spans="1:30">
       <c r="A67" s="3">
         <v>65</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E67" s="8">
-        <f t="shared" ref="E67:E92" si="4">SUM(F67:AJ67)</f>
-        <v>15000</v>
-      </c>
-      <c r="I67" s="3">
-        <v>2000</v>
-      </c>
-      <c r="K67" s="3">
-        <v>1000</v>
-      </c>
-      <c r="N67" s="3">
-        <v>2000</v>
-      </c>
-      <c r="Q67" s="3">
-        <v>1000</v>
-      </c>
-      <c r="S67" s="9">
-        <v>3000</v>
-      </c>
-      <c r="U67" s="3">
-        <v>2000</v>
-      </c>
-      <c r="X67" s="9">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="68" s="3" customFormat="1" spans="1:5">
+        <f>SUM(F67:AJ67)</f>
+        <v>24000</v>
+      </c>
+      <c r="J67" s="9">
+        <v>3000</v>
+      </c>
+      <c r="L67" s="9">
+        <v>3000</v>
+      </c>
+      <c r="O67" s="3">
+        <v>3000</v>
+      </c>
+      <c r="S67" s="3">
+        <v>3000</v>
+      </c>
+      <c r="T67" s="3">
+        <v>3000</v>
+      </c>
+      <c r="X67" s="3">
+        <v>3000</v>
+      </c>
+      <c r="Z67" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AD67" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="68" s="3" customFormat="1" spans="1:30">
       <c r="A68" s="3">
         <v>66</v>
       </c>
+      <c r="C68" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="D68" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E68" s="8">
+        <f t="shared" ref="E68:E84" si="4">SUM(F68:AJ68)</f>
+        <v>17000</v>
+      </c>
+      <c r="I68" s="3">
+        <v>2000</v>
+      </c>
+      <c r="K68" s="3">
+        <v>1000</v>
+      </c>
+      <c r="N68" s="3">
+        <v>2000</v>
+      </c>
+      <c r="Q68" s="3">
+        <v>1000</v>
+      </c>
+      <c r="S68" s="9">
+        <v>3000</v>
+      </c>
+      <c r="U68" s="3">
+        <v>2000</v>
+      </c>
+      <c r="X68" s="9">
+        <v>4000</v>
+      </c>
+      <c r="AD68" s="9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="69" s="3" customFormat="1" spans="1:5">
+      <c r="A69" s="3">
+        <v>67</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E69" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="69" s="3" customFormat="1" spans="1:23">
-      <c r="A69" s="3">
-        <v>67</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E69" s="8">
-        <f t="shared" si="4"/>
-        <v>4000</v>
-      </c>
-      <c r="W69" s="3">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="70" s="3" customFormat="1" spans="1:27">
+    <row r="70" s="3" customFormat="1" spans="1:23">
       <c r="A70" s="3">
         <v>68</v>
       </c>
-      <c r="B70" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C70" s="3" t="s">
+      <c r="D70" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="E70" s="8">
         <f t="shared" si="4"/>
         <v>4000</v>
       </c>
-      <c r="P70" s="9">
-        <v>2000</v>
-      </c>
-      <c r="AA70" s="9">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="71" s="3" customFormat="1" spans="1:5">
+      <c r="W70" s="3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="71" s="3" customFormat="1" spans="1:27">
       <c r="A71" s="3">
         <v>69</v>
       </c>
+      <c r="B71" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="D71" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E71" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4000</v>
+      </c>
+      <c r="P71" s="9">
+        <v>2000</v>
+      </c>
+      <c r="AA71" s="9">
+        <v>2000</v>
       </c>
     </row>
     <row r="72" s="3" customFormat="1" spans="1:5">
@@ -3812,7 +3991,7 @@
         <v>70</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E72" s="8">
         <f t="shared" si="4"/>
@@ -3824,7 +4003,7 @@
         <v>71</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E73" s="8">
         <f t="shared" si="4"/>
@@ -3836,7 +4015,7 @@
         <v>72</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E74" s="8">
         <f t="shared" si="4"/>
@@ -3848,23 +4027,29 @@
         <v>73</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E75" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="76" s="3" customFormat="1" spans="1:5">
+    <row r="76" s="3" customFormat="1" spans="1:30">
       <c r="A76" s="3">
         <v>74</v>
       </c>
+      <c r="B76" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D76" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E76" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3000</v>
+      </c>
+      <c r="AD76" s="9">
+        <v>3000</v>
       </c>
     </row>
     <row r="77" s="3" customFormat="1" spans="1:5">
@@ -3872,7 +4057,7 @@
         <v>75</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E77" s="8">
         <f t="shared" si="4"/>
@@ -3884,7 +4069,7 @@
         <v>76</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E78" s="8">
         <f t="shared" si="4"/>
@@ -3896,41 +4081,47 @@
         <v>77</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E79" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="80" s="3" customFormat="1" spans="1:27">
+    <row r="80" s="3" customFormat="1" spans="1:5">
       <c r="A80" s="3">
         <v>78</v>
       </c>
-      <c r="C80" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="D80" s="4" t="s">
         <v>104</v>
       </c>
       <c r="E80" s="8">
         <f t="shared" si="4"/>
-        <v>2000</v>
-      </c>
-      <c r="AA80" s="9">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="81" s="3" customFormat="1" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" s="3" customFormat="1" spans="1:30">
       <c r="A81" s="3">
         <v>79</v>
       </c>
+      <c r="C81" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="D81" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E81" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8000</v>
+      </c>
+      <c r="AA81" s="9">
+        <v>2000</v>
+      </c>
+      <c r="AB81" s="9">
+        <v>3000</v>
+      </c>
+      <c r="AD81" s="9">
+        <v>3000</v>
       </c>
     </row>
     <row r="82" s="3" customFormat="1" spans="1:5">
@@ -3938,44 +4129,44 @@
         <v>80</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E82" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="83" s="3" customFormat="1" spans="1:27">
+    <row r="83" s="3" customFormat="1" spans="1:5">
       <c r="A83" s="3">
         <v>81</v>
       </c>
-      <c r="B83" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="D83" s="4" t="s">
         <v>108</v>
       </c>
       <c r="E83" s="8">
         <f t="shared" si="4"/>
-        <v>2000</v>
-      </c>
-      <c r="AA83" s="9">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="84" s="3" customFormat="1" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" s="3" customFormat="1" spans="1:27">
       <c r="A84" s="3">
         <v>82</v>
       </c>
+      <c r="B84" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="D84" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E84" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="AA84" s="9">
+        <v>2000</v>
       </c>
     </row>
     <row r="85" s="3" customFormat="1" spans="1:5">
@@ -3983,10 +4174,10 @@
         <v>83</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E85" s="8">
-        <f t="shared" si="4"/>
+        <f>SUM(F85:AJ85)</f>
         <v>0</v>
       </c>
     </row>
@@ -3995,10 +4186,10 @@
         <v>84</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E86" s="8">
-        <f t="shared" si="4"/>
+        <f>SUM(F86:AJ86)</f>
         <v>0</v>
       </c>
     </row>
@@ -4007,10 +4198,10 @@
         <v>85</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E87" s="8">
-        <f t="shared" si="4"/>
+        <f>SUM(F87:AJ87)</f>
         <v>0</v>
       </c>
     </row>
@@ -4019,10 +4210,10 @@
         <v>86</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E88" s="8">
-        <f t="shared" si="4"/>
+        <f>SUM(F88:AJ88)</f>
         <v>0</v>
       </c>
     </row>
@@ -4031,10 +4222,10 @@
         <v>87</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E89" s="8">
-        <f t="shared" si="4"/>
+        <f>SUM(F89:AJ89)</f>
         <v>0</v>
       </c>
     </row>
@@ -4043,10 +4234,10 @@
         <v>88</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E90" s="8">
-        <f t="shared" si="4"/>
+        <f>SUM(F90:AJ90)</f>
         <v>0</v>
       </c>
     </row>
@@ -4055,10 +4246,10 @@
         <v>89</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E91" s="8">
-        <f t="shared" si="4"/>
+        <f>SUM(F91:AJ91)</f>
         <v>0</v>
       </c>
     </row>
@@ -4067,10 +4258,10 @@
         <v>90</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E92" s="8">
-        <f t="shared" si="4"/>
+        <f>SUM(F92:AJ92)</f>
         <v>0</v>
       </c>
     </row>
@@ -4079,7 +4270,7 @@
         <v>91</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E93" s="8">
         <f>SUM(F93:AJ93)</f>

</xml_diff>

<commit_message>
data updated till 31Dec 6AM
</commit_message>
<xml_diff>
--- a/Daily Collection/December-2020-Collection.xlsx
+++ b/Daily Collection/December-2020-Collection.xlsx
@@ -234,7 +234,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="130">
   <si>
     <t>S.No.</t>
   </si>
@@ -534,6 +534,9 @@
   </si>
   <si>
     <t>PRAKASH GENERAL SRINGAR STORE(661303685)</t>
+  </si>
+  <si>
+    <t>Sunil Kr.</t>
   </si>
   <si>
     <t>ANAND SRINGAR STORE(660831268)</t>
@@ -628,10 +631,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="23">
@@ -659,9 +662,32 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -673,6 +699,75 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -689,68 +784,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -759,48 +792,18 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
@@ -839,7 +842,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -851,175 +1016,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1033,61 +1036,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1110,8 +1063,32 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1130,12 +1107,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1153,130 +1156,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1641,11 +1644,11 @@
   <dimension ref="A1:AK94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="AC84" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="AC51" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:A94"/>
+      <selection pane="bottomRight" activeCell="AJ71" sqref="AJ71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1774,14 +1777,14 @@
     <row r="2" s="2" customFormat="1" spans="4:37">
       <c r="D2" s="6">
         <f>SUM(F3:F119)</f>
-        <v>1092500</v>
+        <v>1132500</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="6">
-        <f>SUM(G2:AK2)</f>
-        <v>1092500</v>
+        <f t="shared" ref="F2:F16" si="0">SUM(G2:AK2)</f>
+        <v>1132500</v>
       </c>
       <c r="G2" s="2">
         <f>SUM(G3:G120)</f>
@@ -1804,107 +1807,107 @@
         <v>21000</v>
       </c>
       <c r="L2" s="2">
-        <f t="shared" ref="L2:AK2" si="0">SUM(L3:L120)</f>
+        <f t="shared" ref="L2:AK2" si="1">SUM(L3:L120)</f>
         <v>47500</v>
       </c>
       <c r="M2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42500</v>
       </c>
       <c r="N2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27000</v>
       </c>
       <c r="O2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>71900</v>
       </c>
       <c r="P2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59000</v>
       </c>
       <c r="Q2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26000</v>
       </c>
       <c r="R2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29100</v>
       </c>
       <c r="S2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>75000</v>
       </c>
       <c r="U2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49500</v>
       </c>
       <c r="V2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47000</v>
       </c>
       <c r="W2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53000</v>
       </c>
       <c r="X2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56300</v>
       </c>
       <c r="Y2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42100</v>
       </c>
       <c r="Z2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7000</v>
       </c>
       <c r="AA2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33000</v>
       </c>
       <c r="AB2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39400</v>
       </c>
       <c r="AC2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41500</v>
       </c>
       <c r="AD2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54500</v>
       </c>
       <c r="AE2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39700</v>
       </c>
       <c r="AF2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17500</v>
       </c>
       <c r="AG2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31500</v>
       </c>
       <c r="AH2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59000</v>
       </c>
       <c r="AI2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50500</v>
       </c>
       <c r="AJ2" s="2">
-        <f t="shared" si="0"/>
-        <v>2000</v>
+        <f t="shared" si="1"/>
+        <v>42000</v>
       </c>
       <c r="AK2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1919,7 +1922,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="8">
-        <f>SUM(G3:AK3)</f>
+        <f t="shared" si="0"/>
         <v>6000</v>
       </c>
       <c r="V3" s="9">
@@ -1940,7 +1943,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="8">
-        <f>SUM(G4:AK4)</f>
+        <f t="shared" si="0"/>
         <v>6000</v>
       </c>
       <c r="L4" s="9">
@@ -1964,7 +1967,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="8">
-        <f>SUM(G5:AK5)</f>
+        <f t="shared" si="0"/>
         <v>14000</v>
       </c>
       <c r="I5" s="3">
@@ -2009,7 +2012,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="8">
-        <f>SUM(G6:AK6)</f>
+        <f t="shared" si="0"/>
         <v>24500</v>
       </c>
       <c r="I6" s="9">
@@ -2051,7 +2054,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="8">
-        <f>SUM(G7:AK7)</f>
+        <f t="shared" si="0"/>
         <v>46000</v>
       </c>
       <c r="I7" s="3">
@@ -2102,7 +2105,7 @@
         <v>13</v>
       </c>
       <c r="F8" s="8">
-        <f>SUM(G8:AK8)</f>
+        <f t="shared" si="0"/>
         <v>5000</v>
       </c>
       <c r="O8" s="3">
@@ -2126,7 +2129,7 @@
         <v>14</v>
       </c>
       <c r="F9" s="8">
-        <f>SUM(G9:AK9)</f>
+        <f t="shared" si="0"/>
         <v>8000</v>
       </c>
       <c r="I9" s="3">
@@ -2156,7 +2159,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="8">
-        <f>SUM(G10:AK10)</f>
+        <f t="shared" si="0"/>
         <v>40000</v>
       </c>
       <c r="I10" s="3">
@@ -2201,7 +2204,7 @@
         <v>18</v>
       </c>
       <c r="F11" s="8">
-        <f>SUM(G11:AK11)</f>
+        <f t="shared" si="0"/>
         <v>13000</v>
       </c>
       <c r="I11" s="9">
@@ -2220,7 +2223,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="12" s="3" customFormat="1" spans="1:34">
+    <row r="12" s="3" customFormat="1" spans="1:36">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -2231,8 +2234,8 @@
         <v>19</v>
       </c>
       <c r="F12" s="8">
-        <f>SUM(G12:AK12)</f>
-        <v>6000</v>
+        <f t="shared" si="0"/>
+        <v>7000</v>
       </c>
       <c r="M12" s="3">
         <v>1000</v>
@@ -2255,8 +2258,11 @@
       <c r="AH12" s="3">
         <v>500</v>
       </c>
-    </row>
-    <row r="13" s="3" customFormat="1" spans="1:31">
+      <c r="AJ12" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" s="3" customFormat="1" spans="1:36">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -2267,8 +2273,8 @@
         <v>20</v>
       </c>
       <c r="F13" s="8">
-        <f>SUM(G13:AK13)</f>
-        <v>28000</v>
+        <f t="shared" si="0"/>
+        <v>33000</v>
       </c>
       <c r="I13" s="3">
         <v>2000</v>
@@ -2288,8 +2294,11 @@
       <c r="AE13" s="3">
         <v>5000</v>
       </c>
-    </row>
-    <row r="14" s="3" customFormat="1" spans="1:35">
+      <c r="AJ13" s="9">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="14" s="3" customFormat="1" spans="1:36">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2300,8 +2309,8 @@
         <v>21</v>
       </c>
       <c r="F14" s="8">
-        <f>SUM(G14:AK14)</f>
-        <v>45500</v>
+        <f t="shared" si="0"/>
+        <v>47500</v>
       </c>
       <c r="I14" s="3">
         <v>2000</v>
@@ -2362,6 +2371,9 @@
       </c>
       <c r="AI14" s="3">
         <v>2500</v>
+      </c>
+      <c r="AJ14" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" spans="1:35">
@@ -2378,7 +2390,7 @@
         <v>23</v>
       </c>
       <c r="F15" s="8">
-        <f>SUM(G15:AK15)</f>
+        <f t="shared" si="0"/>
         <v>8000</v>
       </c>
       <c r="T15" s="3">
@@ -2408,7 +2420,7 @@
         <v>25</v>
       </c>
       <c r="F16" s="8">
-        <f>SUM(G16:AK16)</f>
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
       <c r="AH16" s="9">
@@ -2429,7 +2441,7 @@
         <v>27</v>
       </c>
       <c r="F17" s="8">
-        <f t="shared" ref="F17:F35" si="1">SUM(G17:AK17)</f>
+        <f t="shared" ref="F17:F35" si="2">SUM(G17:AK17)</f>
         <v>18000</v>
       </c>
       <c r="N17" s="3">
@@ -2454,7 +2466,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="18" s="3" customFormat="1" spans="1:30">
+    <row r="18" s="3" customFormat="1" spans="1:36">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -2465,8 +2477,8 @@
         <v>29</v>
       </c>
       <c r="F18" s="8">
-        <f t="shared" si="1"/>
-        <v>24000</v>
+        <f t="shared" si="2"/>
+        <v>29000</v>
       </c>
       <c r="J18" s="3">
         <v>3000</v>
@@ -2481,6 +2493,9 @@
         <v>5000</v>
       </c>
       <c r="AD18" s="3">
+        <v>5000</v>
+      </c>
+      <c r="AJ18" s="9">
         <v>5000</v>
       </c>
     </row>
@@ -2498,7 +2513,7 @@
         <v>31</v>
       </c>
       <c r="F19" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9000</v>
       </c>
       <c r="T19" s="9">
@@ -2520,7 +2535,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="20" s="3" customFormat="1" spans="1:34">
+    <row r="20" s="3" customFormat="1" spans="1:36">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -2531,8 +2546,8 @@
         <v>32</v>
       </c>
       <c r="F20" s="8">
-        <f t="shared" si="1"/>
-        <v>10500</v>
+        <f t="shared" si="2"/>
+        <v>12000</v>
       </c>
       <c r="J20" s="3">
         <v>1000</v>
@@ -2553,6 +2568,9 @@
         <v>1500</v>
       </c>
       <c r="AH20" s="3">
+        <v>1500</v>
+      </c>
+      <c r="AJ20" s="3">
         <v>1500</v>
       </c>
     </row>
@@ -2567,7 +2585,7 @@
         <v>33</v>
       </c>
       <c r="F21" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22000</v>
       </c>
       <c r="Q21" s="9">
@@ -2583,7 +2601,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="22" s="3" customFormat="1" spans="1:29">
+    <row r="22" s="3" customFormat="1" spans="1:36">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -2594,8 +2612,8 @@
         <v>34</v>
       </c>
       <c r="F22" s="8">
-        <f t="shared" si="1"/>
-        <v>7000</v>
+        <f t="shared" si="2"/>
+        <v>9000</v>
       </c>
       <c r="J22" s="3">
         <v>2000</v>
@@ -2615,8 +2633,11 @@
       <c r="AC22" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="23" s="3" customFormat="1" spans="1:32">
+      <c r="AJ22" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="23" s="3" customFormat="1" spans="1:36">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -2627,8 +2648,8 @@
         <v>35</v>
       </c>
       <c r="F23" s="8">
-        <f t="shared" si="1"/>
-        <v>18000</v>
+        <f t="shared" si="2"/>
+        <v>21000</v>
       </c>
       <c r="J23" s="3">
         <v>3000</v>
@@ -2646,6 +2667,9 @@
         <v>3000</v>
       </c>
       <c r="AF23" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AJ23" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -2663,7 +2687,7 @@
         <v>37</v>
       </c>
       <c r="F24" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22000</v>
       </c>
       <c r="T24" s="9">
@@ -2682,7 +2706,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="25" s="3" customFormat="1" spans="1:31">
+    <row r="25" s="3" customFormat="1" spans="1:36">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -2696,8 +2720,8 @@
         <v>38</v>
       </c>
       <c r="F25" s="8">
-        <f t="shared" si="1"/>
-        <v>21000</v>
+        <f t="shared" si="2"/>
+        <v>24000</v>
       </c>
       <c r="O25" s="3">
         <v>6000</v>
@@ -2723,8 +2747,11 @@
       <c r="AE25" s="3">
         <v>2500</v>
       </c>
-    </row>
-    <row r="26" s="3" customFormat="1" spans="1:35">
+      <c r="AJ25" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="26" s="3" customFormat="1" spans="1:36">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -2735,8 +2762,8 @@
         <v>39</v>
       </c>
       <c r="F26" s="8">
-        <f t="shared" si="1"/>
-        <v>11500</v>
+        <f t="shared" si="2"/>
+        <v>12500</v>
       </c>
       <c r="N26" s="3">
         <v>3000</v>
@@ -2762,8 +2789,11 @@
       <c r="AI26" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="27" s="3" customFormat="1" spans="1:30">
+      <c r="AJ26" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" s="3" customFormat="1" spans="1:36">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -2774,8 +2804,8 @@
         <v>40</v>
       </c>
       <c r="F27" s="8">
-        <f t="shared" si="1"/>
-        <v>5000</v>
+        <f t="shared" si="2"/>
+        <v>7000</v>
       </c>
       <c r="W27" s="3">
         <v>3000</v>
@@ -2783,8 +2813,11 @@
       <c r="AD27" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="28" s="3" customFormat="1" spans="1:24">
+      <c r="AJ27" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="28" s="3" customFormat="1" spans="1:36">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -2795,8 +2828,8 @@
         <v>41</v>
       </c>
       <c r="F28" s="8">
-        <f t="shared" si="1"/>
-        <v>8000</v>
+        <f t="shared" si="2"/>
+        <v>10000</v>
       </c>
       <c r="J28" s="3">
         <v>1000</v>
@@ -2815,6 +2848,9 @@
       </c>
       <c r="X28" s="3">
         <v>1000</v>
+      </c>
+      <c r="AJ28" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="29" s="3" customFormat="1" spans="1:34">
@@ -2828,7 +2864,7 @@
         <v>42</v>
       </c>
       <c r="F29" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22000</v>
       </c>
       <c r="I29" s="9">
@@ -2867,7 +2903,7 @@
         <v>44</v>
       </c>
       <c r="F30" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>54000</v>
       </c>
       <c r="J30" s="3">
@@ -2909,7 +2945,7 @@
         <v>45</v>
       </c>
       <c r="F31" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14000</v>
       </c>
       <c r="J31" s="3">
@@ -2969,7 +3005,7 @@
         <v>47</v>
       </c>
       <c r="F32" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11000</v>
       </c>
       <c r="I32" s="3">
@@ -3005,7 +3041,7 @@
         <v>48</v>
       </c>
       <c r="F33" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6000</v>
       </c>
       <c r="I33" s="3">
@@ -3038,7 +3074,7 @@
         <v>49</v>
       </c>
       <c r="F34" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4000</v>
       </c>
       <c r="I34" s="3">
@@ -3057,7 +3093,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="35" s="3" customFormat="1" spans="1:34">
+    <row r="35" s="3" customFormat="1" spans="1:36">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -3068,8 +3104,8 @@
         <v>50</v>
       </c>
       <c r="F35" s="8">
-        <f t="shared" si="1"/>
-        <v>27000</v>
+        <f t="shared" si="2"/>
+        <v>30000</v>
       </c>
       <c r="I35" s="3">
         <v>2000</v>
@@ -3093,6 +3129,9 @@
         <v>3000</v>
       </c>
       <c r="AH35" s="9">
+        <v>3000</v>
+      </c>
+      <c r="AJ35" s="9">
         <v>3000</v>
       </c>
     </row>
@@ -3107,7 +3146,7 @@
         <v>51</v>
       </c>
       <c r="F36" s="8">
-        <f t="shared" ref="F36:F68" si="2">SUM(G36:AK36)</f>
+        <f t="shared" ref="F36:F73" si="3">SUM(G36:AK36)</f>
         <v>4000</v>
       </c>
       <c r="W36" s="3">
@@ -3128,7 +3167,7 @@
         <v>52</v>
       </c>
       <c r="F37" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21000</v>
       </c>
       <c r="I37" s="9">
@@ -3164,7 +3203,7 @@
         <v>53</v>
       </c>
       <c r="F38" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9000</v>
       </c>
       <c r="K38" s="3">
@@ -3191,7 +3230,7 @@
         <v>54</v>
       </c>
       <c r="F39" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12000</v>
       </c>
       <c r="M39" s="3">
@@ -3221,7 +3260,7 @@
         <v>55</v>
       </c>
       <c r="F40" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11000</v>
       </c>
       <c r="I40" s="3">
@@ -3246,7 +3285,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="41" s="3" customFormat="1" spans="1:34">
+    <row r="41" s="3" customFormat="1" spans="1:36">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -3260,8 +3299,8 @@
         <v>56</v>
       </c>
       <c r="F41" s="8">
-        <f t="shared" si="2"/>
-        <v>33000</v>
+        <f t="shared" si="3"/>
+        <v>36000</v>
       </c>
       <c r="I41" s="3">
         <v>2000</v>
@@ -3291,6 +3330,9 @@
         <v>4000</v>
       </c>
       <c r="AH41" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AJ41" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -3305,7 +3347,7 @@
         <v>57</v>
       </c>
       <c r="F42" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5000</v>
       </c>
       <c r="L42" s="3">
@@ -3329,7 +3371,7 @@
         <v>58</v>
       </c>
       <c r="F43" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3344,7 +3386,7 @@
         <v>59</v>
       </c>
       <c r="F44" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21000</v>
       </c>
       <c r="I44" s="9">
@@ -3380,7 +3422,7 @@
         <v>61</v>
       </c>
       <c r="F45" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23000</v>
       </c>
       <c r="J45" s="3">
@@ -3413,7 +3455,7 @@
         <v>62</v>
       </c>
       <c r="F46" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22000</v>
       </c>
       <c r="J46" s="3">
@@ -3455,7 +3497,7 @@
         <v>64</v>
       </c>
       <c r="F47" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6000</v>
       </c>
       <c r="J47" s="9">
@@ -3482,7 +3524,7 @@
         <v>65</v>
       </c>
       <c r="F48" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14000</v>
       </c>
       <c r="P48" s="3">
@@ -3501,7 +3543,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="49" s="3" customFormat="1" spans="1:30">
+    <row r="49" s="3" customFormat="1" spans="1:36">
       <c r="A49" s="3">
         <v>47</v>
       </c>
@@ -3518,8 +3560,8 @@
         <v>67</v>
       </c>
       <c r="F49" s="8">
-        <f t="shared" si="2"/>
-        <v>21000</v>
+        <f t="shared" si="3"/>
+        <v>24000</v>
       </c>
       <c r="J49" s="9">
         <v>2000</v>
@@ -3541,6 +3583,9 @@
       </c>
       <c r="AD49" s="9">
         <v>6000</v>
+      </c>
+      <c r="AJ49" s="9">
+        <v>3000</v>
       </c>
     </row>
     <row r="50" s="3" customFormat="1" spans="1:28">
@@ -3557,7 +3602,7 @@
         <v>69</v>
       </c>
       <c r="F50" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9000</v>
       </c>
       <c r="J50" s="3">
@@ -3587,7 +3632,7 @@
         <v>70</v>
       </c>
       <c r="F51" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8000</v>
       </c>
       <c r="J51" s="3">
@@ -3617,7 +3662,7 @@
         <v>72</v>
       </c>
       <c r="F52" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22000</v>
       </c>
       <c r="J52" s="9">
@@ -3656,7 +3701,7 @@
         <v>73</v>
       </c>
       <c r="F53" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="AC53" s="3">
@@ -3677,7 +3722,7 @@
         <v>75</v>
       </c>
       <c r="F54" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9000</v>
       </c>
       <c r="R54" s="3">
@@ -3704,7 +3749,7 @@
         <v>76</v>
       </c>
       <c r="F55" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>33000</v>
       </c>
       <c r="O55" s="3">
@@ -3740,7 +3785,7 @@
         <v>77</v>
       </c>
       <c r="F56" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9500</v>
       </c>
       <c r="M56" s="3">
@@ -3773,7 +3818,7 @@
         <v>80</v>
       </c>
       <c r="F57" s="8">
-        <f>SUM(G57:AK57)</f>
+        <f t="shared" si="3"/>
         <v>5000</v>
       </c>
       <c r="AH57" s="9">
@@ -3794,7 +3839,7 @@
         <v>82</v>
       </c>
       <c r="F58" s="8">
-        <f>SUM(G58:AK58)</f>
+        <f t="shared" si="3"/>
         <v>9000</v>
       </c>
       <c r="P58" s="9">
@@ -3818,7 +3863,7 @@
         <v>85</v>
       </c>
       <c r="F59" s="8">
-        <f>SUM(G59:AK59)</f>
+        <f t="shared" si="3"/>
         <v>14000</v>
       </c>
       <c r="K59" s="3">
@@ -3854,7 +3899,7 @@
         <v>87</v>
       </c>
       <c r="F60" s="8">
-        <f>SUM(G60:AK60)</f>
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="W60" s="3">
@@ -3875,7 +3920,7 @@
         <v>89</v>
       </c>
       <c r="F61" s="8">
-        <f>SUM(G61:AK61)</f>
+        <f t="shared" si="3"/>
         <v>9000</v>
       </c>
       <c r="Q61" s="3">
@@ -3899,7 +3944,7 @@
         <v>90</v>
       </c>
       <c r="F62" s="8">
-        <f>SUM(G62:AK62)</f>
+        <f t="shared" si="3"/>
         <v>11000</v>
       </c>
       <c r="K62" s="3">
@@ -3929,7 +3974,7 @@
         <v>91</v>
       </c>
       <c r="F63" s="8">
-        <f>SUM(G63:AK63)</f>
+        <f t="shared" si="3"/>
         <v>5000</v>
       </c>
       <c r="K63" s="3">
@@ -3953,7 +3998,7 @@
         <v>92</v>
       </c>
       <c r="F64" s="8">
-        <f>SUM(G64:AK64)</f>
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="K64" s="3">
@@ -3977,7 +4022,7 @@
         <v>93</v>
       </c>
       <c r="F65" s="8">
-        <f>SUM(G65:AK65)</f>
+        <f t="shared" si="3"/>
         <v>52000</v>
       </c>
       <c r="K65" s="3">
@@ -4019,7 +4064,7 @@
         <v>94</v>
       </c>
       <c r="F66" s="8">
-        <f>SUM(G66:AK66)</f>
+        <f t="shared" si="3"/>
         <v>24000</v>
       </c>
       <c r="L66" s="9">
@@ -4058,7 +4103,7 @@
         <v>95</v>
       </c>
       <c r="F67" s="8">
-        <f>SUM(G67:AK67)</f>
+        <f t="shared" si="3"/>
         <v>6000</v>
       </c>
       <c r="X67" s="3">
@@ -4079,7 +4124,7 @@
         <v>96</v>
       </c>
       <c r="F68" s="8">
-        <f>SUM(G68:AK68)</f>
+        <f t="shared" si="3"/>
         <v>3000</v>
       </c>
       <c r="Y68" s="3">
@@ -4092,7 +4137,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="69" s="3" customFormat="1" spans="1:31">
+    <row r="69" s="3" customFormat="1" spans="1:36">
       <c r="A69" s="3">
         <v>67</v>
       </c>
@@ -4106,8 +4151,8 @@
         <v>98</v>
       </c>
       <c r="F69" s="8">
-        <f>SUM(G69:AK69)</f>
-        <v>15000</v>
+        <f t="shared" si="3"/>
+        <v>16500</v>
       </c>
       <c r="J69" s="9">
         <v>1000</v>
@@ -4135,6 +4180,9 @@
       </c>
       <c r="AE69" s="9">
         <v>2200</v>
+      </c>
+      <c r="AJ69" s="3">
+        <v>1500</v>
       </c>
     </row>
     <row r="70" s="3" customFormat="1" spans="1:35">
@@ -4148,7 +4196,7 @@
         <v>99</v>
       </c>
       <c r="F70" s="8">
-        <f>SUM(G70:AK70)</f>
+        <f t="shared" si="3"/>
         <v>27000</v>
       </c>
       <c r="K70" s="9">
@@ -4179,19 +4227,22 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="71" s="3" customFormat="1" spans="1:31">
+    <row r="71" s="3" customFormat="1" spans="1:36">
       <c r="A71" s="3">
         <v>69</v>
       </c>
+      <c r="B71" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="D71" s="3" t="s">
         <v>97</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F71" s="8">
-        <f>SUM(G71:AK71)</f>
-        <v>17000</v>
+        <f t="shared" si="3"/>
+        <v>19000</v>
       </c>
       <c r="J71" s="3">
         <v>2000</v>
@@ -4215,6 +4266,9 @@
         <v>4000</v>
       </c>
       <c r="AE71" s="9">
+        <v>2000</v>
+      </c>
+      <c r="AJ71" s="9">
         <v>2000</v>
       </c>
     </row>
@@ -4223,10 +4277,10 @@
         <v>70</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F72" s="8">
-        <f>SUM(G72:AK72)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -4235,16 +4289,16 @@
         <v>71</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F73" s="8">
-        <f>SUM(G73:AK73)</f>
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="Q73" s="9">
@@ -4259,10 +4313,10 @@
         <v>72</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F74" s="8">
-        <f t="shared" ref="F69:F94" si="3">SUM(G74:AK74)</f>
+        <f t="shared" ref="F69:F94" si="4">SUM(G74:AK74)</f>
         <v>0</v>
       </c>
     </row>
@@ -4271,13 +4325,13 @@
         <v>73</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F75" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3000</v>
       </c>
       <c r="AH75" s="9">
@@ -4289,10 +4343,10 @@
         <v>74</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F76" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4304,10 +4358,10 @@
         <v>30</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F77" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3000</v>
       </c>
       <c r="AE77" s="9">
@@ -4319,10 +4373,10 @@
         <v>76</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F78" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4331,10 +4385,10 @@
         <v>77</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F79" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4343,10 +4397,10 @@
         <v>78</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F80" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4355,10 +4409,10 @@
         <v>79</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F81" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4367,13 +4421,13 @@
         <v>80</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F82" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13000</v>
       </c>
       <c r="AB82" s="9">
@@ -4394,10 +4448,10 @@
         <v>81</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F83" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4406,10 +4460,10 @@
         <v>82</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F84" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4418,16 +4472,16 @@
         <v>83</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F85" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2000</v>
       </c>
       <c r="AB85" s="9">
@@ -4439,10 +4493,10 @@
         <v>84</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F86" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4451,10 +4505,10 @@
         <v>85</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F87" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4463,10 +4517,10 @@
         <v>86</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F88" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4475,10 +4529,10 @@
         <v>87</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F89" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4487,10 +4541,10 @@
         <v>88</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F90" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4499,10 +4553,10 @@
         <v>89</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F91" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4511,10 +4565,10 @@
         <v>90</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F92" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4523,10 +4577,10 @@
         <v>91</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F93" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4535,10 +4589,10 @@
         <v>92</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F94" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data updated till 31 Dec 11PM
</commit_message>
<xml_diff>
--- a/Daily Collection/December-2020-Collection.xlsx
+++ b/Daily Collection/December-2020-Collection.xlsx
@@ -234,7 +234,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="131">
   <si>
     <t>S.No.</t>
   </si>
@@ -429,6 +429,9 @@
   </si>
   <si>
     <t>KUMAR INTERNET(660322625)</t>
+  </si>
+  <si>
+    <t>Sanjeev Kr.</t>
   </si>
   <si>
     <t>PRITI MOBILE CENTRE(660297509)</t>
@@ -631,11 +634,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -668,16 +671,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -693,14 +696,22 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -715,22 +726,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -754,30 +758,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -792,18 +773,40 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
@@ -842,13 +845,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -860,13 +953,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -878,151 +1025,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1036,35 +1039,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1108,6 +1093,39 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1118,35 +1136,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1156,130 +1159,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1299,7 +1302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1644,11 +1647,11 @@
   <dimension ref="A1:AK94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="AC51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="AD20" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AJ71" sqref="AJ71"/>
+      <selection pane="bottomRight" activeCell="AK29" sqref="AK29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1777,14 +1780,14 @@
     <row r="2" s="2" customFormat="1" spans="4:37">
       <c r="D2" s="6">
         <f>SUM(F3:F119)</f>
-        <v>1132500</v>
+        <v>1182000</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="6">
         <f t="shared" ref="F2:F16" si="0">SUM(G2:AK2)</f>
-        <v>1132500</v>
+        <v>1182000</v>
       </c>
       <c r="G2" s="2">
         <f>SUM(G3:G120)</f>
@@ -1908,13 +1911,16 @@
       </c>
       <c r="AK2" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>49500</v>
       </c>
     </row>
     <row r="3" s="3" customFormat="1" spans="1:29">
       <c r="A3" s="3">
         <v>1</v>
       </c>
+      <c r="C3" s="3">
+        <v>9334066332</v>
+      </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1956,10 +1962,13 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" s="3" customFormat="1" spans="1:35">
+    <row r="5" s="3" customFormat="1" spans="1:37">
       <c r="A5" s="3">
         <v>3</v>
       </c>
+      <c r="C5" s="3">
+        <v>8340365412</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1968,7 +1977,7 @@
       </c>
       <c r="F5" s="8">
         <f t="shared" si="0"/>
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="I5" s="3">
         <v>1000</v>
@@ -2000,11 +2009,17 @@
       <c r="AI5" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="6" s="3" customFormat="1" spans="1:33">
+      <c r="AK5" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" s="3" customFormat="1" spans="1:37">
       <c r="A6" s="3">
         <v>4</v>
       </c>
+      <c r="C6" s="3">
+        <v>9102317719</v>
+      </c>
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
@@ -2013,7 +2028,7 @@
       </c>
       <c r="F6" s="8">
         <f t="shared" si="0"/>
-        <v>24500</v>
+        <v>26500</v>
       </c>
       <c r="I6" s="9">
         <v>3000</v>
@@ -2042,11 +2057,17 @@
       <c r="AG6" s="9">
         <v>3000</v>
       </c>
-    </row>
-    <row r="7" s="3" customFormat="1" spans="1:35">
+      <c r="AK6" s="9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" s="3" customFormat="1" spans="1:37">
       <c r="A7" s="3">
         <v>5</v>
       </c>
+      <c r="C7" s="3">
+        <v>8210924561</v>
+      </c>
       <c r="D7" s="3" t="s">
         <v>7</v>
       </c>
@@ -2055,7 +2076,7 @@
       </c>
       <c r="F7" s="8">
         <f t="shared" si="0"/>
-        <v>46000</v>
+        <v>56000</v>
       </c>
       <c r="I7" s="3">
         <v>2000</v>
@@ -2093,11 +2114,17 @@
       <c r="AI7" s="9">
         <v>5000</v>
       </c>
-    </row>
-    <row r="8" s="3" customFormat="1" spans="1:24">
+      <c r="AK7" s="3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="8" s="3" customFormat="1" spans="1:37">
       <c r="A8" s="3">
         <v>6</v>
       </c>
+      <c r="C8" s="3">
+        <v>9110978139</v>
+      </c>
       <c r="D8" s="3" t="s">
         <v>7</v>
       </c>
@@ -2106,7 +2133,7 @@
       </c>
       <c r="F8" s="8">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="O8" s="3">
         <v>1000</v>
@@ -2115,6 +2142,9 @@
         <v>2000</v>
       </c>
       <c r="X8" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AK8" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -2122,6 +2152,9 @@
       <c r="A9" s="3">
         <v>7</v>
       </c>
+      <c r="C9" s="3">
+        <v>8340201321</v>
+      </c>
       <c r="D9" s="3" t="s">
         <v>7</v>
       </c>
@@ -2148,10 +2181,13 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" s="3" customFormat="1" spans="1:33">
+    <row r="10" s="3" customFormat="1" spans="1:37">
       <c r="A10" s="3">
         <v>8</v>
       </c>
+      <c r="C10" s="3">
+        <v>7004365158</v>
+      </c>
       <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
@@ -2160,7 +2196,7 @@
       </c>
       <c r="F10" s="8">
         <f t="shared" si="0"/>
-        <v>40000</v>
+        <v>45000</v>
       </c>
       <c r="I10" s="3">
         <v>2000</v>
@@ -2187,6 +2223,9 @@
         <v>5000</v>
       </c>
       <c r="AG10" s="3">
+        <v>5000</v>
+      </c>
+      <c r="AK10" s="3">
         <v>5000</v>
       </c>
     </row>
@@ -2197,6 +2236,9 @@
       <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="C11" s="3">
+        <v>9973022718</v>
+      </c>
       <c r="D11" s="3" t="s">
         <v>17</v>
       </c>
@@ -2266,6 +2308,9 @@
       <c r="A13" s="3">
         <v>11</v>
       </c>
+      <c r="C13" s="3">
+        <v>8340182577</v>
+      </c>
       <c r="D13" s="3" t="s">
         <v>17</v>
       </c>
@@ -2298,10 +2343,13 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="14" s="3" customFormat="1" spans="1:36">
+    <row r="14" s="3" customFormat="1" spans="1:37">
       <c r="A14" s="3">
         <v>12</v>
       </c>
+      <c r="C14" s="3">
+        <v>7004740439</v>
+      </c>
       <c r="D14" s="3" t="s">
         <v>17</v>
       </c>
@@ -2310,7 +2358,7 @@
       </c>
       <c r="F14" s="8">
         <f t="shared" si="0"/>
-        <v>47500</v>
+        <v>49000</v>
       </c>
       <c r="I14" s="3">
         <v>2000</v>
@@ -2375,8 +2423,11 @@
       <c r="AJ14" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="15" s="3" customFormat="1" spans="1:35">
+      <c r="AK14" s="3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="15" s="3" customFormat="1" spans="1:37">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -2391,7 +2442,7 @@
       </c>
       <c r="F15" s="8">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>10000</v>
       </c>
       <c r="T15" s="3">
         <v>2000</v>
@@ -2405,8 +2456,11 @@
       <c r="AI15" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="16" spans="1:34">
+      <c r="AK15" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -2421,10 +2475,13 @@
       </c>
       <c r="F16" s="8">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="AH16" s="9">
         <v>2000</v>
+      </c>
+      <c r="AK16" s="3">
+        <v>500</v>
       </c>
     </row>
     <row r="17" s="3" customFormat="1" spans="1:35">
@@ -2470,6 +2527,9 @@
       <c r="A18" s="3">
         <v>16</v>
       </c>
+      <c r="C18" s="3">
+        <v>9661555592</v>
+      </c>
       <c r="D18" s="3" t="s">
         <v>28</v>
       </c>
@@ -2506,6 +2566,9 @@
       <c r="B19" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="C19" s="3">
+        <v>8340523512</v>
+      </c>
       <c r="D19" s="3" t="s">
         <v>28</v>
       </c>
@@ -2539,6 +2602,9 @@
       <c r="A20" s="3">
         <v>18</v>
       </c>
+      <c r="C20" s="3">
+        <v>8825310472</v>
+      </c>
       <c r="D20" s="3" t="s">
         <v>28</v>
       </c>
@@ -2578,6 +2644,9 @@
       <c r="A21" s="3">
         <v>19</v>
       </c>
+      <c r="C21" s="3">
+        <v>7004478123</v>
+      </c>
       <c r="D21" s="3" t="s">
         <v>28</v>
       </c>
@@ -2605,6 +2674,9 @@
       <c r="A22" s="3">
         <v>20</v>
       </c>
+      <c r="C22" s="3">
+        <v>7667895364</v>
+      </c>
       <c r="D22" s="3" t="s">
         <v>28</v>
       </c>
@@ -2641,6 +2713,9 @@
       <c r="A23" s="3">
         <v>21</v>
       </c>
+      <c r="C23" s="3">
+        <v>7006041121</v>
+      </c>
       <c r="D23" s="3" t="s">
         <v>28</v>
       </c>
@@ -2680,6 +2755,9 @@
       <c r="B24" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="C24" s="3">
+        <v>8709658240</v>
+      </c>
       <c r="D24" s="3" t="s">
         <v>28</v>
       </c>
@@ -2853,7 +2931,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="29" s="3" customFormat="1" spans="1:34">
+    <row r="29" s="3" customFormat="1" spans="1:37">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -2865,7 +2943,7 @@
       </c>
       <c r="F29" s="8">
         <f t="shared" si="2"/>
-        <v>22000</v>
+        <v>27000</v>
       </c>
       <c r="I29" s="9">
         <v>2000</v>
@@ -2886,6 +2964,9 @@
         <v>5000</v>
       </c>
       <c r="AH29" s="9">
+        <v>5000</v>
+      </c>
+      <c r="AK29" s="9">
         <v>5000</v>
       </c>
     </row>
@@ -3030,7 +3111,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="33" s="3" customFormat="1" spans="1:32">
+    <row r="33" s="3" customFormat="1" spans="1:37">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -3042,7 +3123,7 @@
       </c>
       <c r="F33" s="8">
         <f t="shared" si="2"/>
-        <v>6000</v>
+        <v>7000</v>
       </c>
       <c r="I33" s="3">
         <v>1000</v>
@@ -3060,6 +3141,9 @@
         <v>1000</v>
       </c>
       <c r="AF33" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AK33" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -3093,7 +3177,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="35" s="3" customFormat="1" spans="1:36">
+    <row r="35" s="3" customFormat="1" spans="1:37">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -3105,7 +3189,7 @@
       </c>
       <c r="F35" s="8">
         <f t="shared" si="2"/>
-        <v>30000</v>
+        <v>33000</v>
       </c>
       <c r="I35" s="3">
         <v>2000</v>
@@ -3132,6 +3216,9 @@
         <v>3000</v>
       </c>
       <c r="AJ35" s="9">
+        <v>3000</v>
+      </c>
+      <c r="AK35" s="9">
         <v>3000</v>
       </c>
     </row>
@@ -3510,10 +3597,13 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="48" s="3" customFormat="1" spans="1:30">
+    <row r="48" s="3" customFormat="1" spans="1:37">
       <c r="A48" s="3">
         <v>46</v>
       </c>
+      <c r="B48" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="C48" s="3">
         <v>8863097933</v>
       </c>
@@ -3521,11 +3611,11 @@
         <v>60</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F48" s="8">
         <f t="shared" si="3"/>
-        <v>14000</v>
+        <v>17000</v>
       </c>
       <c r="P48" s="3">
         <v>2000</v>
@@ -3540,6 +3630,9 @@
         <v>3000</v>
       </c>
       <c r="AD48" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AK48" s="9">
         <v>3000</v>
       </c>
     </row>
@@ -3548,7 +3641,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C49" s="3">
         <v>9835443096</v>
@@ -3557,7 +3650,7 @@
         <v>60</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F49" s="8">
         <f t="shared" si="3"/>
@@ -3593,13 +3686,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F50" s="8">
         <f t="shared" si="3"/>
@@ -3629,7 +3722,7 @@
         <v>60</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F51" s="8">
         <f t="shared" si="3"/>
@@ -3653,13 +3746,13 @@
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F52" s="8">
         <f t="shared" si="3"/>
@@ -3698,7 +3791,7 @@
         <v>60</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F53" s="8">
         <f t="shared" si="3"/>
@@ -3716,10 +3809,10 @@
         <v>52</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F54" s="8">
         <f t="shared" si="3"/>
@@ -3738,19 +3831,19 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="55" s="3" customFormat="1" spans="1:34">
+    <row r="55" s="3" customFormat="1" spans="1:37">
       <c r="A55" s="3">
         <v>53</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F55" s="8">
         <f t="shared" si="3"/>
-        <v>33000</v>
+        <v>38000</v>
       </c>
       <c r="O55" s="3">
         <v>8000</v>
@@ -3771,6 +3864,9 @@
         <v>5000</v>
       </c>
       <c r="AH55" s="3">
+        <v>5000</v>
+      </c>
+      <c r="AK55" s="3">
         <v>5000</v>
       </c>
     </row>
@@ -3779,10 +3875,10 @@
         <v>54</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F56" s="8">
         <f t="shared" si="3"/>
@@ -3809,13 +3905,13 @@
         <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F57" s="8">
         <f t="shared" si="3"/>
@@ -3830,13 +3926,13 @@
         <v>56</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F58" s="8">
         <f t="shared" si="3"/>
@@ -3854,13 +3950,13 @@
         <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F59" s="8">
         <f t="shared" si="3"/>
@@ -3893,10 +3989,10 @@
         <v>58</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F60" s="8">
         <f t="shared" si="3"/>
@@ -3909,19 +4005,19 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="61" s="3" customFormat="1" spans="1:28">
+    <row r="61" s="3" customFormat="1" spans="1:37">
       <c r="A61" s="3">
         <v>59</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F61" s="8">
         <f t="shared" si="3"/>
-        <v>9000</v>
+        <v>13000</v>
       </c>
       <c r="Q61" s="3">
         <v>5000</v>
@@ -3931,6 +4027,9 @@
       </c>
       <c r="AB61" s="3">
         <v>2000</v>
+      </c>
+      <c r="AK61" s="3">
+        <v>4000</v>
       </c>
     </row>
     <row r="62" s="3" customFormat="1" spans="1:35">
@@ -3938,10 +4037,10 @@
         <v>60</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F62" s="8">
         <f t="shared" si="3"/>
@@ -3963,19 +4062,19 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="63" s="3" customFormat="1" spans="1:26">
+    <row r="63" s="3" customFormat="1" spans="1:37">
       <c r="A63" s="3">
         <v>61</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F63" s="8">
         <f t="shared" si="3"/>
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="K63" s="3">
         <v>1000</v>
@@ -3984,6 +4083,9 @@
         <v>2000</v>
       </c>
       <c r="Z63" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AK63" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -3992,10 +4094,10 @@
         <v>62</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F64" s="8">
         <f t="shared" si="3"/>
@@ -4016,10 +4118,10 @@
         <v>63</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F65" s="8">
         <f t="shared" si="3"/>
@@ -4058,10 +4160,10 @@
         <v>64</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F66" s="8">
         <f t="shared" si="3"/>
@@ -4097,10 +4199,10 @@
         <v>65</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F67" s="8">
         <f t="shared" si="3"/>
@@ -4113,19 +4215,19 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="68" s="3" customFormat="1" spans="1:31">
+    <row r="68" s="3" customFormat="1" spans="1:37">
       <c r="A68" s="3">
         <v>66</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F68" s="8">
         <f t="shared" si="3"/>
-        <v>3000</v>
+        <v>3500</v>
       </c>
       <c r="Y68" s="3">
         <v>1500</v>
@@ -4135,6 +4237,9 @@
       </c>
       <c r="AE68" s="3">
         <v>1000</v>
+      </c>
+      <c r="AK68" s="3">
+        <v>500</v>
       </c>
     </row>
     <row r="69" s="3" customFormat="1" spans="1:36">
@@ -4145,10 +4250,10 @@
         <v>6200769032</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F69" s="8">
         <f t="shared" si="3"/>
@@ -4190,10 +4295,10 @@
         <v>68</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F70" s="8">
         <f t="shared" si="3"/>
@@ -4232,13 +4337,13 @@
         <v>69</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F71" s="8">
         <f t="shared" si="3"/>
@@ -4277,34 +4382,37 @@
         <v>70</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F72" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="73" s="3" customFormat="1" spans="1:28">
+    <row r="73" s="3" customFormat="1" spans="1:37">
       <c r="A73" s="3">
         <v>71</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F73" s="8">
         <f t="shared" si="3"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="Q73" s="9">
         <v>2000</v>
       </c>
       <c r="AB73" s="9">
+        <v>2000</v>
+      </c>
+      <c r="AK73" s="9">
         <v>2000</v>
       </c>
     </row>
@@ -4313,7 +4421,7 @@
         <v>72</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F74" s="8">
         <f t="shared" ref="F69:F94" si="4">SUM(G74:AK74)</f>
@@ -4325,10 +4433,10 @@
         <v>73</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F75" s="8">
         <f t="shared" si="4"/>
@@ -4343,7 +4451,7 @@
         <v>74</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F76" s="8">
         <f t="shared" si="4"/>
@@ -4358,7 +4466,7 @@
         <v>30</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F77" s="8">
         <f t="shared" si="4"/>
@@ -4373,7 +4481,7 @@
         <v>76</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F78" s="8">
         <f t="shared" si="4"/>
@@ -4385,7 +4493,7 @@
         <v>77</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F79" s="8">
         <f t="shared" si="4"/>
@@ -4397,7 +4505,7 @@
         <v>78</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F80" s="8">
         <f t="shared" si="4"/>
@@ -4409,7 +4517,7 @@
         <v>79</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F81" s="8">
         <f t="shared" si="4"/>
@@ -4421,10 +4529,10 @@
         <v>80</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F82" s="8">
         <f t="shared" si="4"/>
@@ -4448,7 +4556,7 @@
         <v>81</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F83" s="8">
         <f t="shared" si="4"/>
@@ -4460,7 +4568,7 @@
         <v>82</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F84" s="8">
         <f t="shared" si="4"/>
@@ -4472,13 +4580,13 @@
         <v>83</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F85" s="8">
         <f t="shared" si="4"/>
@@ -4493,7 +4601,7 @@
         <v>84</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F86" s="8">
         <f t="shared" si="4"/>
@@ -4505,7 +4613,7 @@
         <v>85</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F87" s="8">
         <f t="shared" si="4"/>
@@ -4517,7 +4625,7 @@
         <v>86</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F88" s="8">
         <f t="shared" si="4"/>
@@ -4529,7 +4637,7 @@
         <v>87</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F89" s="8">
         <f t="shared" si="4"/>
@@ -4541,7 +4649,7 @@
         <v>88</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F90" s="8">
         <f t="shared" si="4"/>
@@ -4553,7 +4661,7 @@
         <v>89</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F91" s="8">
         <f t="shared" si="4"/>
@@ -4565,7 +4673,7 @@
         <v>90</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F92" s="8">
         <f t="shared" si="4"/>
@@ -4577,7 +4685,7 @@
         <v>91</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F93" s="8">
         <f t="shared" si="4"/>
@@ -4589,7 +4697,7 @@
         <v>92</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F94" s="8">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
data updated till 6Jan 9AM
</commit_message>
<xml_diff>
--- a/Daily Collection/December-2020-Collection.xlsx
+++ b/Daily Collection/December-2020-Collection.xlsx
@@ -234,7 +234,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="135">
   <si>
     <t>S.No.</t>
   </si>
@@ -257,6 +257,9 @@
     <t>Total:</t>
   </si>
   <si>
+    <t>Sanjeev Kr. Rahi</t>
+  </si>
+  <si>
     <t>AGNOOR</t>
   </si>
   <si>
@@ -269,6 +272,9 @@
     <t>MAHI TELECOM ELECTRONICS(661644706)</t>
   </si>
   <si>
+    <t>Ganesh Lal Khatri</t>
+  </si>
+  <si>
     <t>ARVIND AIRTEL EGRECHARGE CENTR(661591709)</t>
   </si>
   <si>
@@ -335,6 +341,9 @@
     <t>ANIL PAN DUKAN(661705269)</t>
   </si>
   <si>
+    <t>Aarti 9523733118</t>
+  </si>
+  <si>
     <t>MAA VINDHWASHNI COMMUNICATION(660301564)</t>
   </si>
   <si>
@@ -344,7 +353,7 @@
     <t>Maa Bhindwashni Mobile Center(660587310)</t>
   </si>
   <si>
-    <t>Santnu Kr.</t>
+    <t>Shantnu Kr.</t>
   </si>
   <si>
     <t>MS RIYA ENTERPRISES(661562283)</t>
@@ -392,6 +401,9 @@
     <t>Kaler Electronics(660628532)</t>
   </si>
   <si>
+    <t>Sonu Kr.</t>
+  </si>
+  <si>
     <t>MS OM COMPUTER(661542289)</t>
   </si>
   <si>
@@ -473,7 +485,7 @@
     <t>KALER ENTERPRISES(661674410)</t>
   </si>
   <si>
-    <t>Ranjeet Kr.</t>
+    <t>Ranjit Kr. 9504958065</t>
   </si>
   <si>
     <t>BADRABAD</t>
@@ -634,11 +646,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -657,6 +669,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -671,16 +691,37 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -688,22 +729,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -718,6 +744,14 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -725,16 +759,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -750,17 +783,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -773,7 +799,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -782,20 +808,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -845,7 +857,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -857,13 +995,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -875,157 +1037,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1040,6 +1052,39 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1049,6 +1094,21 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1078,54 +1138,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1141,15 +1153,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1159,134 +1171,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1302,7 +1314,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1310,6 +1322,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1647,11 +1662,11 @@
   <dimension ref="A1:AK94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="AD20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="T32" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AK29" sqref="AK29"/>
+      <selection pane="bottomRight" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1918,23 +1933,26 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
+      <c r="B3" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="C3" s="3">
         <v>9334066332</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="8">
+        <v>9</v>
+      </c>
+      <c r="F3" s="9">
         <f t="shared" si="0"/>
         <v>6000</v>
       </c>
-      <c r="V3" s="9">
-        <v>3000</v>
-      </c>
-      <c r="AC3" s="9">
+      <c r="V3" s="10">
+        <v>3000</v>
+      </c>
+      <c r="AC3" s="10">
         <v>3000</v>
       </c>
     </row>
@@ -1943,22 +1961,22 @@
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="8">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9">
         <f t="shared" si="0"/>
         <v>6000</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="10">
         <v>2000</v>
       </c>
       <c r="AC4" s="3">
         <v>2000</v>
       </c>
-      <c r="AG4" s="9">
+      <c r="AG4" s="10">
         <v>2000</v>
       </c>
     </row>
@@ -1970,12 +1988,12 @@
         <v>8340365412</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="8">
+        <v>11</v>
+      </c>
+      <c r="F5" s="9">
         <f t="shared" si="0"/>
         <v>15000</v>
       </c>
@@ -2017,47 +2035,50 @@
       <c r="A6" s="3">
         <v>4</v>
       </c>
+      <c r="B6" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="C6" s="3">
         <v>9102317719</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="8">
+        <v>13</v>
+      </c>
+      <c r="F6" s="9">
         <f t="shared" si="0"/>
         <v>26500</v>
       </c>
-      <c r="I6" s="9">
-        <v>3000</v>
-      </c>
-      <c r="K6" s="9">
-        <v>2000</v>
-      </c>
-      <c r="L6" s="9">
+      <c r="I6" s="10">
+        <v>3000</v>
+      </c>
+      <c r="K6" s="10">
+        <v>2000</v>
+      </c>
+      <c r="L6" s="10">
         <v>1500</v>
       </c>
-      <c r="O6" s="9">
+      <c r="O6" s="10">
         <v>4000</v>
       </c>
-      <c r="P6" s="9">
+      <c r="P6" s="10">
         <v>4000</v>
       </c>
-      <c r="V6" s="9">
-        <v>2000</v>
-      </c>
-      <c r="Y6" s="9">
-        <v>3000</v>
-      </c>
-      <c r="AC6" s="9">
-        <v>2000</v>
-      </c>
-      <c r="AG6" s="9">
-        <v>3000</v>
-      </c>
-      <c r="AK6" s="9">
+      <c r="V6" s="10">
+        <v>2000</v>
+      </c>
+      <c r="Y6" s="10">
+        <v>3000</v>
+      </c>
+      <c r="AC6" s="10">
+        <v>2000</v>
+      </c>
+      <c r="AG6" s="10">
+        <v>3000</v>
+      </c>
+      <c r="AK6" s="10">
         <v>2000</v>
       </c>
     </row>
@@ -2069,49 +2090,49 @@
         <v>8210924561</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="8">
+        <v>14</v>
+      </c>
+      <c r="F7" s="9">
         <f t="shared" si="0"/>
         <v>56000</v>
       </c>
       <c r="I7" s="3">
         <v>2000</v>
       </c>
-      <c r="O7" s="9">
+      <c r="O7" s="10">
         <v>6000</v>
       </c>
-      <c r="P7" s="9">
-        <v>5000</v>
-      </c>
-      <c r="R7" s="9">
+      <c r="P7" s="10">
+        <v>5000</v>
+      </c>
+      <c r="R7" s="10">
         <v>1500</v>
       </c>
-      <c r="T7" s="9">
+      <c r="T7" s="10">
         <v>4500</v>
       </c>
       <c r="V7" s="3">
         <v>1500</v>
       </c>
-      <c r="W7" s="9">
+      <c r="W7" s="10">
         <v>3500</v>
       </c>
       <c r="Y7" s="3">
         <v>5000</v>
       </c>
-      <c r="AB7" s="9">
+      <c r="AB7" s="10">
         <v>6000</v>
       </c>
-      <c r="AD7" s="9">
+      <c r="AD7" s="10">
         <v>4000</v>
       </c>
-      <c r="AG7" s="9">
-        <v>2000</v>
-      </c>
-      <c r="AI7" s="9">
+      <c r="AG7" s="10">
+        <v>2000</v>
+      </c>
+      <c r="AI7" s="10">
         <v>5000</v>
       </c>
       <c r="AK7" s="3">
@@ -2126,12 +2147,12 @@
         <v>9110978139</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="8">
+        <v>15</v>
+      </c>
+      <c r="F8" s="9">
         <f t="shared" si="0"/>
         <v>7000</v>
       </c>
@@ -2156,12 +2177,12 @@
         <v>8340201321</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="8">
+        <v>16</v>
+      </c>
+      <c r="F9" s="9">
         <f t="shared" si="0"/>
         <v>8000</v>
       </c>
@@ -2189,12 +2210,12 @@
         <v>7004365158</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="8">
+        <v>17</v>
+      </c>
+      <c r="F10" s="9">
         <f t="shared" si="0"/>
         <v>45000</v>
       </c>
@@ -2234,34 +2255,34 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C11" s="3">
         <v>9973022718</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="8">
+        <v>20</v>
+      </c>
+      <c r="F11" s="9">
         <f t="shared" si="0"/>
         <v>13000</v>
       </c>
-      <c r="I11" s="9">
-        <v>2000</v>
-      </c>
-      <c r="L11" s="9">
-        <v>2000</v>
-      </c>
-      <c r="O11" s="9">
-        <v>5000</v>
-      </c>
-      <c r="W11" s="9">
-        <v>2000</v>
-      </c>
-      <c r="AF11" s="9">
+      <c r="I11" s="10">
+        <v>2000</v>
+      </c>
+      <c r="L11" s="10">
+        <v>2000</v>
+      </c>
+      <c r="O11" s="10">
+        <v>5000</v>
+      </c>
+      <c r="W11" s="10">
+        <v>2000</v>
+      </c>
+      <c r="AF11" s="10">
         <v>2000</v>
       </c>
     </row>
@@ -2270,12 +2291,12 @@
         <v>10</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="8">
+        <v>21</v>
+      </c>
+      <c r="F12" s="9">
         <f t="shared" si="0"/>
         <v>7000</v>
       </c>
@@ -2312,19 +2333,19 @@
         <v>8340182577</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="8">
+        <v>22</v>
+      </c>
+      <c r="F13" s="9">
         <f t="shared" si="0"/>
         <v>33000</v>
       </c>
       <c r="I13" s="3">
         <v>2000</v>
       </c>
-      <c r="M13" s="9">
+      <c r="M13" s="10">
         <v>6000</v>
       </c>
       <c r="O13" s="3">
@@ -2339,7 +2360,7 @@
       <c r="AE13" s="3">
         <v>5000</v>
       </c>
-      <c r="AJ13" s="9">
+      <c r="AJ13" s="10">
         <v>5000</v>
       </c>
     </row>
@@ -2351,12 +2372,12 @@
         <v>7004740439</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="8">
+        <v>23</v>
+      </c>
+      <c r="F14" s="9">
         <f t="shared" si="0"/>
         <v>49000</v>
       </c>
@@ -2432,15 +2453,15 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="8">
+        <v>25</v>
+      </c>
+      <c r="F15" s="9">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
@@ -2465,19 +2486,19 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="8">
+        <v>27</v>
+      </c>
+      <c r="F16" s="9">
         <f t="shared" si="0"/>
         <v>2500</v>
       </c>
-      <c r="AH16" s="9">
+      <c r="AH16" s="10">
         <v>2000</v>
       </c>
       <c r="AK16" s="3">
@@ -2489,15 +2510,15 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="8">
+        <v>29</v>
+      </c>
+      <c r="F17" s="9">
         <f t="shared" ref="F17:F35" si="2">SUM(G17:AK17)</f>
         <v>18000</v>
       </c>
@@ -2519,7 +2540,7 @@
       <c r="AD17" s="3">
         <v>3000</v>
       </c>
-      <c r="AI17" s="9">
+      <c r="AI17" s="10">
         <v>3000</v>
       </c>
     </row>
@@ -2531,12 +2552,12 @@
         <v>9661555592</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="8">
+        <v>31</v>
+      </c>
+      <c r="F18" s="9">
         <f t="shared" si="2"/>
         <v>29000</v>
       </c>
@@ -2546,16 +2567,16 @@
       <c r="M18" s="3">
         <v>6000</v>
       </c>
-      <c r="O18" s="9">
-        <v>5000</v>
-      </c>
-      <c r="T18" s="9">
+      <c r="O18" s="10">
+        <v>5000</v>
+      </c>
+      <c r="T18" s="10">
         <v>5000</v>
       </c>
       <c r="AD18" s="3">
         <v>5000</v>
       </c>
-      <c r="AJ18" s="9">
+      <c r="AJ18" s="10">
         <v>5000</v>
       </c>
     </row>
@@ -2564,34 +2585,34 @@
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C19" s="3">
         <v>8340523512</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="8">
+        <v>33</v>
+      </c>
+      <c r="F19" s="9">
         <f t="shared" si="2"/>
         <v>9000</v>
       </c>
-      <c r="T19" s="9">
-        <v>1000</v>
-      </c>
-      <c r="X19" s="9">
-        <v>1000</v>
-      </c>
-      <c r="Y19" s="9">
+      <c r="T19" s="10">
+        <v>1000</v>
+      </c>
+      <c r="X19" s="10">
+        <v>1000</v>
+      </c>
+      <c r="Y19" s="10">
         <v>1000</v>
       </c>
       <c r="AC19" s="3">
         <v>2000</v>
       </c>
-      <c r="AD19" s="9">
+      <c r="AD19" s="10">
         <v>2000</v>
       </c>
       <c r="AI19" s="3">
@@ -2606,12 +2627,12 @@
         <v>8825310472</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" s="8">
+        <v>34</v>
+      </c>
+      <c r="F20" s="9">
         <f t="shared" si="2"/>
         <v>12000</v>
       </c>
@@ -2644,29 +2665,32 @@
       <c r="A21" s="3">
         <v>19</v>
       </c>
+      <c r="B21" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="C21" s="3">
         <v>7004478123</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="8">
+        <v>36</v>
+      </c>
+      <c r="F21" s="9">
         <f t="shared" si="2"/>
         <v>22000</v>
       </c>
-      <c r="Q21" s="9">
-        <v>5000</v>
-      </c>
-      <c r="U21" s="9">
+      <c r="Q21" s="10">
+        <v>5000</v>
+      </c>
+      <c r="U21" s="10">
         <v>7000</v>
       </c>
-      <c r="Y21" s="9">
-        <v>5000</v>
-      </c>
-      <c r="AG21" s="9">
+      <c r="Y21" s="10">
+        <v>5000</v>
+      </c>
+      <c r="AG21" s="10">
         <v>5000</v>
       </c>
     </row>
@@ -2678,12 +2702,12 @@
         <v>7667895364</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="8">
+        <v>37</v>
+      </c>
+      <c r="F22" s="9">
         <f t="shared" si="2"/>
         <v>9000</v>
       </c>
@@ -2717,12 +2741,12 @@
         <v>7006041121</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="8">
+        <v>38</v>
+      </c>
+      <c r="F23" s="9">
         <f t="shared" si="2"/>
         <v>21000</v>
       </c>
@@ -2753,34 +2777,34 @@
         <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C24" s="3">
         <v>8709658240</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="8">
+        <v>40</v>
+      </c>
+      <c r="F24" s="9">
         <f t="shared" si="2"/>
         <v>22000</v>
       </c>
-      <c r="T24" s="9">
-        <v>2000</v>
-      </c>
-      <c r="U24" s="9">
-        <v>5000</v>
-      </c>
-      <c r="X24" s="9">
-        <v>5000</v>
-      </c>
-      <c r="AC24" s="9">
-        <v>5000</v>
-      </c>
-      <c r="AF24" s="9">
+      <c r="T24" s="10">
+        <v>2000</v>
+      </c>
+      <c r="U24" s="10">
+        <v>5000</v>
+      </c>
+      <c r="X24" s="10">
+        <v>5000</v>
+      </c>
+      <c r="AC24" s="10">
+        <v>5000</v>
+      </c>
+      <c r="AF24" s="10">
         <v>5000</v>
       </c>
     </row>
@@ -2792,12 +2816,12 @@
         <v>8709612020</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F25" s="8">
+        <v>41</v>
+      </c>
+      <c r="F25" s="9">
         <f t="shared" si="2"/>
         <v>24000</v>
       </c>
@@ -2834,12 +2858,12 @@
         <v>24</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" s="8">
+        <v>42</v>
+      </c>
+      <c r="F26" s="9">
         <f t="shared" si="2"/>
         <v>12500</v>
       </c>
@@ -2876,12 +2900,12 @@
         <v>25</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" s="8">
+        <v>43</v>
+      </c>
+      <c r="F27" s="9">
         <f t="shared" si="2"/>
         <v>7000</v>
       </c>
@@ -2900,12 +2924,12 @@
         <v>26</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F28" s="8">
+        <v>44</v>
+      </c>
+      <c r="F28" s="9">
         <f t="shared" si="2"/>
         <v>10000</v>
       </c>
@@ -2936,37 +2960,37 @@
         <v>27</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F29" s="8">
+        <v>45</v>
+      </c>
+      <c r="F29" s="9">
         <f t="shared" si="2"/>
         <v>27000</v>
       </c>
-      <c r="I29" s="9">
-        <v>2000</v>
-      </c>
-      <c r="J29" s="9">
-        <v>1000</v>
-      </c>
-      <c r="L29" s="9">
-        <v>3000</v>
-      </c>
-      <c r="N29" s="9">
-        <v>1000</v>
-      </c>
-      <c r="P29" s="9">
-        <v>5000</v>
-      </c>
-      <c r="V29" s="9">
-        <v>5000</v>
-      </c>
-      <c r="AH29" s="9">
-        <v>5000</v>
-      </c>
-      <c r="AK29" s="9">
+      <c r="I29" s="10">
+        <v>2000</v>
+      </c>
+      <c r="J29" s="10">
+        <v>1000</v>
+      </c>
+      <c r="L29" s="10">
+        <v>3000</v>
+      </c>
+      <c r="N29" s="10">
+        <v>1000</v>
+      </c>
+      <c r="P29" s="10">
+        <v>5000</v>
+      </c>
+      <c r="V29" s="10">
+        <v>5000</v>
+      </c>
+      <c r="AH29" s="10">
+        <v>5000</v>
+      </c>
+      <c r="AK29" s="10">
         <v>5000</v>
       </c>
     </row>
@@ -2975,43 +2999,43 @@
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" s="8">
+        <v>47</v>
+      </c>
+      <c r="F30" s="9">
         <f t="shared" si="2"/>
         <v>54000</v>
       </c>
       <c r="J30" s="3">
         <v>2000</v>
       </c>
-      <c r="L30" s="9">
+      <c r="L30" s="10">
         <v>12000</v>
       </c>
       <c r="O30" s="3">
         <v>5000</v>
       </c>
-      <c r="Q30" s="9">
-        <v>5000</v>
-      </c>
-      <c r="V30" s="9">
+      <c r="Q30" s="10">
+        <v>5000</v>
+      </c>
+      <c r="V30" s="10">
         <v>10000</v>
       </c>
       <c r="X30" s="3">
         <v>5000</v>
       </c>
-      <c r="AB30" s="9">
-        <v>5000</v>
-      </c>
-      <c r="AC30" s="9">
-        <v>5000</v>
-      </c>
-      <c r="AH30" s="9">
+      <c r="AB30" s="10">
+        <v>5000</v>
+      </c>
+      <c r="AC30" s="10">
+        <v>5000</v>
+      </c>
+      <c r="AH30" s="10">
         <v>5000</v>
       </c>
     </row>
@@ -3020,12 +3044,12 @@
         <v>29</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" s="8">
+        <v>48</v>
+      </c>
+      <c r="F31" s="9">
         <f t="shared" si="2"/>
         <v>14000</v>
       </c>
@@ -3080,12 +3104,12 @@
         <v>30</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F32" s="8">
+        <v>50</v>
+      </c>
+      <c r="F32" s="9">
         <f t="shared" si="2"/>
         <v>11000</v>
       </c>
@@ -3116,12 +3140,12 @@
         <v>31</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F33" s="8">
+        <v>51</v>
+      </c>
+      <c r="F33" s="9">
         <f t="shared" si="2"/>
         <v>7000</v>
       </c>
@@ -3152,12 +3176,12 @@
         <v>32</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F34" s="8">
+        <v>52</v>
+      </c>
+      <c r="F34" s="9">
         <f t="shared" si="2"/>
         <v>4000</v>
       </c>
@@ -3182,12 +3206,12 @@
         <v>33</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" s="8">
+        <v>53</v>
+      </c>
+      <c r="F35" s="9">
         <f t="shared" si="2"/>
         <v>33000</v>
       </c>
@@ -3197,28 +3221,28 @@
       <c r="M35" s="3">
         <v>4000</v>
       </c>
-      <c r="Q35" s="9">
+      <c r="Q35" s="10">
         <v>6000</v>
       </c>
-      <c r="V35" s="9">
-        <v>3000</v>
-      </c>
-      <c r="X35" s="9">
-        <v>3000</v>
-      </c>
-      <c r="AC35" s="9">
+      <c r="V35" s="10">
+        <v>3000</v>
+      </c>
+      <c r="X35" s="10">
+        <v>3000</v>
+      </c>
+      <c r="AC35" s="10">
         <v>3000</v>
       </c>
       <c r="AE35" s="3">
         <v>3000</v>
       </c>
-      <c r="AH35" s="9">
-        <v>3000</v>
-      </c>
-      <c r="AJ35" s="9">
-        <v>3000</v>
-      </c>
-      <c r="AK35" s="9">
+      <c r="AH35" s="10">
+        <v>3000</v>
+      </c>
+      <c r="AJ35" s="10">
+        <v>3000</v>
+      </c>
+      <c r="AK35" s="10">
         <v>3000</v>
       </c>
     </row>
@@ -3227,12 +3251,12 @@
         <v>34</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F36" s="8">
+        <v>54</v>
+      </c>
+      <c r="F36" s="9">
         <f t="shared" ref="F36:F73" si="3">SUM(G36:AK36)</f>
         <v>4000</v>
       </c>
@@ -3247,35 +3271,38 @@
       <c r="A37" s="3">
         <v>35</v>
       </c>
+      <c r="B37" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D37" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F37" s="8">
+        <v>56</v>
+      </c>
+      <c r="F37" s="9">
         <f t="shared" si="3"/>
         <v>21000</v>
       </c>
-      <c r="I37" s="9">
-        <v>3000</v>
-      </c>
-      <c r="M37" s="9">
-        <v>3000</v>
-      </c>
-      <c r="R37" s="9">
-        <v>3000</v>
-      </c>
-      <c r="T37" s="9">
+      <c r="I37" s="10">
+        <v>3000</v>
+      </c>
+      <c r="M37" s="10">
+        <v>3000</v>
+      </c>
+      <c r="R37" s="10">
+        <v>3000</v>
+      </c>
+      <c r="T37" s="10">
         <v>3000</v>
       </c>
       <c r="X37" s="3">
         <v>3000</v>
       </c>
-      <c r="AB37" s="9">
-        <v>3000</v>
-      </c>
-      <c r="AH37" s="9">
+      <c r="AB37" s="10">
+        <v>3000</v>
+      </c>
+      <c r="AH37" s="10">
         <v>3000</v>
       </c>
     </row>
@@ -3284,25 +3311,25 @@
         <v>36</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F38" s="8">
+        <v>57</v>
+      </c>
+      <c r="F38" s="9">
         <f t="shared" si="3"/>
         <v>9000</v>
       </c>
       <c r="K38" s="3">
         <v>2000</v>
       </c>
-      <c r="U38" s="9">
-        <v>2000</v>
-      </c>
-      <c r="AA38" s="9">
-        <v>2000</v>
-      </c>
-      <c r="AI38" s="9">
+      <c r="U38" s="10">
+        <v>2000</v>
+      </c>
+      <c r="AA38" s="10">
+        <v>2000</v>
+      </c>
+      <c r="AI38" s="10">
         <v>3000</v>
       </c>
     </row>
@@ -3311,12 +3338,12 @@
         <v>37</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F39" s="8">
+        <v>58</v>
+      </c>
+      <c r="F39" s="9">
         <f t="shared" si="3"/>
         <v>12000</v>
       </c>
@@ -3341,12 +3368,12 @@
         <v>38</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F40" s="8">
+        <v>59</v>
+      </c>
+      <c r="F40" s="9">
         <f t="shared" si="3"/>
         <v>11000</v>
       </c>
@@ -3380,12 +3407,12 @@
         <v>8210095108</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F41" s="8">
+        <v>60</v>
+      </c>
+      <c r="F41" s="9">
         <f t="shared" si="3"/>
         <v>36000</v>
       </c>
@@ -3428,12 +3455,12 @@
         <v>40</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F42" s="8">
+        <v>61</v>
+      </c>
+      <c r="F42" s="9">
         <f t="shared" si="3"/>
         <v>5000</v>
       </c>
@@ -3452,12 +3479,12 @@
         <v>41</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F43" s="8">
+        <v>62</v>
+      </c>
+      <c r="F43" s="9">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3467,22 +3494,22 @@
         <v>42</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F44" s="8">
+        <v>63</v>
+      </c>
+      <c r="F44" s="9">
         <f t="shared" si="3"/>
         <v>21000</v>
       </c>
-      <c r="I44" s="9">
-        <v>5000</v>
-      </c>
-      <c r="N44" s="9">
-        <v>3000</v>
-      </c>
-      <c r="T44" s="9">
+      <c r="I44" s="10">
+        <v>5000</v>
+      </c>
+      <c r="N44" s="10">
+        <v>3000</v>
+      </c>
+      <c r="T44" s="10">
         <v>1000</v>
       </c>
       <c r="U44" s="3">
@@ -3494,7 +3521,7 @@
       <c r="AD44" s="3">
         <v>3000</v>
       </c>
-      <c r="AH44" s="9">
+      <c r="AH44" s="10">
         <v>3000</v>
       </c>
     </row>
@@ -3503,12 +3530,12 @@
         <v>43</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F45" s="8">
+        <v>65</v>
+      </c>
+      <c r="F45" s="9">
         <f t="shared" si="3"/>
         <v>23000</v>
       </c>
@@ -3521,13 +3548,13 @@
       <c r="U45" s="3">
         <v>3000</v>
       </c>
-      <c r="Y45" s="9">
+      <c r="Y45" s="10">
         <v>3000</v>
       </c>
       <c r="AB45" s="3">
         <v>3000</v>
       </c>
-      <c r="AH45" s="9">
+      <c r="AH45" s="10">
         <v>6000</v>
       </c>
     </row>
@@ -3536,12 +3563,12 @@
         <v>44</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F46" s="8">
+        <v>66</v>
+      </c>
+      <c r="F46" s="9">
         <f t="shared" si="3"/>
         <v>22000</v>
       </c>
@@ -3575,25 +3602,25 @@
         <v>45</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F47" s="8">
+        <v>68</v>
+      </c>
+      <c r="F47" s="9">
         <f t="shared" si="3"/>
         <v>6000</v>
       </c>
-      <c r="J47" s="9">
-        <v>2000</v>
-      </c>
-      <c r="T47" s="9">
-        <v>2000</v>
-      </c>
-      <c r="AB47" s="9">
+      <c r="J47" s="10">
+        <v>2000</v>
+      </c>
+      <c r="T47" s="10">
+        <v>2000</v>
+      </c>
+      <c r="AB47" s="10">
         <v>2000</v>
       </c>
     </row>
@@ -3602,37 +3629,37 @@
         <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C48" s="3">
         <v>8863097933</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F48" s="8">
+        <v>70</v>
+      </c>
+      <c r="F48" s="9">
         <f t="shared" si="3"/>
         <v>17000</v>
       </c>
       <c r="P48" s="3">
         <v>2000</v>
       </c>
-      <c r="T48" s="9">
-        <v>3000</v>
-      </c>
-      <c r="U48" s="9">
-        <v>3000</v>
-      </c>
-      <c r="Y48" s="9">
+      <c r="T48" s="10">
+        <v>3000</v>
+      </c>
+      <c r="U48" s="10">
+        <v>3000</v>
+      </c>
+      <c r="Y48" s="10">
         <v>3000</v>
       </c>
       <c r="AD48" s="3">
         <v>3000</v>
       </c>
-      <c r="AK48" s="9">
+      <c r="AK48" s="10">
         <v>3000</v>
       </c>
     </row>
@@ -3641,22 +3668,22 @@
         <v>47</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C49" s="3">
         <v>9835443096</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F49" s="8">
+        <v>72</v>
+      </c>
+      <c r="F49" s="9">
         <f t="shared" si="3"/>
         <v>24000</v>
       </c>
-      <c r="J49" s="9">
+      <c r="J49" s="10">
         <v>2000</v>
       </c>
       <c r="N49" s="3">
@@ -3665,19 +3692,19 @@
       <c r="P49" s="3">
         <v>3000</v>
       </c>
-      <c r="U49" s="9">
-        <v>3000</v>
-      </c>
-      <c r="W49" s="9">
+      <c r="U49" s="10">
+        <v>3000</v>
+      </c>
+      <c r="W49" s="10">
         <v>2500</v>
       </c>
-      <c r="Y49" s="9">
+      <c r="Y49" s="10">
         <v>500</v>
       </c>
-      <c r="AD49" s="9">
+      <c r="AD49" s="10">
         <v>6000</v>
       </c>
-      <c r="AJ49" s="9">
+      <c r="AJ49" s="10">
         <v>3000</v>
       </c>
     </row>
@@ -3686,15 +3713,15 @@
         <v>48</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F50" s="8">
+        <v>74</v>
+      </c>
+      <c r="F50" s="9">
         <f t="shared" si="3"/>
         <v>9000</v>
       </c>
@@ -3704,13 +3731,13 @@
       <c r="P50" s="3">
         <v>2000</v>
       </c>
-      <c r="T50" s="9">
+      <c r="T50" s="10">
         <v>2000</v>
       </c>
       <c r="Y50" s="3">
         <v>2000</v>
       </c>
-      <c r="AB50" s="9">
+      <c r="AB50" s="10">
         <v>2000</v>
       </c>
     </row>
@@ -3719,25 +3746,25 @@
         <v>49</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F51" s="8">
+        <v>75</v>
+      </c>
+      <c r="F51" s="9">
         <f t="shared" si="3"/>
         <v>8000</v>
       </c>
       <c r="J51" s="3">
         <v>1000</v>
       </c>
-      <c r="N51" s="9">
-        <v>3000</v>
-      </c>
-      <c r="V51" s="9">
-        <v>2000</v>
-      </c>
-      <c r="AI51" s="9">
+      <c r="N51" s="10">
+        <v>3000</v>
+      </c>
+      <c r="V51" s="10">
+        <v>2000</v>
+      </c>
+      <c r="AI51" s="10">
         <v>2000</v>
       </c>
     </row>
@@ -3746,40 +3773,40 @@
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F52" s="8">
+        <v>77</v>
+      </c>
+      <c r="F52" s="9">
         <f t="shared" si="3"/>
         <v>22000</v>
       </c>
-      <c r="J52" s="9">
+      <c r="J52" s="10">
         <v>4000</v>
       </c>
-      <c r="N52" s="9">
+      <c r="N52" s="10">
         <v>3000</v>
       </c>
       <c r="R52" s="3">
         <v>3000</v>
       </c>
-      <c r="V52" s="9">
-        <v>3000</v>
-      </c>
-      <c r="X52" s="9">
+      <c r="V52" s="10">
+        <v>3000</v>
+      </c>
+      <c r="X52" s="10">
         <v>2000</v>
       </c>
       <c r="Y52" s="3">
         <v>1000</v>
       </c>
-      <c r="AE52" s="9">
-        <v>3000</v>
-      </c>
-      <c r="AH52" s="9">
+      <c r="AE52" s="10">
+        <v>3000</v>
+      </c>
+      <c r="AH52" s="10">
         <v>3000</v>
       </c>
     </row>
@@ -3788,19 +3815,19 @@
         <v>51</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F53" s="8">
+        <v>78</v>
+      </c>
+      <c r="F53" s="9">
         <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="AC53" s="3">
         <v>2000</v>
       </c>
-      <c r="AH53" s="9">
+      <c r="AH53" s="10">
         <v>2000</v>
       </c>
     </row>
@@ -3809,12 +3836,12 @@
         <v>52</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F54" s="8">
+        <v>80</v>
+      </c>
+      <c r="F54" s="9">
         <f t="shared" si="3"/>
         <v>9000</v>
       </c>
@@ -3836,12 +3863,12 @@
         <v>53</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F55" s="8">
+        <v>81</v>
+      </c>
+      <c r="F55" s="9">
         <f t="shared" si="3"/>
         <v>38000</v>
       </c>
@@ -3875,12 +3902,12 @@
         <v>54</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F56" s="8">
+        <v>82</v>
+      </c>
+      <c r="F56" s="9">
         <f t="shared" si="3"/>
         <v>9500</v>
       </c>
@@ -3893,7 +3920,7 @@
       <c r="U56" s="3">
         <v>1500</v>
       </c>
-      <c r="AA56" s="9">
+      <c r="AA56" s="10">
         <v>2000</v>
       </c>
       <c r="AI56" s="3">
@@ -3904,20 +3931,20 @@
       <c r="A57" s="3">
         <v>55</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>79</v>
+      <c r="B57" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F57" s="8">
+        <v>85</v>
+      </c>
+      <c r="F57" s="9">
         <f t="shared" si="3"/>
         <v>5000</v>
       </c>
-      <c r="AH57" s="9">
+      <c r="AH57" s="10">
         <v>5000</v>
       </c>
     </row>
@@ -3926,22 +3953,22 @@
         <v>56</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F58" s="8">
+        <v>87</v>
+      </c>
+      <c r="F58" s="9">
         <f t="shared" si="3"/>
         <v>9000</v>
       </c>
-      <c r="P58" s="9">
+      <c r="P58" s="10">
         <v>4000</v>
       </c>
-      <c r="AC58" s="9">
+      <c r="AC58" s="10">
         <v>5000</v>
       </c>
     </row>
@@ -3950,37 +3977,37 @@
         <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F59" s="8">
+        <v>90</v>
+      </c>
+      <c r="F59" s="9">
         <f t="shared" si="3"/>
         <v>14000</v>
       </c>
       <c r="K59" s="3">
         <v>1000</v>
       </c>
-      <c r="R59" s="9">
-        <v>2000</v>
-      </c>
-      <c r="T59" s="9">
-        <v>1000</v>
-      </c>
-      <c r="W59" s="9">
-        <v>2000</v>
-      </c>
-      <c r="AD59" s="9">
+      <c r="R59" s="10">
+        <v>2000</v>
+      </c>
+      <c r="T59" s="10">
+        <v>1000</v>
+      </c>
+      <c r="W59" s="10">
+        <v>2000</v>
+      </c>
+      <c r="AD59" s="10">
         <v>4000</v>
       </c>
-      <c r="AG59" s="9">
-        <v>2000</v>
-      </c>
-      <c r="AJ59" s="9">
+      <c r="AG59" s="10">
+        <v>2000</v>
+      </c>
+      <c r="AJ59" s="10">
         <v>2000</v>
       </c>
     </row>
@@ -3989,12 +4016,12 @@
         <v>58</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F60" s="8">
+        <v>92</v>
+      </c>
+      <c r="F60" s="9">
         <f t="shared" si="3"/>
         <v>4000</v>
       </c>
@@ -4010,12 +4037,12 @@
         <v>59</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F61" s="8">
+        <v>94</v>
+      </c>
+      <c r="F61" s="9">
         <f t="shared" si="3"/>
         <v>13000</v>
       </c>
@@ -4037,12 +4064,12 @@
         <v>60</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F62" s="8">
+        <v>95</v>
+      </c>
+      <c r="F62" s="9">
         <f t="shared" si="3"/>
         <v>11000</v>
       </c>
@@ -4067,12 +4094,12 @@
         <v>61</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F63" s="8">
+        <v>96</v>
+      </c>
+      <c r="F63" s="9">
         <f t="shared" si="3"/>
         <v>7000</v>
       </c>
@@ -4094,12 +4121,12 @@
         <v>62</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F64" s="8">
+        <v>97</v>
+      </c>
+      <c r="F64" s="9">
         <f t="shared" si="3"/>
         <v>4000</v>
       </c>
@@ -4118,12 +4145,12 @@
         <v>63</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F65" s="8">
+        <v>98</v>
+      </c>
+      <c r="F65" s="9">
         <f t="shared" si="3"/>
         <v>52000</v>
       </c>
@@ -4160,16 +4187,16 @@
         <v>64</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F66" s="8">
+        <v>99</v>
+      </c>
+      <c r="F66" s="9">
         <f t="shared" si="3"/>
         <v>24000</v>
       </c>
-      <c r="L66" s="9">
+      <c r="L66" s="10">
         <v>4000</v>
       </c>
       <c r="M66" s="3">
@@ -4199,12 +4226,12 @@
         <v>65</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F67" s="8">
+        <v>100</v>
+      </c>
+      <c r="F67" s="9">
         <f t="shared" si="3"/>
         <v>6000</v>
       </c>
@@ -4220,12 +4247,12 @@
         <v>66</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F68" s="8">
+        <v>101</v>
+      </c>
+      <c r="F68" s="9">
         <f t="shared" si="3"/>
         <v>3500</v>
       </c>
@@ -4250,19 +4277,19 @@
         <v>6200769032</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F69" s="8">
+        <v>103</v>
+      </c>
+      <c r="F69" s="9">
         <f t="shared" si="3"/>
         <v>16500</v>
       </c>
-      <c r="J69" s="9">
-        <v>1000</v>
-      </c>
-      <c r="M69" s="9">
+      <c r="J69" s="10">
+        <v>1000</v>
+      </c>
+      <c r="M69" s="10">
         <v>2000</v>
       </c>
       <c r="T69" s="3">
@@ -4283,7 +4310,7 @@
       <c r="AB69" s="3">
         <v>1900</v>
       </c>
-      <c r="AE69" s="9">
+      <c r="AE69" s="10">
         <v>2200</v>
       </c>
       <c r="AJ69" s="3">
@@ -4295,19 +4322,19 @@
         <v>68</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F70" s="8">
+        <v>104</v>
+      </c>
+      <c r="F70" s="9">
         <f t="shared" si="3"/>
         <v>27000</v>
       </c>
-      <c r="K70" s="9">
-        <v>3000</v>
-      </c>
-      <c r="M70" s="9">
+      <c r="K70" s="10">
+        <v>3000</v>
+      </c>
+      <c r="M70" s="10">
         <v>3000</v>
       </c>
       <c r="P70" s="3">
@@ -4328,7 +4355,7 @@
       <c r="AE70" s="3">
         <v>3000</v>
       </c>
-      <c r="AI70" s="9">
+      <c r="AI70" s="10">
         <v>3000</v>
       </c>
     </row>
@@ -4337,15 +4364,15 @@
         <v>69</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F71" s="8">
+        <v>106</v>
+      </c>
+      <c r="F71" s="9">
         <f t="shared" si="3"/>
         <v>19000</v>
       </c>
@@ -4361,19 +4388,19 @@
       <c r="R71" s="3">
         <v>1000</v>
       </c>
-      <c r="T71" s="9">
+      <c r="T71" s="10">
         <v>3000</v>
       </c>
       <c r="V71" s="3">
         <v>2000</v>
       </c>
-      <c r="Y71" s="9">
+      <c r="Y71" s="10">
         <v>4000</v>
       </c>
-      <c r="AE71" s="9">
-        <v>2000</v>
-      </c>
-      <c r="AJ71" s="9">
+      <c r="AE71" s="10">
+        <v>2000</v>
+      </c>
+      <c r="AJ71" s="10">
         <v>2000</v>
       </c>
     </row>
@@ -4382,9 +4409,9 @@
         <v>70</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F72" s="8">
+        <v>107</v>
+      </c>
+      <c r="F72" s="9">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4394,25 +4421,25 @@
         <v>71</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="F73" s="8">
+        <v>110</v>
+      </c>
+      <c r="F73" s="9">
         <f t="shared" si="3"/>
         <v>6000</v>
       </c>
-      <c r="Q73" s="9">
-        <v>2000</v>
-      </c>
-      <c r="AB73" s="9">
-        <v>2000</v>
-      </c>
-      <c r="AK73" s="9">
+      <c r="Q73" s="10">
+        <v>2000</v>
+      </c>
+      <c r="AB73" s="10">
+        <v>2000</v>
+      </c>
+      <c r="AK73" s="10">
         <v>2000</v>
       </c>
     </row>
@@ -4421,9 +4448,9 @@
         <v>72</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F74" s="8">
+        <v>111</v>
+      </c>
+      <c r="F74" s="9">
         <f t="shared" ref="F69:F94" si="4">SUM(G74:AK74)</f>
         <v>0</v>
       </c>
@@ -4433,16 +4460,16 @@
         <v>73</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F75" s="8">
+        <v>113</v>
+      </c>
+      <c r="F75" s="9">
         <f t="shared" si="4"/>
         <v>3000</v>
       </c>
-      <c r="AH75" s="9">
+      <c r="AH75" s="10">
         <v>3000</v>
       </c>
     </row>
@@ -4451,9 +4478,9 @@
         <v>74</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F76" s="8">
+        <v>114</v>
+      </c>
+      <c r="F76" s="9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4463,16 +4490,16 @@
         <v>75</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F77" s="8">
+        <v>115</v>
+      </c>
+      <c r="F77" s="9">
         <f t="shared" si="4"/>
         <v>3000</v>
       </c>
-      <c r="AE77" s="9">
+      <c r="AE77" s="10">
         <v>3000</v>
       </c>
     </row>
@@ -4481,9 +4508,9 @@
         <v>76</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F78" s="8">
+        <v>116</v>
+      </c>
+      <c r="F78" s="9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4493,9 +4520,9 @@
         <v>77</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="F79" s="8">
+        <v>117</v>
+      </c>
+      <c r="F79" s="9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4505,9 +4532,9 @@
         <v>78</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F80" s="8">
+        <v>118</v>
+      </c>
+      <c r="F80" s="9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4517,9 +4544,9 @@
         <v>79</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F81" s="8">
+        <v>119</v>
+      </c>
+      <c r="F81" s="9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4529,25 +4556,25 @@
         <v>80</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F82" s="8">
+        <v>121</v>
+      </c>
+      <c r="F82" s="9">
         <f t="shared" si="4"/>
         <v>13000</v>
       </c>
-      <c r="AB82" s="9">
-        <v>2000</v>
-      </c>
-      <c r="AC82" s="9">
-        <v>3000</v>
-      </c>
-      <c r="AE82" s="9">
-        <v>3000</v>
-      </c>
-      <c r="AH82" s="9">
+      <c r="AB82" s="10">
+        <v>2000</v>
+      </c>
+      <c r="AC82" s="10">
+        <v>3000</v>
+      </c>
+      <c r="AE82" s="10">
+        <v>3000</v>
+      </c>
+      <c r="AH82" s="10">
         <v>5000</v>
       </c>
     </row>
@@ -4556,9 +4583,9 @@
         <v>81</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F83" s="8">
+        <v>122</v>
+      </c>
+      <c r="F83" s="9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4568,9 +4595,9 @@
         <v>82</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="F84" s="8">
+        <v>123</v>
+      </c>
+      <c r="F84" s="9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4580,19 +4607,19 @@
         <v>83</v>
       </c>
       <c r="B85" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D85" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D85" s="3" t="s">
-        <v>116</v>
-      </c>
       <c r="E85" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="F85" s="8">
+        <v>125</v>
+      </c>
+      <c r="F85" s="9">
         <f t="shared" si="4"/>
         <v>2000</v>
       </c>
-      <c r="AB85" s="9">
+      <c r="AB85" s="10">
         <v>2000</v>
       </c>
     </row>
@@ -4601,9 +4628,9 @@
         <v>84</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="F86" s="8">
+        <v>126</v>
+      </c>
+      <c r="F86" s="9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4613,9 +4640,9 @@
         <v>85</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="F87" s="8">
+        <v>127</v>
+      </c>
+      <c r="F87" s="9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4625,9 +4652,9 @@
         <v>86</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="F88" s="8">
+        <v>128</v>
+      </c>
+      <c r="F88" s="9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4637,9 +4664,9 @@
         <v>87</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F89" s="8">
+        <v>129</v>
+      </c>
+      <c r="F89" s="9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4649,9 +4676,9 @@
         <v>88</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="F90" s="8">
+        <v>130</v>
+      </c>
+      <c r="F90" s="9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4661,9 +4688,9 @@
         <v>89</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F91" s="8">
+        <v>131</v>
+      </c>
+      <c r="F91" s="9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4673,9 +4700,9 @@
         <v>90</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="F92" s="8">
+        <v>132</v>
+      </c>
+      <c r="F92" s="9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4685,9 +4712,9 @@
         <v>91</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="F93" s="8">
+        <v>133</v>
+      </c>
+      <c r="F93" s="9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4697,9 +4724,9 @@
         <v>92</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F94" s="8">
+        <v>134</v>
+      </c>
+      <c r="F94" s="9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
data updated till 24 Jan 8PM
</commit_message>
<xml_diff>
--- a/Daily Collection/December-2020-Collection.xlsx
+++ b/Daily Collection/December-2020-Collection.xlsx
@@ -646,10 +646,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="23">
@@ -677,8 +677,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -692,36 +709,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -729,7 +717,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -744,6 +732,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -752,8 +748,22 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -761,6 +771,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -774,9 +798,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -784,30 +807,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -857,73 +857,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -935,37 +869,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -983,7 +899,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -995,49 +1031,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1068,9 +1068,59 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1098,70 +1148,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1174,127 +1174,127 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1662,11 +1662,11 @@
   <dimension ref="A1:AK94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="T32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="X65" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E39" sqref="E39"/>
+      <selection pane="bottomRight" activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>

</xml_diff>